<commit_message>
Optimize patient indicator with cached dataframe
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="621" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="File active" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
   <si>
     <t>Région</t>
   </si>
@@ -123,10 +123,136 @@
     <t>{key: 'DEAD_DURING_PERIOD', age_max: 15, gender: 0}</t>
   </si>
   <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'DEAD_DURING_PERIOD', age_min: 50, gender: 1}</t>
+  </si>
+  <si>
     <t>Nombre Total d’adultes et d’enfants sous antirétroviraux Ayant arrêté le traitement au cours au cours de la période de raportage (I)</t>
   </si>
   <si>
     <t>Nombre Total d’adultes et d’enfants sous antirétroviraux transférés au cours au cours de la période de raportage (J)</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', gender: 1}</t>
+  </si>
+  <si>
+    <t>{key:'TRANSFERRED_DURING_PERIOD', age_max: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD'}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_max: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'TRANSFERRED_DURING_PERIOD', age_min: 50, gender: 1}</t>
   </si>
   <si>
     <t>Nombre d’adultes et d’enfants qui sont sous TARV (Anciens et Nouveaux poursuivant les ARV) à la fin du 1er semestre 2016 (au 30 juin 2016)  K=(A+B+C+D+E) -(G+H+I+J)</t>
@@ -397,7 +523,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* \-??\ _€_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* \-??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -489,6 +615,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
     <font>
@@ -756,7 +888,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -873,18 +1005,26 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -973,7 +1113,7 @@
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -993,7 +1133,7 @@
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1078,15 +1218,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>164160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>565560</xdr:colOff>
+      <xdr:colOff>592200</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1099,8 +1239,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="772920"/>
-          <a:ext cx="484560" cy="360720"/>
+          <a:off x="108000" y="763920"/>
+          <a:ext cx="484200" cy="360360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1122,8 +1262,8 @@
   </sheetPr>
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB21" activeCellId="0" sqref="AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1574,7 +1714,7 @@
       <c r="AA16" s="24"/>
       <c r="AB16" s="27"/>
     </row>
-    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="21" t="s">
         <v>27</v>
       </c>
@@ -1613,7 +1753,7 @@
       <c r="B18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="15" t="s">
@@ -1622,37 +1762,79 @@
       <c r="E18" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="17"/>
-      <c r="V18" s="17"/>
-      <c r="W18" s="17"/>
-      <c r="X18" s="17"/>
-      <c r="Y18" s="17"/>
-      <c r="Z18" s="17"/>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="20"/>
-    </row>
-    <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="O18" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="P18" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q18" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="S18" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="T18" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="U18" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="V18" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="W18" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="X18" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y18" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z18" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA18" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB18" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="21" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -1682,41 +1864,95 @@
       <c r="AA19" s="19"/>
       <c r="AB19" s="20"/>
     </row>
-    <row r="20" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="17"/>
-      <c r="W20" s="17"/>
-      <c r="X20" s="17"/>
-      <c r="Y20" s="17"/>
-      <c r="Z20" s="17"/>
-      <c r="AA20" s="19"/>
-      <c r="AB20" s="20"/>
+        <v>54</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="O20" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="P20" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q20" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="R20" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="S20" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="T20" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="U20" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="V20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W20" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="X20" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y20" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z20" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA20" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB20" s="30" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="29" t="s">
-        <v>37</v>
+      <c r="A21" s="31" t="s">
+        <v>79</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -1746,9 +1982,9 @@
       <c r="AA21" s="24"/>
       <c r="AB21" s="27"/>
     </row>
-    <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="21" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -1780,7 +2016,7 @@
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1812,7 +2048,7 @@
     </row>
     <row r="24" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="21" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -1844,7 +2080,7 @@
     </row>
     <row r="25" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="21" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -1876,7 +2112,7 @@
     </row>
     <row r="26" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="21" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1908,7 +2144,7 @@
     </row>
     <row r="27" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="21" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1939,8 +2175,8 @@
       <c r="AB27" s="20"/>
     </row>
     <row r="28" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="30" t="s">
-        <v>44</v>
+      <c r="A28" s="32" t="s">
+        <v>86</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1971,8 +2207,8 @@
       <c r="AB28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="30" t="s">
-        <v>45</v>
+      <c r="A29" s="32" t="s">
+        <v>87</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2003,8 +2239,8 @@
       <c r="AB29" s="20"/>
     </row>
     <row r="30" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="30" t="s">
-        <v>46</v>
+      <c r="A30" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2035,8 +2271,8 @@
       <c r="AB30" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="31" t="s">
-        <v>47</v>
+      <c r="A31" s="33" t="s">
+        <v>89</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2067,8 +2303,8 @@
       <c r="AB31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="s">
-        <v>48</v>
+      <c r="A32" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2099,8 +2335,8 @@
       <c r="AB32" s="20"/>
     </row>
     <row r="33" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31" t="s">
-        <v>49</v>
+      <c r="A33" s="33" t="s">
+        <v>91</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2131,36 +2367,36 @@
       <c r="AB33" s="20"/>
     </row>
     <row r="34" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
-      <c r="P34" s="33"/>
-      <c r="Q34" s="33"/>
-      <c r="R34" s="33"/>
-      <c r="S34" s="33"/>
-      <c r="T34" s="33"/>
-      <c r="U34" s="33"/>
-      <c r="V34" s="33"/>
-      <c r="W34" s="33"/>
-      <c r="X34" s="33"/>
-      <c r="Y34" s="33"/>
-      <c r="Z34" s="33"/>
-      <c r="AA34" s="33"/>
-      <c r="AB34" s="33"/>
+      <c r="A34" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
+      <c r="V34" s="35"/>
+      <c r="W34" s="35"/>
+      <c r="X34" s="35"/>
+      <c r="Y34" s="35"/>
+      <c r="Z34" s="35"/>
+      <c r="AA34" s="35"/>
+      <c r="AB34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="21"/>
@@ -2194,7 +2430,7 @@
     </row>
     <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="21" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2226,7 +2462,7 @@
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="21" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2258,7 +2494,7 @@
     </row>
     <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="21" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2290,7 +2526,7 @@
     </row>
     <row r="39" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2321,36 +2557,36 @@
       <c r="AB39" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="37"/>
-      <c r="N40" s="37"/>
-      <c r="O40" s="37"/>
-      <c r="P40" s="37"/>
-      <c r="Q40" s="37"/>
-      <c r="R40" s="37"/>
-      <c r="S40" s="37"/>
-      <c r="T40" s="37"/>
-      <c r="U40" s="37"/>
-      <c r="V40" s="37"/>
-      <c r="W40" s="37"/>
-      <c r="X40" s="37"/>
-      <c r="Y40" s="37"/>
-      <c r="Z40" s="37"/>
-      <c r="AA40" s="36"/>
-      <c r="AB40" s="38"/>
+      <c r="A40" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="39"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="39"/>
+      <c r="O40" s="39"/>
+      <c r="P40" s="39"/>
+      <c r="Q40" s="39"/>
+      <c r="R40" s="39"/>
+      <c r="S40" s="39"/>
+      <c r="T40" s="39"/>
+      <c r="U40" s="39"/>
+      <c r="V40" s="39"/>
+      <c r="W40" s="39"/>
+      <c r="X40" s="39"/>
+      <c r="Y40" s="39"/>
+      <c r="Z40" s="39"/>
+      <c r="AA40" s="38"/>
+      <c r="AB40" s="40"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2407,1383 +2643,1383 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
-        <v>56</v>
+      <c r="A1" s="41" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>57</v>
+      <c r="A2" s="41" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
-        <v>58</v>
+      <c r="A3" s="41" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
-        <v>59</v>
+      <c r="A4" s="41" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
-        <v>60</v>
+      <c r="A6" s="41" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
-        <v>61</v>
+      <c r="A7" s="41" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39"/>
+      <c r="A8" s="41"/>
     </row>
     <row r="9" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40" t="s">
-        <v>62</v>
+      <c r="A9" s="42" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="41" t="s">
-        <v>63</v>
+      <c r="A10" s="43" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42"/>
+      <c r="A11" s="44"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42" t="s">
-        <v>64</v>
+      <c r="A12" s="44" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="43"/>
+      <c r="A13" s="45"/>
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45" t="s">
+      <c r="A14" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45" t="s">
+      <c r="K14" s="47"/>
+      <c r="L14" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45" t="s">
+      <c r="M14" s="47"/>
+      <c r="N14" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="U14" s="45"/>
-      <c r="V14" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="W14" s="45"/>
-      <c r="X14" s="46" t="s">
+      <c r="O14" s="47"/>
+      <c r="P14" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="S14" s="47"/>
+      <c r="T14" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="U14" s="47"/>
+      <c r="V14" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="W14" s="47"/>
+      <c r="X14" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="Y14" s="46"/>
+      <c r="Y14" s="48"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="44"/>
-      <c r="B15" s="47" t="s">
+      <c r="A15" s="46"/>
+      <c r="B15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="47" t="s">
+      <c r="G15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="47" t="s">
+      <c r="H15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="47" t="s">
+      <c r="I15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="47" t="s">
+      <c r="J15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="47" t="s">
+      <c r="K15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="L15" s="47" t="s">
+      <c r="L15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M15" s="47" t="s">
+      <c r="M15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="N15" s="47" t="s">
+      <c r="N15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="O15" s="47" t="s">
+      <c r="O15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="47" t="s">
+      <c r="P15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="Q15" s="47" t="s">
+      <c r="Q15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="R15" s="47" t="s">
+      <c r="R15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="S15" s="47" t="s">
+      <c r="S15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="T15" s="47" t="s">
+      <c r="T15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="U15" s="47" t="s">
+      <c r="U15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="V15" s="47" t="s">
+      <c r="V15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="W15" s="47" t="s">
+      <c r="W15" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="X15" s="47" t="s">
+      <c r="X15" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="Y15" s="48" t="s">
+      <c r="Y15" s="50" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="49"/>
-      <c r="R16" s="49"/>
-      <c r="S16" s="49"/>
-      <c r="T16" s="49"/>
-      <c r="U16" s="49"/>
-      <c r="V16" s="49"/>
-      <c r="W16" s="49"/>
-      <c r="X16" s="49"/>
-      <c r="Y16" s="49"/>
+      <c r="A16" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="51"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="51"/>
+      <c r="U16" s="51"/>
+      <c r="V16" s="51"/>
+      <c r="W16" s="51"/>
+      <c r="X16" s="51"/>
+      <c r="Y16" s="51"/>
     </row>
     <row r="17" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="51"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="51"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="52"/>
+      <c r="A17" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="53"/>
+      <c r="T17" s="53"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="54"/>
     </row>
     <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="51"/>
-      <c r="T18" s="51"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
-      <c r="W18" s="51"/>
-      <c r="X18" s="51"/>
-      <c r="Y18" s="52"/>
+      <c r="A18" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="53"/>
+      <c r="R18" s="53"/>
+      <c r="S18" s="53"/>
+      <c r="T18" s="53"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
+      <c r="Y18" s="54"/>
     </row>
     <row r="19" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="52"/>
+      <c r="A19" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="53"/>
+      <c r="R19" s="53"/>
+      <c r="S19" s="53"/>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="53"/>
+      <c r="Y19" s="54"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51"/>
-      <c r="P20" s="51"/>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="51"/>
-      <c r="T20" s="51"/>
-      <c r="U20" s="51"/>
-      <c r="V20" s="51"/>
-      <c r="W20" s="51"/>
-      <c r="X20" s="51"/>
-      <c r="Y20" s="52"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="53"/>
+      <c r="S20" s="53"/>
+      <c r="T20" s="53"/>
+      <c r="U20" s="53"/>
+      <c r="V20" s="53"/>
+      <c r="W20" s="53"/>
+      <c r="X20" s="53"/>
+      <c r="Y20" s="54"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="51"/>
-      <c r="T21" s="51"/>
-      <c r="U21" s="51"/>
-      <c r="V21" s="51"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="52"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
+      <c r="O21" s="53"/>
+      <c r="P21" s="53"/>
+      <c r="Q21" s="53"/>
+      <c r="R21" s="53"/>
+      <c r="S21" s="53"/>
+      <c r="T21" s="53"/>
+      <c r="U21" s="53"/>
+      <c r="V21" s="53"/>
+      <c r="W21" s="53"/>
+      <c r="X21" s="53"/>
+      <c r="Y21" s="54"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
-      <c r="Q22" s="49"/>
-      <c r="R22" s="49"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="49"/>
-      <c r="U22" s="49"/>
-      <c r="V22" s="49"/>
-      <c r="W22" s="49"/>
-      <c r="X22" s="49"/>
-      <c r="Y22" s="49"/>
+      <c r="A22" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="51"/>
+      <c r="S22" s="51"/>
+      <c r="T22" s="51"/>
+      <c r="U22" s="51"/>
+      <c r="V22" s="51"/>
+      <c r="W22" s="51"/>
+      <c r="X22" s="51"/>
+      <c r="Y22" s="51"/>
     </row>
     <row r="23" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="51"/>
-      <c r="S23" s="51"/>
-      <c r="T23" s="51"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="51"/>
-      <c r="W23" s="51"/>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="52"/>
+      <c r="A23" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53"/>
+      <c r="T23" s="53"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
+      <c r="Y23" s="54"/>
     </row>
     <row r="24" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="51"/>
-      <c r="T24" s="51"/>
-      <c r="U24" s="51"/>
-      <c r="V24" s="51"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="51"/>
-      <c r="Y24" s="52"/>
+      <c r="A24" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="53"/>
+      <c r="T24" s="53"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="53"/>
+      <c r="Y24" s="54"/>
     </row>
     <row r="25" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
-      <c r="T25" s="51"/>
-      <c r="U25" s="51"/>
-      <c r="V25" s="51"/>
-      <c r="W25" s="51"/>
-      <c r="X25" s="51"/>
-      <c r="Y25" s="52"/>
+      <c r="A25" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="53"/>
+      <c r="T25" s="53"/>
+      <c r="U25" s="53"/>
+      <c r="V25" s="53"/>
+      <c r="W25" s="53"/>
+      <c r="X25" s="53"/>
+      <c r="Y25" s="54"/>
     </row>
     <row r="26" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
-      <c r="T26" s="51"/>
-      <c r="U26" s="51"/>
-      <c r="V26" s="51"/>
-      <c r="W26" s="51"/>
-      <c r="X26" s="51"/>
-      <c r="Y26" s="52"/>
+      <c r="A26" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="53"/>
+      <c r="P26" s="53"/>
+      <c r="Q26" s="53"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="53"/>
+      <c r="T26" s="53"/>
+      <c r="U26" s="53"/>
+      <c r="V26" s="53"/>
+      <c r="W26" s="53"/>
+      <c r="X26" s="53"/>
+      <c r="Y26" s="54"/>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="50"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="51"/>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="51"/>
-      <c r="R27" s="51"/>
-      <c r="S27" s="51"/>
-      <c r="T27" s="51"/>
-      <c r="U27" s="51"/>
-      <c r="V27" s="51"/>
-      <c r="W27" s="51"/>
-      <c r="X27" s="51"/>
-      <c r="Y27" s="52"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="53"/>
+      <c r="T27" s="53"/>
+      <c r="U27" s="53"/>
+      <c r="V27" s="53"/>
+      <c r="W27" s="53"/>
+      <c r="X27" s="53"/>
+      <c r="Y27" s="54"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="50"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="51"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="51"/>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="52"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="53"/>
+      <c r="Q28" s="53"/>
+      <c r="R28" s="53"/>
+      <c r="S28" s="53"/>
+      <c r="T28" s="53"/>
+      <c r="U28" s="53"/>
+      <c r="V28" s="53"/>
+      <c r="W28" s="53"/>
+      <c r="X28" s="53"/>
+      <c r="Y28" s="54"/>
     </row>
     <row r="29" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="51"/>
-      <c r="T29" s="51"/>
-      <c r="U29" s="51"/>
-      <c r="V29" s="51"/>
-      <c r="W29" s="51"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="52"/>
+      <c r="A29" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="53"/>
+      <c r="T29" s="53"/>
+      <c r="U29" s="53"/>
+      <c r="V29" s="53"/>
+      <c r="W29" s="53"/>
+      <c r="X29" s="53"/>
+      <c r="Y29" s="54"/>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="49"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="49"/>
-      <c r="U30" s="49"/>
-      <c r="V30" s="49"/>
-      <c r="W30" s="49"/>
-      <c r="X30" s="49"/>
-      <c r="Y30" s="49"/>
+      <c r="A30" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
+      <c r="T30" s="51"/>
+      <c r="U30" s="51"/>
+      <c r="V30" s="51"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
+      <c r="Y30" s="51"/>
     </row>
     <row r="31" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="51"/>
-      <c r="T31" s="51"/>
-      <c r="U31" s="51"/>
-      <c r="V31" s="51"/>
-      <c r="W31" s="51"/>
-      <c r="X31" s="51"/>
-      <c r="Y31" s="52"/>
+      <c r="A31" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="53"/>
+      <c r="P31" s="53"/>
+      <c r="Q31" s="53"/>
+      <c r="R31" s="53"/>
+      <c r="S31" s="53"/>
+      <c r="T31" s="53"/>
+      <c r="U31" s="53"/>
+      <c r="V31" s="53"/>
+      <c r="W31" s="53"/>
+      <c r="X31" s="53"/>
+      <c r="Y31" s="54"/>
     </row>
     <row r="32" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="51"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="51"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="51"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="51"/>
-      <c r="S32" s="51"/>
-      <c r="T32" s="51"/>
-      <c r="U32" s="51"/>
-      <c r="V32" s="51"/>
-      <c r="W32" s="51"/>
-      <c r="X32" s="51"/>
-      <c r="Y32" s="52"/>
+      <c r="A32" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="53"/>
+      <c r="N32" s="53"/>
+      <c r="O32" s="53"/>
+      <c r="P32" s="53"/>
+      <c r="Q32" s="53"/>
+      <c r="R32" s="53"/>
+      <c r="S32" s="53"/>
+      <c r="T32" s="53"/>
+      <c r="U32" s="53"/>
+      <c r="V32" s="53"/>
+      <c r="W32" s="53"/>
+      <c r="X32" s="53"/>
+      <c r="Y32" s="54"/>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="50"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="51"/>
-      <c r="P33" s="51"/>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="51"/>
-      <c r="S33" s="51"/>
-      <c r="T33" s="51"/>
-      <c r="U33" s="51"/>
-      <c r="V33" s="51"/>
-      <c r="W33" s="51"/>
-      <c r="X33" s="51"/>
-      <c r="Y33" s="52"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="53"/>
+      <c r="N33" s="53"/>
+      <c r="O33" s="53"/>
+      <c r="P33" s="53"/>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="53"/>
+      <c r="T33" s="53"/>
+      <c r="U33" s="53"/>
+      <c r="V33" s="53"/>
+      <c r="W33" s="53"/>
+      <c r="X33" s="53"/>
+      <c r="Y33" s="54"/>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="50"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="51"/>
-      <c r="P34" s="51"/>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="51"/>
-      <c r="S34" s="51"/>
-      <c r="T34" s="51"/>
-      <c r="U34" s="51"/>
-      <c r="V34" s="51"/>
-      <c r="W34" s="51"/>
-      <c r="X34" s="51"/>
-      <c r="Y34" s="52"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="53"/>
+      <c r="O34" s="53"/>
+      <c r="P34" s="53"/>
+      <c r="Q34" s="53"/>
+      <c r="R34" s="53"/>
+      <c r="S34" s="53"/>
+      <c r="T34" s="53"/>
+      <c r="U34" s="53"/>
+      <c r="V34" s="53"/>
+      <c r="W34" s="53"/>
+      <c r="X34" s="53"/>
+      <c r="Y34" s="54"/>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="49"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
-      <c r="T35" s="49"/>
-      <c r="U35" s="49"/>
-      <c r="V35" s="49"/>
-      <c r="W35" s="49"/>
-      <c r="X35" s="49"/>
-      <c r="Y35" s="49"/>
+      <c r="A35" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="51"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="51"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="51"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="51"/>
+      <c r="T35" s="51"/>
+      <c r="U35" s="51"/>
+      <c r="V35" s="51"/>
+      <c r="W35" s="51"/>
+      <c r="X35" s="51"/>
+      <c r="Y35" s="51"/>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="50"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="51"/>
-      <c r="O36" s="51"/>
-      <c r="P36" s="51"/>
-      <c r="Q36" s="51"/>
-      <c r="R36" s="51"/>
-      <c r="S36" s="51"/>
-      <c r="T36" s="51"/>
-      <c r="U36" s="51"/>
-      <c r="V36" s="51"/>
-      <c r="W36" s="51"/>
-      <c r="X36" s="51"/>
-      <c r="Y36" s="52"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="53"/>
+      <c r="N36" s="53"/>
+      <c r="O36" s="53"/>
+      <c r="P36" s="53"/>
+      <c r="Q36" s="53"/>
+      <c r="R36" s="53"/>
+      <c r="S36" s="53"/>
+      <c r="T36" s="53"/>
+      <c r="U36" s="53"/>
+      <c r="V36" s="53"/>
+      <c r="W36" s="53"/>
+      <c r="X36" s="53"/>
+      <c r="Y36" s="54"/>
     </row>
     <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="53"/>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="51"/>
-      <c r="L37" s="51"/>
-      <c r="M37" s="51"/>
-      <c r="N37" s="51"/>
-      <c r="O37" s="51"/>
-      <c r="P37" s="51"/>
-      <c r="Q37" s="51"/>
-      <c r="R37" s="51"/>
-      <c r="S37" s="51"/>
-      <c r="T37" s="51"/>
-      <c r="U37" s="51"/>
-      <c r="V37" s="51"/>
-      <c r="W37" s="51"/>
-      <c r="X37" s="51"/>
-      <c r="Y37" s="52"/>
+      <c r="A37" s="55"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="53"/>
+      <c r="O37" s="53"/>
+      <c r="P37" s="53"/>
+      <c r="Q37" s="53"/>
+      <c r="R37" s="53"/>
+      <c r="S37" s="53"/>
+      <c r="T37" s="53"/>
+      <c r="U37" s="53"/>
+      <c r="V37" s="53"/>
+      <c r="W37" s="53"/>
+      <c r="X37" s="53"/>
+      <c r="Y37" s="54"/>
     </row>
     <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="53"/>
-      <c r="B38" s="51"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="51"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="51"/>
-      <c r="O38" s="51"/>
-      <c r="P38" s="51"/>
-      <c r="Q38" s="51"/>
-      <c r="R38" s="51"/>
-      <c r="S38" s="51"/>
-      <c r="T38" s="51"/>
-      <c r="U38" s="51"/>
-      <c r="V38" s="51"/>
-      <c r="W38" s="51"/>
-      <c r="X38" s="51"/>
-      <c r="Y38" s="52"/>
+      <c r="A38" s="55"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="53"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="53"/>
+      <c r="O38" s="53"/>
+      <c r="P38" s="53"/>
+      <c r="Q38" s="53"/>
+      <c r="R38" s="53"/>
+      <c r="S38" s="53"/>
+      <c r="T38" s="53"/>
+      <c r="U38" s="53"/>
+      <c r="V38" s="53"/>
+      <c r="W38" s="53"/>
+      <c r="X38" s="53"/>
+      <c r="Y38" s="54"/>
     </row>
     <row r="39" customFormat="false" ht="66.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="51"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="51"/>
-      <c r="O39" s="51"/>
-      <c r="P39" s="51"/>
-      <c r="Q39" s="51"/>
-      <c r="R39" s="51"/>
-      <c r="S39" s="51"/>
-      <c r="T39" s="51"/>
-      <c r="U39" s="51"/>
-      <c r="V39" s="51"/>
-      <c r="W39" s="51"/>
-      <c r="X39" s="51"/>
-      <c r="Y39" s="52"/>
+      <c r="A39" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="53"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="53"/>
+      <c r="Q39" s="53"/>
+      <c r="R39" s="53"/>
+      <c r="S39" s="53"/>
+      <c r="T39" s="53"/>
+      <c r="U39" s="53"/>
+      <c r="V39" s="53"/>
+      <c r="W39" s="53"/>
+      <c r="X39" s="53"/>
+      <c r="Y39" s="54"/>
     </row>
     <row r="40" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="53" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="51"/>
-      <c r="P40" s="51"/>
-      <c r="Q40" s="51"/>
-      <c r="R40" s="51"/>
-      <c r="S40" s="51"/>
-      <c r="T40" s="51"/>
-      <c r="U40" s="51"/>
-      <c r="V40" s="51"/>
-      <c r="W40" s="51"/>
-      <c r="X40" s="51"/>
-      <c r="Y40" s="52"/>
+      <c r="A40" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="53"/>
+      <c r="S40" s="53"/>
+      <c r="T40" s="53"/>
+      <c r="U40" s="53"/>
+      <c r="V40" s="53"/>
+      <c r="W40" s="53"/>
+      <c r="X40" s="53"/>
+      <c r="Y40" s="54"/>
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="49"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="49"/>
-      <c r="I41" s="49"/>
-      <c r="J41" s="49"/>
-      <c r="K41" s="49"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="49"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
-      <c r="S41" s="49"/>
-      <c r="T41" s="49"/>
-      <c r="U41" s="49"/>
-      <c r="V41" s="49"/>
-      <c r="W41" s="49"/>
-      <c r="X41" s="49"/>
-      <c r="Y41" s="49"/>
+      <c r="A41" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="51"/>
+      <c r="L41" s="51"/>
+      <c r="M41" s="51"/>
+      <c r="N41" s="51"/>
+      <c r="O41" s="51"/>
+      <c r="P41" s="51"/>
+      <c r="Q41" s="51"/>
+      <c r="R41" s="51"/>
+      <c r="S41" s="51"/>
+      <c r="T41" s="51"/>
+      <c r="U41" s="51"/>
+      <c r="V41" s="51"/>
+      <c r="W41" s="51"/>
+      <c r="X41" s="51"/>
+      <c r="Y41" s="51"/>
     </row>
     <row r="42" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="51"/>
-      <c r="O42" s="51"/>
-      <c r="P42" s="51"/>
-      <c r="Q42" s="51"/>
-      <c r="R42" s="51"/>
-      <c r="S42" s="51"/>
-      <c r="T42" s="51"/>
-      <c r="U42" s="51"/>
-      <c r="V42" s="51"/>
-      <c r="W42" s="51"/>
-      <c r="X42" s="51"/>
-      <c r="Y42" s="52"/>
+      <c r="A42" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
+      <c r="U42" s="53"/>
+      <c r="V42" s="53"/>
+      <c r="W42" s="53"/>
+      <c r="X42" s="53"/>
+      <c r="Y42" s="54"/>
     </row>
     <row r="43" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="51"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="51"/>
-      <c r="H43" s="51"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
-      <c r="K43" s="51"/>
-      <c r="L43" s="51"/>
-      <c r="M43" s="51"/>
-      <c r="N43" s="51"/>
-      <c r="O43" s="51"/>
-      <c r="P43" s="51"/>
-      <c r="Q43" s="51"/>
-      <c r="R43" s="51"/>
-      <c r="S43" s="51"/>
-      <c r="T43" s="51"/>
-      <c r="U43" s="51"/>
-      <c r="V43" s="51"/>
-      <c r="W43" s="51"/>
-      <c r="X43" s="51"/>
-      <c r="Y43" s="52"/>
+      <c r="A43" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="53"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="53"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
+      <c r="U43" s="53"/>
+      <c r="V43" s="53"/>
+      <c r="W43" s="53"/>
+      <c r="X43" s="53"/>
+      <c r="Y43" s="54"/>
     </row>
     <row r="44" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="51"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
-      <c r="O44" s="51"/>
-      <c r="P44" s="51"/>
-      <c r="Q44" s="51"/>
-      <c r="R44" s="51"/>
-      <c r="S44" s="51"/>
-      <c r="T44" s="51"/>
-      <c r="U44" s="51"/>
-      <c r="V44" s="51"/>
-      <c r="W44" s="51"/>
-      <c r="X44" s="51"/>
-      <c r="Y44" s="52"/>
+      <c r="A44" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="53"/>
+      <c r="Q44" s="53"/>
+      <c r="R44" s="53"/>
+      <c r="S44" s="53"/>
+      <c r="T44" s="53"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="53"/>
+      <c r="W44" s="53"/>
+      <c r="X44" s="53"/>
+      <c r="Y44" s="54"/>
     </row>
     <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="50"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="51"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="51"/>
-      <c r="L45" s="51"/>
-      <c r="M45" s="51"/>
-      <c r="N45" s="51"/>
-      <c r="O45" s="51"/>
-      <c r="P45" s="51"/>
-      <c r="Q45" s="51"/>
-      <c r="R45" s="51"/>
-      <c r="S45" s="51"/>
-      <c r="T45" s="51"/>
-      <c r="U45" s="51"/>
-      <c r="V45" s="51"/>
-      <c r="W45" s="51"/>
-      <c r="X45" s="51"/>
-      <c r="Y45" s="52"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="53"/>
+      <c r="L45" s="53"/>
+      <c r="M45" s="53"/>
+      <c r="N45" s="53"/>
+      <c r="O45" s="53"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="53"/>
+      <c r="R45" s="53"/>
+      <c r="S45" s="53"/>
+      <c r="T45" s="53"/>
+      <c r="U45" s="53"/>
+      <c r="V45" s="53"/>
+      <c r="W45" s="53"/>
+      <c r="X45" s="53"/>
+      <c r="Y45" s="54"/>
     </row>
     <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="50"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="51"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="51"/>
-      <c r="O46" s="51"/>
-      <c r="P46" s="51"/>
-      <c r="Q46" s="51"/>
-      <c r="R46" s="51"/>
-      <c r="S46" s="51"/>
-      <c r="T46" s="51"/>
-      <c r="U46" s="51"/>
-      <c r="V46" s="51"/>
-      <c r="W46" s="51"/>
-      <c r="X46" s="51"/>
-      <c r="Y46" s="52"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
+      <c r="K46" s="53"/>
+      <c r="L46" s="53"/>
+      <c r="M46" s="53"/>
+      <c r="N46" s="53"/>
+      <c r="O46" s="53"/>
+      <c r="P46" s="53"/>
+      <c r="Q46" s="53"/>
+      <c r="R46" s="53"/>
+      <c r="S46" s="53"/>
+      <c r="T46" s="53"/>
+      <c r="U46" s="53"/>
+      <c r="V46" s="53"/>
+      <c r="W46" s="53"/>
+      <c r="X46" s="53"/>
+      <c r="Y46" s="54"/>
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="49"/>
-      <c r="J47" s="49"/>
-      <c r="K47" s="49"/>
-      <c r="L47" s="49"/>
-      <c r="M47" s="49"/>
-      <c r="N47" s="49"/>
-      <c r="O47" s="49"/>
-      <c r="P47" s="49"/>
-      <c r="Q47" s="49"/>
-      <c r="R47" s="49"/>
-      <c r="S47" s="49"/>
-      <c r="T47" s="49"/>
-      <c r="U47" s="49"/>
-      <c r="V47" s="49"/>
-      <c r="W47" s="49"/>
-      <c r="X47" s="49"/>
-      <c r="Y47" s="49"/>
+      <c r="A47" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="51"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="51"/>
+      <c r="R47" s="51"/>
+      <c r="S47" s="51"/>
+      <c r="T47" s="51"/>
+      <c r="U47" s="51"/>
+      <c r="V47" s="51"/>
+      <c r="W47" s="51"/>
+      <c r="X47" s="51"/>
+      <c r="Y47" s="51"/>
     </row>
     <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="50"/>
-      <c r="B48" s="51"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="51"/>
-      <c r="I48" s="51"/>
-      <c r="J48" s="51"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="51"/>
-      <c r="M48" s="51"/>
-      <c r="N48" s="51"/>
-      <c r="O48" s="51"/>
-      <c r="P48" s="51"/>
-      <c r="Q48" s="51"/>
-      <c r="R48" s="51"/>
-      <c r="S48" s="51"/>
-      <c r="T48" s="51"/>
-      <c r="U48" s="51"/>
-      <c r="V48" s="51"/>
-      <c r="W48" s="51"/>
-      <c r="X48" s="51"/>
-      <c r="Y48" s="52"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="53"/>
+      <c r="N48" s="53"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="53"/>
+      <c r="S48" s="53"/>
+      <c r="T48" s="53"/>
+      <c r="U48" s="53"/>
+      <c r="V48" s="53"/>
+      <c r="W48" s="53"/>
+      <c r="X48" s="53"/>
+      <c r="Y48" s="54"/>
     </row>
     <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="50"/>
-      <c r="B49" s="51"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="51"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="51"/>
-      <c r="J49" s="51"/>
-      <c r="K49" s="51"/>
-      <c r="L49" s="51"/>
-      <c r="M49" s="51"/>
-      <c r="N49" s="51"/>
-      <c r="O49" s="51"/>
-      <c r="P49" s="51"/>
-      <c r="Q49" s="51"/>
-      <c r="R49" s="51"/>
-      <c r="S49" s="51"/>
-      <c r="T49" s="51"/>
-      <c r="U49" s="51"/>
-      <c r="V49" s="51"/>
-      <c r="W49" s="51"/>
-      <c r="X49" s="51"/>
-      <c r="Y49" s="52"/>
+      <c r="A49" s="52"/>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="53"/>
+      <c r="L49" s="53"/>
+      <c r="M49" s="53"/>
+      <c r="N49" s="53"/>
+      <c r="O49" s="53"/>
+      <c r="P49" s="53"/>
+      <c r="Q49" s="53"/>
+      <c r="R49" s="53"/>
+      <c r="S49" s="53"/>
+      <c r="T49" s="53"/>
+      <c r="U49" s="53"/>
+      <c r="V49" s="53"/>
+      <c r="W49" s="53"/>
+      <c r="X49" s="53"/>
+      <c r="Y49" s="54"/>
     </row>
     <row r="50" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="51"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="51"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="51"/>
-      <c r="K50" s="51"/>
-      <c r="L50" s="51"/>
-      <c r="M50" s="51"/>
-      <c r="N50" s="51"/>
-      <c r="O50" s="51"/>
-      <c r="P50" s="51"/>
-      <c r="Q50" s="51"/>
-      <c r="R50" s="51"/>
-      <c r="S50" s="51"/>
-      <c r="T50" s="51"/>
-      <c r="U50" s="51"/>
-      <c r="V50" s="51"/>
-      <c r="W50" s="51"/>
-      <c r="X50" s="51"/>
-      <c r="Y50" s="52"/>
+      <c r="A50" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+      <c r="L50" s="53"/>
+      <c r="M50" s="53"/>
+      <c r="N50" s="53"/>
+      <c r="O50" s="53"/>
+      <c r="P50" s="53"/>
+      <c r="Q50" s="53"/>
+      <c r="R50" s="53"/>
+      <c r="S50" s="53"/>
+      <c r="T50" s="53"/>
+      <c r="U50" s="53"/>
+      <c r="V50" s="53"/>
+      <c r="W50" s="53"/>
+      <c r="X50" s="53"/>
+      <c r="Y50" s="54"/>
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="49"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="49"/>
-      <c r="H51" s="49"/>
-      <c r="I51" s="49"/>
-      <c r="J51" s="49"/>
-      <c r="K51" s="49"/>
-      <c r="L51" s="49"/>
-      <c r="M51" s="49"/>
-      <c r="N51" s="49"/>
-      <c r="O51" s="49"/>
-      <c r="P51" s="49"/>
-      <c r="Q51" s="49"/>
-      <c r="R51" s="49"/>
-      <c r="S51" s="49"/>
-      <c r="T51" s="49"/>
-      <c r="U51" s="49"/>
-      <c r="V51" s="49"/>
-      <c r="W51" s="49"/>
-      <c r="X51" s="49"/>
-      <c r="Y51" s="49"/>
+      <c r="A51" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="51"/>
+      <c r="O51" s="51"/>
+      <c r="P51" s="51"/>
+      <c r="Q51" s="51"/>
+      <c r="R51" s="51"/>
+      <c r="S51" s="51"/>
+      <c r="T51" s="51"/>
+      <c r="U51" s="51"/>
+      <c r="V51" s="51"/>
+      <c r="W51" s="51"/>
+      <c r="X51" s="51"/>
+      <c r="Y51" s="51"/>
     </row>
     <row r="52" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="51"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="51"/>
-      <c r="K52" s="51"/>
-      <c r="L52" s="51"/>
-      <c r="M52" s="51"/>
-      <c r="N52" s="51"/>
-      <c r="O52" s="51"/>
-      <c r="P52" s="51"/>
-      <c r="Q52" s="51"/>
-      <c r="R52" s="51"/>
-      <c r="S52" s="51"/>
-      <c r="T52" s="51"/>
-      <c r="U52" s="51"/>
-      <c r="V52" s="51"/>
-      <c r="W52" s="51"/>
-      <c r="X52" s="51"/>
-      <c r="Y52" s="52"/>
+      <c r="A52" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="53"/>
+      <c r="L52" s="53"/>
+      <c r="M52" s="53"/>
+      <c r="N52" s="53"/>
+      <c r="O52" s="53"/>
+      <c r="P52" s="53"/>
+      <c r="Q52" s="53"/>
+      <c r="R52" s="53"/>
+      <c r="S52" s="53"/>
+      <c r="T52" s="53"/>
+      <c r="U52" s="53"/>
+      <c r="V52" s="53"/>
+      <c r="W52" s="53"/>
+      <c r="X52" s="53"/>
+      <c r="Y52" s="54"/>
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="B53" s="51"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="51"/>
-      <c r="H53" s="51"/>
-      <c r="I53" s="51"/>
-      <c r="J53" s="51"/>
-      <c r="K53" s="51"/>
-      <c r="L53" s="51"/>
-      <c r="M53" s="51"/>
-      <c r="N53" s="51"/>
-      <c r="O53" s="51"/>
-      <c r="P53" s="51"/>
-      <c r="Q53" s="51"/>
-      <c r="R53" s="51"/>
-      <c r="S53" s="51"/>
-      <c r="T53" s="51"/>
-      <c r="U53" s="51"/>
-      <c r="V53" s="51"/>
-      <c r="W53" s="51"/>
-      <c r="X53" s="51"/>
-      <c r="Y53" s="52"/>
+      <c r="A53" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="53"/>
+      <c r="J53" s="53"/>
+      <c r="K53" s="53"/>
+      <c r="L53" s="53"/>
+      <c r="M53" s="53"/>
+      <c r="N53" s="53"/>
+      <c r="O53" s="53"/>
+      <c r="P53" s="53"/>
+      <c r="Q53" s="53"/>
+      <c r="R53" s="53"/>
+      <c r="S53" s="53"/>
+      <c r="T53" s="53"/>
+      <c r="U53" s="53"/>
+      <c r="V53" s="53"/>
+      <c r="W53" s="53"/>
+      <c r="X53" s="53"/>
+      <c r="Y53" s="54"/>
     </row>
     <row r="54" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="51"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="51"/>
-      <c r="H54" s="51"/>
-      <c r="I54" s="51"/>
-      <c r="J54" s="51"/>
-      <c r="K54" s="51"/>
-      <c r="L54" s="51"/>
-      <c r="M54" s="51"/>
-      <c r="N54" s="51"/>
-      <c r="O54" s="51"/>
-      <c r="P54" s="51"/>
-      <c r="Q54" s="51"/>
-      <c r="R54" s="51"/>
-      <c r="S54" s="51"/>
-      <c r="T54" s="51"/>
-      <c r="U54" s="51"/>
-      <c r="V54" s="51"/>
-      <c r="W54" s="51"/>
-      <c r="X54" s="51"/>
-      <c r="Y54" s="52"/>
+      <c r="A54" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="53"/>
+      <c r="L54" s="53"/>
+      <c r="M54" s="53"/>
+      <c r="N54" s="53"/>
+      <c r="O54" s="53"/>
+      <c r="P54" s="53"/>
+      <c r="Q54" s="53"/>
+      <c r="R54" s="53"/>
+      <c r="S54" s="53"/>
+      <c r="T54" s="53"/>
+      <c r="U54" s="53"/>
+      <c r="V54" s="53"/>
+      <c r="W54" s="53"/>
+      <c r="X54" s="53"/>
+      <c r="Y54" s="54"/>
     </row>
     <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="50"/>
-      <c r="B55" s="51"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="51"/>
-      <c r="E55" s="51"/>
-      <c r="F55" s="51"/>
-      <c r="G55" s="51"/>
-      <c r="H55" s="51"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="51"/>
-      <c r="K55" s="51"/>
-      <c r="L55" s="51"/>
-      <c r="M55" s="51"/>
-      <c r="N55" s="51"/>
-      <c r="O55" s="51"/>
-      <c r="P55" s="51"/>
-      <c r="Q55" s="51"/>
-      <c r="R55" s="51"/>
-      <c r="S55" s="51"/>
-      <c r="T55" s="51"/>
-      <c r="U55" s="51"/>
-      <c r="V55" s="51"/>
-      <c r="W55" s="51"/>
-      <c r="X55" s="51"/>
-      <c r="Y55" s="52"/>
+      <c r="A55" s="52"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="53"/>
+      <c r="L55" s="53"/>
+      <c r="M55" s="53"/>
+      <c r="N55" s="53"/>
+      <c r="O55" s="53"/>
+      <c r="P55" s="53"/>
+      <c r="Q55" s="53"/>
+      <c r="R55" s="53"/>
+      <c r="S55" s="53"/>
+      <c r="T55" s="53"/>
+      <c r="U55" s="53"/>
+      <c r="V55" s="53"/>
+      <c r="W55" s="53"/>
+      <c r="X55" s="53"/>
+      <c r="Y55" s="54"/>
     </row>
     <row r="56" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="B56" s="51"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="51"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="51"/>
-      <c r="G56" s="51"/>
-      <c r="H56" s="51"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="51"/>
-      <c r="K56" s="51"/>
-      <c r="L56" s="51"/>
-      <c r="M56" s="51"/>
-      <c r="N56" s="51"/>
-      <c r="O56" s="51"/>
-      <c r="P56" s="51"/>
-      <c r="Q56" s="51"/>
-      <c r="R56" s="51"/>
-      <c r="S56" s="51"/>
-      <c r="T56" s="51"/>
-      <c r="U56" s="51"/>
-      <c r="V56" s="51"/>
-      <c r="W56" s="51"/>
-      <c r="X56" s="51"/>
-      <c r="Y56" s="52"/>
+      <c r="A56" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="53"/>
+      <c r="L56" s="53"/>
+      <c r="M56" s="53"/>
+      <c r="N56" s="53"/>
+      <c r="O56" s="53"/>
+      <c r="P56" s="53"/>
+      <c r="Q56" s="53"/>
+      <c r="R56" s="53"/>
+      <c r="S56" s="53"/>
+      <c r="T56" s="53"/>
+      <c r="U56" s="53"/>
+      <c r="V56" s="53"/>
+      <c r="W56" s="53"/>
+      <c r="X56" s="53"/>
+      <c r="Y56" s="54"/>
     </row>
     <row r="57" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="57"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="57"/>
-      <c r="F57" s="57"/>
-      <c r="G57" s="57"/>
-      <c r="H57" s="57"/>
-      <c r="I57" s="57"/>
-      <c r="J57" s="57"/>
-      <c r="K57" s="57"/>
-      <c r="L57" s="57"/>
-      <c r="M57" s="57"/>
-      <c r="N57" s="57"/>
-      <c r="O57" s="57"/>
-      <c r="P57" s="57"/>
-      <c r="Q57" s="57"/>
-      <c r="R57" s="57"/>
-      <c r="S57" s="57"/>
-      <c r="T57" s="57"/>
-      <c r="U57" s="57"/>
-      <c r="V57" s="57"/>
-      <c r="W57" s="57"/>
-      <c r="X57" s="57"/>
-      <c r="Y57" s="58"/>
+      <c r="A57" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" s="59"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="59"/>
+      <c r="J57" s="59"/>
+      <c r="K57" s="59"/>
+      <c r="L57" s="59"/>
+      <c r="M57" s="59"/>
+      <c r="N57" s="59"/>
+      <c r="O57" s="59"/>
+      <c r="P57" s="59"/>
+      <c r="Q57" s="59"/>
+      <c r="R57" s="59"/>
+      <c r="S57" s="59"/>
+      <c r="T57" s="59"/>
+      <c r="U57" s="59"/>
+      <c r="V57" s="59"/>
+      <c r="W57" s="59"/>
+      <c r="X57" s="59"/>
+      <c r="Y57" s="60"/>
     </row>
     <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="59"/>
+      <c r="A58" s="61"/>
     </row>
     <row r="59" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="60" t="s">
-        <v>102</v>
+      <c r="A59" s="62" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement arv started during period
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="169">
   <si>
     <t>Région</t>
   </si>
@@ -85,6 +85,78 @@
   </si>
   <si>
     <t>Nombre d’adultes et d’enfants  chez qui on a initié la TARV au cours de la période de raportage (B)</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', gender: 1}</t>
+  </si>
+  <si>
+    <t>{key:'ARV_STARTED_DURING_PERIOD', age_max: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD'}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_max: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_STARTED_DURING_PERIOD', age_min: 50, gender: 1}</t>
   </si>
   <si>
     <t>Nombre d’adultes et d’enfants déjà sous TARV  reçus dans le centre en provenance d'un autre centre de traitement au cours dau cours de la période de raportage (C)</t>
@@ -606,13 +678,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -622,6 +687,13 @@
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -973,11 +1045,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -998,18 +1082,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="8" fillId="2" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1262,8 +1334,8 @@
   </sheetPr>
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB21" activeCellId="0" sqref="AB21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1317,7 +1389,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1554,41 +1626,95 @@
       <c r="AA11" s="19"/>
       <c r="AB11" s="20"/>
     </row>
-    <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="27.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="19"/>
-      <c r="AB12" s="20"/>
+      <c r="B12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="R12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="S12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="T12" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="U12" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="V12" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="W12" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="X12" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y12" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z12" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA12" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB12" s="23" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="s">
-        <v>23</v>
+      <c r="A13" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -1618,9 +1744,9 @@
       <c r="AA13" s="19"/>
       <c r="AB13" s="20"/>
     </row>
-    <row r="14" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
-        <v>24</v>
+    <row r="14" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="24" t="s">
+        <v>48</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -1650,9 +1776,9 @@
       <c r="AA14" s="19"/>
       <c r="AB14" s="20"/>
     </row>
-    <row r="15" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="s">
-        <v>25</v>
+    <row r="15" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1683,40 +1809,40 @@
       <c r="AB15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
-      <c r="AA16" s="24"/>
-      <c r="AB16" s="27"/>
+      <c r="A16" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="s">
-        <v>27</v>
+      <c r="A17" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -1747,94 +1873,94 @@
       <c r="AB17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="21" t="s">
-        <v>28</v>
+      <c r="A18" s="24" t="s">
+        <v>52</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" s="28" t="s">
-        <v>37</v>
+        <v>58</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>61</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="L18" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="N18" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="O18" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="P18" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q18" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="R18" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="S18" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="T18" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="U18" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="V18" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="W18" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="X18" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y18" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z18" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA18" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB18" s="30" t="s">
-        <v>30</v>
+        <v>62</v>
+      </c>
+      <c r="L18" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="N18" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="O18" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="P18" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q18" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="R18" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="S18" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="T18" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="U18" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="V18" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="W18" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="X18" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y18" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z18" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA18" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB18" s="23" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21" t="s">
-        <v>53</v>
+      <c r="A19" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -1865,126 +1991,126 @@
       <c r="AB19" s="20"/>
     </row>
     <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21" t="s">
-        <v>54</v>
+      <c r="A20" s="24" t="s">
+        <v>78</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" s="28" t="s">
-        <v>63</v>
+        <v>84</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>87</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="L20" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="M20" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="N20" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="O20" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="P20" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q20" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="R20" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="S20" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="T20" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="U20" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="V20" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="W20" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="X20" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y20" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z20" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA20" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB20" s="30" t="s">
-        <v>56</v>
+        <v>88</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="N20" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="O20" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="P20" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q20" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="R20" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="S20" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="T20" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="U20" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="V20" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="W20" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="X20" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y20" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z20" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA20" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB20" s="23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="27"/>
+        <v>103</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21" t="s">
-        <v>80</v>
+      <c r="A22" s="24" t="s">
+        <v>104</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -2015,8 +2141,8 @@
       <c r="AB22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="s">
-        <v>81</v>
+      <c r="A23" s="24" t="s">
+        <v>105</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -2046,9 +2172,9 @@
       <c r="AA23" s="19"/>
       <c r="AB23" s="20"/>
     </row>
-    <row r="24" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="21" t="s">
-        <v>82</v>
+    <row r="24" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="24" t="s">
+        <v>106</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2078,9 +2204,9 @@
       <c r="AA24" s="19"/>
       <c r="AB24" s="20"/>
     </row>
-    <row r="25" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21" t="s">
-        <v>83</v>
+    <row r="25" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="24" t="s">
+        <v>107</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2110,9 +2236,9 @@
       <c r="AA25" s="19"/>
       <c r="AB25" s="20"/>
     </row>
-    <row r="26" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="s">
-        <v>84</v>
+    <row r="26" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2142,9 +2268,9 @@
       <c r="AA26" s="19"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" s="22" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="21" t="s">
-        <v>85</v>
+    <row r="27" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="24" t="s">
+        <v>109</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2176,7 +2302,7 @@
     </row>
     <row r="28" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="32" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2208,7 +2334,7 @@
     </row>
     <row r="29" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="32" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2240,7 +2366,7 @@
     </row>
     <row r="30" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="32" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2272,7 +2398,7 @@
     </row>
     <row r="31" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="33" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2304,7 +2430,7 @@
     </row>
     <row r="32" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="33" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2336,7 +2462,7 @@
     </row>
     <row r="33" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="33" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2368,7 +2494,7 @@
     </row>
     <row r="34" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="34" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="B34" s="35"/>
       <c r="C34" s="35"/>
@@ -2399,7 +2525,7 @@
       <c r="AB34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="21"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -2429,8 +2555,8 @@
       <c r="AB35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="21" t="s">
-        <v>93</v>
+      <c r="A36" s="24" t="s">
+        <v>117</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2461,8 +2587,8 @@
       <c r="AB36" s="20"/>
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="21" t="s">
-        <v>94</v>
+      <c r="A37" s="24" t="s">
+        <v>118</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2493,8 +2619,8 @@
       <c r="AB37" s="20"/>
     </row>
     <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="21" t="s">
-        <v>95</v>
+      <c r="A38" s="24" t="s">
+        <v>119</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2526,7 +2652,7 @@
     </row>
     <row r="39" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2558,7 +2684,7 @@
     </row>
     <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="36" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="B40" s="37"/>
       <c r="C40" s="37"/>
@@ -2632,7 +2758,7 @@
   </sheetPr>
   <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2644,32 +2770,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="41" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,12 +2803,12 @@
     </row>
     <row r="9" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="42" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="43" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2690,7 +2816,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="44" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2698,22 +2824,22 @@
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="46" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="E14" s="47"/>
       <c r="F14" s="47" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="G14" s="47"/>
       <c r="H14" s="47" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="I14" s="47"/>
       <c r="J14" s="47" t="s">
@@ -2729,19 +2855,19 @@
       </c>
       <c r="O14" s="47"/>
       <c r="P14" s="47" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="Q14" s="47"/>
       <c r="R14" s="47" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="S14" s="47"/>
       <c r="T14" s="47" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="U14" s="47"/>
       <c r="V14" s="47" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="W14" s="47"/>
       <c r="X14" s="48" t="s">
@@ -2826,7 +2952,7 @@
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
@@ -2855,7 +2981,7 @@
     </row>
     <row r="17" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="B17" s="53"/>
       <c r="C17" s="53"/>
@@ -2884,7 +3010,7 @@
     </row>
     <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="52" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
@@ -2913,7 +3039,7 @@
     </row>
     <row r="19" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
@@ -2996,7 +3122,7 @@
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
@@ -3025,7 +3151,7 @@
     </row>
     <row r="23" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="B23" s="53"/>
       <c r="C23" s="53"/>
@@ -3054,7 +3180,7 @@
     </row>
     <row r="24" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="B24" s="53"/>
       <c r="C24" s="53"/>
@@ -3083,7 +3209,7 @@
     </row>
     <row r="25" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
@@ -3112,7 +3238,7 @@
     </row>
     <row r="26" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
@@ -3195,7 +3321,7 @@
     </row>
     <row r="29" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="55" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -3224,7 +3350,7 @@
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="51" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
@@ -3253,7 +3379,7 @@
     </row>
     <row r="31" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>
@@ -3282,7 +3408,7 @@
     </row>
     <row r="32" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>
@@ -3365,7 +3491,7 @@
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="51" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
@@ -3475,7 +3601,7 @@
     </row>
     <row r="39" customFormat="false" ht="66.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="55" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="B39" s="53"/>
       <c r="C39" s="53"/>
@@ -3504,7 +3630,7 @@
     </row>
     <row r="40" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="55" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="B40" s="53"/>
       <c r="C40" s="53"/>
@@ -3533,7 +3659,7 @@
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="51" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
@@ -3562,7 +3688,7 @@
     </row>
     <row r="42" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="52" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="B42" s="53"/>
       <c r="C42" s="53"/>
@@ -3591,7 +3717,7 @@
     </row>
     <row r="43" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="52" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="B43" s="53"/>
       <c r="C43" s="53"/>
@@ -3620,7 +3746,7 @@
     </row>
     <row r="44" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="52" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="B44" s="53"/>
       <c r="C44" s="53"/>
@@ -3703,7 +3829,7 @@
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="51" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
@@ -3786,7 +3912,7 @@
     </row>
     <row r="50" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="52" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="B50" s="53"/>
       <c r="C50" s="53"/>
@@ -3815,7 +3941,7 @@
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="51" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
@@ -3844,7 +3970,7 @@
     </row>
     <row r="52" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="56" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="B52" s="53"/>
       <c r="C52" s="53"/>
@@ -3873,7 +3999,7 @@
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="56" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="B53" s="53"/>
       <c r="C53" s="53"/>
@@ -3902,7 +4028,7 @@
     </row>
     <row r="54" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="56" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="B54" s="53"/>
       <c r="C54" s="53"/>
@@ -3958,7 +4084,7 @@
     </row>
     <row r="56" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="57" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="B56" s="53"/>
       <c r="C56" s="53"/>
@@ -3987,7 +4113,7 @@
     </row>
     <row r="57" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="58" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="B57" s="59"/>
       <c r="C57" s="59"/>
@@ -4019,7 +4145,7 @@
     </row>
     <row r="59" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="62" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement Incoming transfer during perdio
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="193">
   <si>
     <t>Région</t>
   </si>
@@ -160,6 +160,78 @@
   </si>
   <si>
     <t>Nombre d’adultes et d’enfants déjà sous TARV  reçus dans le centre en provenance d'un autre centre de traitement au cours dau cours de la période de raportage (C)</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', gender: 1}</t>
+  </si>
+  <si>
+    <t>{key:'INCOMING_TRANSFER_DURING_PERIOD', age_max: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD'}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_max: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'INCOMING_TRANSFER_DURING_PERIOD', age_min: 50, gender: 1}</t>
   </si>
   <si>
     <t>Nombre d’adultes et d’enfants déjà sous TARV  mais perdus de vue dans le centre et qui ont repris le traitement au cours au cours de la période de raportage (D)</t>
@@ -1334,8 +1406,8 @@
   </sheetPr>
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC13" activeCellId="0" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1712,41 +1784,95 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="20"/>
+      <c r="B13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="P13" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q13" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="R13" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="S13" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="T13" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="U13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="V13" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="W13" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="X13" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y13" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z13" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA13" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB13" s="23" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="24" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -1778,7 +1904,7 @@
     </row>
     <row r="15" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1810,7 +1936,7 @@
     </row>
     <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -1842,7 +1968,7 @@
     </row>
     <row r="17" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -1874,93 +2000,93 @@
     </row>
     <row r="18" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="N18" s="22" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="O18" s="22" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="P18" s="22" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="Q18" s="22" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="R18" s="22" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="S18" s="22" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="T18" s="22" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="U18" s="22" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="V18" s="22" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="W18" s="22" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="X18" s="22" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="Y18" s="22" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="Z18" s="22" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AA18" s="22" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="AB18" s="23" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -1992,93 +2118,93 @@
     </row>
     <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="N20" s="22" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="O20" s="22" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="P20" s="22" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="Q20" s="22" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="R20" s="22" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="S20" s="22" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="T20" s="22" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="U20" s="22" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="V20" s="22" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="W20" s="22" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="X20" s="22" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="Y20" s="22" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="Z20" s="22" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="AA20" s="22" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="AB20" s="23" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -2110,7 +2236,7 @@
     </row>
     <row r="22" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -2142,7 +2268,7 @@
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -2174,7 +2300,7 @@
     </row>
     <row r="24" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2206,7 +2332,7 @@
     </row>
     <row r="25" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2238,7 +2364,7 @@
     </row>
     <row r="26" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2268,9 +2394,9 @@
       <c r="AA26" s="19"/>
       <c r="AB26" s="20"/>
     </row>
-    <row r="27" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" s="25" customFormat="true" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2302,7 +2428,7 @@
     </row>
     <row r="28" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="32" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2334,7 +2460,7 @@
     </row>
     <row r="29" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="32" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2366,7 +2492,7 @@
     </row>
     <row r="30" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="32" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2398,7 +2524,7 @@
     </row>
     <row r="31" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="33" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2430,7 +2556,7 @@
     </row>
     <row r="32" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="33" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2462,7 +2588,7 @@
     </row>
     <row r="33" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="33" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2494,7 +2620,7 @@
     </row>
     <row r="34" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="34" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B34" s="35"/>
       <c r="C34" s="35"/>
@@ -2556,7 +2682,7 @@
     </row>
     <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="24" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2588,7 +2714,7 @@
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="24" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2620,7 +2746,7 @@
     </row>
     <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="24" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2652,7 +2778,7 @@
     </row>
     <row r="39" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2684,7 +2810,7 @@
     </row>
     <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="36" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="B40" s="37"/>
       <c r="C40" s="37"/>
@@ -2770,32 +2896,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="41" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2803,12 +2929,12 @@
     </row>
     <row r="9" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="42" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="43" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,7 +2942,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="44" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2824,22 +2950,22 @@
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="46" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="E14" s="47"/>
       <c r="F14" s="47" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="G14" s="47"/>
       <c r="H14" s="47" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="I14" s="47"/>
       <c r="J14" s="47" t="s">
@@ -2855,19 +2981,19 @@
       </c>
       <c r="O14" s="47"/>
       <c r="P14" s="47" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="Q14" s="47"/>
       <c r="R14" s="47" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="S14" s="47"/>
       <c r="T14" s="47" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="U14" s="47"/>
       <c r="V14" s="47" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="W14" s="47"/>
       <c r="X14" s="48" t="s">
@@ -2952,7 +3078,7 @@
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
@@ -2981,7 +3107,7 @@
     </row>
     <row r="17" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="B17" s="53"/>
       <c r="C17" s="53"/>
@@ -3010,7 +3136,7 @@
     </row>
     <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="52" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
@@ -3039,7 +3165,7 @@
     </row>
     <row r="19" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
@@ -3122,7 +3248,7 @@
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
@@ -3151,7 +3277,7 @@
     </row>
     <row r="23" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="B23" s="53"/>
       <c r="C23" s="53"/>
@@ -3180,7 +3306,7 @@
     </row>
     <row r="24" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="B24" s="53"/>
       <c r="C24" s="53"/>
@@ -3209,7 +3335,7 @@
     </row>
     <row r="25" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
@@ -3238,7 +3364,7 @@
     </row>
     <row r="26" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
@@ -3321,7 +3447,7 @@
     </row>
     <row r="29" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="55" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -3350,7 +3476,7 @@
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="51" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
@@ -3379,7 +3505,7 @@
     </row>
     <row r="31" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>
@@ -3408,7 +3534,7 @@
     </row>
     <row r="32" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>
@@ -3491,7 +3617,7 @@
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="51" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
@@ -3601,7 +3727,7 @@
     </row>
     <row r="39" customFormat="false" ht="66.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="55" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="B39" s="53"/>
       <c r="C39" s="53"/>
@@ -3630,7 +3756,7 @@
     </row>
     <row r="40" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="55" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="B40" s="53"/>
       <c r="C40" s="53"/>
@@ -3659,7 +3785,7 @@
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="51" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
@@ -3688,7 +3814,7 @@
     </row>
     <row r="42" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="52" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="B42" s="53"/>
       <c r="C42" s="53"/>
@@ -3717,7 +3843,7 @@
     </row>
     <row r="43" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="52" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="B43" s="53"/>
       <c r="C43" s="53"/>
@@ -3746,7 +3872,7 @@
     </row>
     <row r="44" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="52" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="B44" s="53"/>
       <c r="C44" s="53"/>
@@ -3829,7 +3955,7 @@
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="51" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
@@ -3912,7 +4038,7 @@
     </row>
     <row r="50" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="52" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="B50" s="53"/>
       <c r="C50" s="53"/>
@@ -3941,7 +4067,7 @@
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="51" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
@@ -3970,7 +4096,7 @@
     </row>
     <row r="52" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="56" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="B52" s="53"/>
       <c r="C52" s="53"/>
@@ -3999,7 +4125,7 @@
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="56" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="B53" s="53"/>
       <c r="C53" s="53"/>
@@ -4028,7 +4154,7 @@
     </row>
     <row r="54" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="56" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="B54" s="53"/>
       <c r="C54" s="53"/>
@@ -4084,7 +4210,7 @@
     </row>
     <row r="56" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="57" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="B56" s="53"/>
       <c r="C56" s="53"/>
@@ -4113,7 +4239,7 @@
     </row>
     <row r="57" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="58" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="B57" s="59"/>
       <c r="C57" s="59"/>
@@ -4145,7 +4271,7 @@
     </row>
     <row r="59" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="62" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement lost back patients
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="241">
   <si>
     <t>Région</t>
   </si>
@@ -235,6 +235,78 @@
   </si>
   <si>
     <t>Nombre d’adultes et d’enfants déjà sous TARV  mais perdus de vue dans le centre et qui ont repris le traitement au cours au cours de la période de raportage (D)</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', gender: 1}</t>
+  </si>
+  <si>
+    <t>{key:'ARV_LOST_BACK', age_max: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK'}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_max: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'ARV_LOST_BACK', age_min: 50, gender: 1}</t>
   </si>
   <si>
     <t>Nombre d’adultes et d’enfants déjà sous TARV  et ayant arrêté le traitement mais qui ont repris au cours au cours de la période de raportage (E)</t>
@@ -1478,8 +1550,8 @@
   </sheetPr>
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B5" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="B17:AB17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14:AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1942,41 +2014,95 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" s="25" customFormat="true" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="25" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="19"/>
-      <c r="AB14" s="20"/>
+      <c r="B14" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="L14" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="P14" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q14" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="R14" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="S14" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="T14" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="U14" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="V14" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="W14" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="X14" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y14" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z14" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA14" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB14" s="23" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" s="25" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -2008,7 +2134,7 @@
     </row>
     <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -2040,179 +2166,179 @@
     </row>
     <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="Q17" s="22" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="R17" s="22" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="S17" s="22" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="T17" s="22" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="U17" s="22" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="V17" s="22" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="W17" s="22" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="X17" s="22" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="Y17" s="22" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="Z17" s="22" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="AA17" s="22" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="AB17" s="23" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="N18" s="22" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="O18" s="22" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="P18" s="22" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="Q18" s="22" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="R18" s="22" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="S18" s="22" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="T18" s="22" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="U18" s="22" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="V18" s="22" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="W18" s="22" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="X18" s="22" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="Y18" s="22" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="Z18" s="22" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="AA18" s="22" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="AB18" s="23" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -2244,93 +2370,93 @@
     </row>
     <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="N20" s="22" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="O20" s="22" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="P20" s="22" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="Q20" s="22" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="R20" s="22" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="S20" s="22" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="T20" s="22" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="U20" s="22" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="V20" s="22" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="W20" s="22" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="X20" s="22" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="Y20" s="22" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="Z20" s="22" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="AA20" s="22" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="AB20" s="23" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -2362,7 +2488,7 @@
     </row>
     <row r="22" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -2394,7 +2520,7 @@
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -2426,7 +2552,7 @@
     </row>
     <row r="24" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2458,7 +2584,7 @@
     </row>
     <row r="25" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2490,7 +2616,7 @@
     </row>
     <row r="26" s="25" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2522,7 +2648,7 @@
     </row>
     <row r="27" s="25" customFormat="true" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2554,7 +2680,7 @@
     </row>
     <row r="28" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="32" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2586,7 +2712,7 @@
     </row>
     <row r="29" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="32" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2618,7 +2744,7 @@
     </row>
     <row r="30" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="32" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2650,7 +2776,7 @@
     </row>
     <row r="31" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="33" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2682,7 +2808,7 @@
     </row>
     <row r="32" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="33" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2714,7 +2840,7 @@
     </row>
     <row r="33" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="33" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2746,7 +2872,7 @@
     </row>
     <row r="34" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="34" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="B34" s="35"/>
       <c r="C34" s="35"/>
@@ -2808,7 +2934,7 @@
     </row>
     <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="24" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2840,7 +2966,7 @@
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="24" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2872,7 +2998,7 @@
     </row>
     <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="24" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2904,7 +3030,7 @@
     </row>
     <row r="39" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2936,7 +3062,7 @@
     </row>
     <row r="40" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="36" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="B40" s="37"/>
       <c r="C40" s="37"/>
@@ -3011,7 +3137,7 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B17:AB17 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B14:AB14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3022,32 +3148,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="41" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3055,12 +3181,12 @@
     </row>
     <row r="9" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="42" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="43" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,7 +3194,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="44" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3076,22 +3202,22 @@
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="46" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="E14" s="47"/>
       <c r="F14" s="47" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="G14" s="47"/>
       <c r="H14" s="47" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="I14" s="47"/>
       <c r="J14" s="47" t="s">
@@ -3107,19 +3233,19 @@
       </c>
       <c r="O14" s="47"/>
       <c r="P14" s="47" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="Q14" s="47"/>
       <c r="R14" s="47" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="S14" s="47"/>
       <c r="T14" s="47" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="U14" s="47"/>
       <c r="V14" s="47" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="W14" s="47"/>
       <c r="X14" s="48" t="s">
@@ -3204,7 +3330,7 @@
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
@@ -3233,7 +3359,7 @@
     </row>
     <row r="17" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="52" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="B17" s="53"/>
       <c r="C17" s="53"/>
@@ -3262,7 +3388,7 @@
     </row>
     <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="52" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
@@ -3291,7 +3417,7 @@
     </row>
     <row r="19" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
@@ -3374,7 +3500,7 @@
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
@@ -3403,7 +3529,7 @@
     </row>
     <row r="23" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="52" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="B23" s="53"/>
       <c r="C23" s="53"/>
@@ -3432,7 +3558,7 @@
     </row>
     <row r="24" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="52" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="B24" s="53"/>
       <c r="C24" s="53"/>
@@ -3461,7 +3587,7 @@
     </row>
     <row r="25" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="52" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
@@ -3490,7 +3616,7 @@
     </row>
     <row r="26" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="52" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
@@ -3573,7 +3699,7 @@
     </row>
     <row r="29" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="55" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -3602,7 +3728,7 @@
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="51" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
@@ -3631,7 +3757,7 @@
     </row>
     <row r="31" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="52" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>
@@ -3660,7 +3786,7 @@
     </row>
     <row r="32" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>
@@ -3743,7 +3869,7 @@
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="51" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
@@ -3853,7 +3979,7 @@
     </row>
     <row r="39" customFormat="false" ht="66.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="55" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="B39" s="53"/>
       <c r="C39" s="53"/>
@@ -3882,7 +4008,7 @@
     </row>
     <row r="40" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="55" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="B40" s="53"/>
       <c r="C40" s="53"/>
@@ -3911,7 +4037,7 @@
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="51" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
@@ -3940,7 +4066,7 @@
     </row>
     <row r="42" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="52" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="B42" s="53"/>
       <c r="C42" s="53"/>
@@ -3969,7 +4095,7 @@
     </row>
     <row r="43" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="52" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="B43" s="53"/>
       <c r="C43" s="53"/>
@@ -3998,7 +4124,7 @@
     </row>
     <row r="44" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="52" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="B44" s="53"/>
       <c r="C44" s="53"/>
@@ -4081,7 +4207,7 @@
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="51" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
@@ -4164,7 +4290,7 @@
     </row>
     <row r="50" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="52" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="B50" s="53"/>
       <c r="C50" s="53"/>
@@ -4193,7 +4319,7 @@
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="51" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
@@ -4222,7 +4348,7 @@
     </row>
     <row r="52" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="56" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="B52" s="53"/>
       <c r="C52" s="53"/>
@@ -4251,7 +4377,7 @@
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="56" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="B53" s="53"/>
       <c r="C53" s="53"/>
@@ -4280,7 +4406,7 @@
     </row>
     <row r="54" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="56" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="B54" s="53"/>
       <c r="C54" s="53"/>
@@ -4336,7 +4462,7 @@
     </row>
     <row r="56" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="57" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="B56" s="53"/>
       <c r="C56" s="53"/>
@@ -4365,7 +4491,7 @@
     </row>
     <row r="57" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="58" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="B57" s="59"/>
       <c r="C57" s="59"/>
@@ -4397,7 +4523,7 @@
     </row>
     <row r="59" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="62" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement followed and ctx eligible
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="313">
   <si>
     <t>Région</t>
   </si>
@@ -691,6 +691,78 @@
   </si>
   <si>
     <t>Nombre de personnes infectées par le VIH, qui répondent aux critères d’éligibilité à la prophylaxie au cotrimoxazole au cours au cours de la période de raportage</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', gender: 1}</t>
+  </si>
+  <si>
+    <t>{key:'CTX_ELIGIBLE', age_max: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE'}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_max: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CTX_ELIGIBLE', age_min: 50, gender: 1}</t>
   </si>
   <si>
     <t>Nombre de personnes  VIH, qui reçoivent  du cotrimoxazole au cours au cours de la période de raportage</t>
@@ -1664,8 +1736,8 @@
   </sheetPr>
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2708,41 +2780,95 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="16"/>
-      <c r="Z22" s="16"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="22"/>
+      <c r="B22" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q22" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="R22" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="S22" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="T22" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="U22" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="V22" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="W22" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="X22" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y22" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z22" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA22" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB22" s="17" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -2774,7 +2900,7 @@
     </row>
     <row r="24" s="19" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2806,7 +2932,7 @@
     </row>
     <row r="25" s="19" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2836,9 +2962,9 @@
       <c r="AA25" s="20"/>
       <c r="AB25" s="22"/>
     </row>
-    <row r="26" s="19" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="19" customFormat="true" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2870,7 +2996,7 @@
     </row>
     <row r="27" s="19" customFormat="true" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2902,7 +3028,7 @@
     </row>
     <row r="28" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="29" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2934,7 +3060,7 @@
     </row>
     <row r="29" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="29" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2966,7 +3092,7 @@
     </row>
     <row r="30" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="29" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2998,7 +3124,7 @@
     </row>
     <row r="31" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="30" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -3030,7 +3156,7 @@
     </row>
     <row r="32" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="30" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -3062,7 +3188,7 @@
     </row>
     <row r="33" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="30" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -3094,7 +3220,7 @@
     </row>
     <row r="34" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="31" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="B34" s="32"/>
       <c r="C34" s="32"/>
@@ -3156,7 +3282,7 @@
     </row>
     <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -3188,7 +3314,7 @@
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -3220,7 +3346,7 @@
     </row>
     <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -3252,7 +3378,7 @@
     </row>
     <row r="39" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3284,7 +3410,7 @@
     </row>
     <row r="40" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="33" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
@@ -3370,32 +3496,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
-        <v>243</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="38" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="38" t="s">
-        <v>246</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="38" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3403,12 +3529,12 @@
     </row>
     <row r="9" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="39" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="40" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,7 +3542,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3424,22 +3550,22 @@
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="43" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="C14" s="44"/>
       <c r="D14" s="44" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="E14" s="44"/>
       <c r="F14" s="44" t="s">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="G14" s="44"/>
       <c r="H14" s="44" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
       <c r="I14" s="44"/>
       <c r="J14" s="44" t="s">
@@ -3455,19 +3581,19 @@
       </c>
       <c r="O14" s="44"/>
       <c r="P14" s="44" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="Q14" s="44"/>
       <c r="R14" s="44" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="S14" s="44"/>
       <c r="T14" s="44" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="U14" s="44"/>
       <c r="V14" s="44" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="W14" s="44"/>
       <c r="X14" s="45" t="s">
@@ -3552,7 +3678,7 @@
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
@@ -3581,7 +3707,7 @@
     </row>
     <row r="17" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="49" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
@@ -3610,7 +3736,7 @@
     </row>
     <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="49" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="B18" s="50"/>
       <c r="C18" s="50"/>
@@ -3639,7 +3765,7 @@
     </row>
     <row r="19" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="49" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="B19" s="50"/>
       <c r="C19" s="50"/>
@@ -3722,7 +3848,7 @@
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="48" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
@@ -3751,7 +3877,7 @@
     </row>
     <row r="23" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="49" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
@@ -3780,7 +3906,7 @@
     </row>
     <row r="24" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="49" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="B24" s="50"/>
       <c r="C24" s="50"/>
@@ -3809,7 +3935,7 @@
     </row>
     <row r="25" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="49" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
       <c r="B25" s="50"/>
       <c r="C25" s="50"/>
@@ -3838,7 +3964,7 @@
     </row>
     <row r="26" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="49" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="B26" s="50"/>
       <c r="C26" s="50"/>
@@ -3921,7 +4047,7 @@
     </row>
     <row r="29" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="52" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="B29" s="50"/>
       <c r="C29" s="50"/>
@@ -3950,7 +4076,7 @@
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="48" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
@@ -3979,7 +4105,7 @@
     </row>
     <row r="31" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="49" t="s">
-        <v>271</v>
+        <v>295</v>
       </c>
       <c r="B31" s="50"/>
       <c r="C31" s="50"/>
@@ -4008,7 +4134,7 @@
     </row>
     <row r="32" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="49" t="s">
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="B32" s="50"/>
       <c r="C32" s="50"/>
@@ -4091,7 +4217,7 @@
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="48" t="s">
-        <v>273</v>
+        <v>297</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
@@ -4201,7 +4327,7 @@
     </row>
     <row r="39" customFormat="false" ht="66.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="52" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
       <c r="B39" s="50"/>
       <c r="C39" s="50"/>
@@ -4230,7 +4356,7 @@
     </row>
     <row r="40" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="52" t="s">
-        <v>275</v>
+        <v>299</v>
       </c>
       <c r="B40" s="50"/>
       <c r="C40" s="50"/>
@@ -4259,7 +4385,7 @@
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="48" t="s">
-        <v>276</v>
+        <v>300</v>
       </c>
       <c r="B41" s="48"/>
       <c r="C41" s="48"/>
@@ -4288,7 +4414,7 @@
     </row>
     <row r="42" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="49" t="s">
-        <v>277</v>
+        <v>301</v>
       </c>
       <c r="B42" s="50"/>
       <c r="C42" s="50"/>
@@ -4317,7 +4443,7 @@
     </row>
     <row r="43" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="49" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="B43" s="50"/>
       <c r="C43" s="50"/>
@@ -4346,7 +4472,7 @@
     </row>
     <row r="44" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="49" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="B44" s="50"/>
       <c r="C44" s="50"/>
@@ -4429,7 +4555,7 @@
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="48" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="B47" s="48"/>
       <c r="C47" s="48"/>
@@ -4512,7 +4638,7 @@
     </row>
     <row r="50" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="49" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="B50" s="50"/>
       <c r="C50" s="50"/>
@@ -4541,7 +4667,7 @@
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="48" t="s">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="B51" s="48"/>
       <c r="C51" s="48"/>
@@ -4570,7 +4696,7 @@
     </row>
     <row r="52" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="53" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="B52" s="50"/>
       <c r="C52" s="50"/>
@@ -4599,7 +4725,7 @@
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="53" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="B53" s="50"/>
       <c r="C53" s="50"/>
@@ -4628,7 +4754,7 @@
     </row>
     <row r="54" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="53" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="B54" s="50"/>
       <c r="C54" s="50"/>
@@ -4684,7 +4810,7 @@
     </row>
     <row r="56" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="54" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="B56" s="50"/>
       <c r="C56" s="50"/>
@@ -4713,7 +4839,7 @@
     </row>
     <row r="57" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="55" t="s">
-        <v>287</v>
+        <v>311</v>
       </c>
       <c r="B57" s="56"/>
       <c r="C57" s="56"/>
@@ -4745,7 +4871,7 @@
     </row>
     <row r="59" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="59" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement viral load indicators
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="625">
   <si>
     <t>Région</t>
   </si>
@@ -1669,6 +1669,78 @@
   </si>
   <si>
     <t>Nombre de personnes vivant avec le VIH et sous TARV pour lesquelles un résultat de mesure de la charge virale est disponible 12 mois après la mise en route du TARV.</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', gender: 1}</t>
+  </si>
+  <si>
+    <t>{key:'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START'}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 50, gender: 1}</t>
   </si>
   <si>
     <t>Nombre d’adultes et d’enfants infectés par le VIH qui présentent suppression charge virale (&lt;1000 copies/ml) 12 mois après la mise en route du TARV</t>
@@ -2631,7 +2703,7 @@
   <dimension ref="A1:AB57"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37:AB37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4854,41 +4926,95 @@
         <v>527</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="41.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
         <v>550</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16"/>
-      <c r="N37" s="16"/>
-      <c r="O37" s="16"/>
-      <c r="P37" s="16"/>
-      <c r="Q37" s="16"/>
-      <c r="R37" s="16"/>
-      <c r="S37" s="16"/>
-      <c r="T37" s="16"/>
-      <c r="U37" s="16"/>
-      <c r="V37" s="16"/>
-      <c r="W37" s="16"/>
-      <c r="X37" s="16"/>
-      <c r="Y37" s="16"/>
-      <c r="Z37" s="16"/>
-      <c r="AA37" s="20"/>
-      <c r="AB37" s="22"/>
-    </row>
-    <row r="38" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="36" t="s">
+        <v>551</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>552</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>553</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>554</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>555</v>
+      </c>
+      <c r="G37" s="36" t="s">
+        <v>556</v>
+      </c>
+      <c r="H37" s="36" t="s">
+        <v>557</v>
+      </c>
+      <c r="I37" s="36" t="s">
+        <v>558</v>
+      </c>
+      <c r="J37" s="36" t="s">
+        <v>559</v>
+      </c>
+      <c r="K37" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="L37" s="37" t="s">
+        <v>561</v>
+      </c>
+      <c r="M37" s="37" t="s">
+        <v>562</v>
+      </c>
+      <c r="N37" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="O37" s="37" t="s">
+        <v>563</v>
+      </c>
+      <c r="P37" s="37" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q37" s="37" t="s">
+        <v>565</v>
+      </c>
+      <c r="R37" s="37" t="s">
+        <v>566</v>
+      </c>
+      <c r="S37" s="37" t="s">
+        <v>567</v>
+      </c>
+      <c r="T37" s="37" t="s">
+        <v>568</v>
+      </c>
+      <c r="U37" s="37" t="s">
+        <v>569</v>
+      </c>
+      <c r="V37" s="37" t="s">
+        <v>570</v>
+      </c>
+      <c r="W37" s="37" t="s">
+        <v>571</v>
+      </c>
+      <c r="X37" s="37" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y37" s="37" t="s">
+        <v>573</v>
+      </c>
+      <c r="Z37" s="37" t="s">
+        <v>574</v>
+      </c>
+      <c r="AA37" s="37" t="s">
+        <v>551</v>
+      </c>
+      <c r="AB37" s="38" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="s">
-        <v>551</v>
+        <v>575</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -4918,9 +5044,9 @@
       <c r="AA38" s="20"/>
       <c r="AB38" s="22"/>
     </row>
-    <row r="39" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>552</v>
+        <v>576</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -4952,7 +5078,7 @@
     </row>
     <row r="40" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="39" t="s">
-        <v>553</v>
+        <v>577</v>
       </c>
       <c r="B40" s="40"/>
       <c r="C40" s="40"/>
@@ -5027,7 +5153,7 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B37:AB37 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5038,32 +5164,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="44" t="s">
-        <v>554</v>
+        <v>578</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>555</v>
+        <v>579</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>556</v>
+        <v>580</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="44" t="s">
-        <v>557</v>
+        <v>581</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="44" t="s">
-        <v>558</v>
+        <v>582</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44" t="s">
-        <v>559</v>
+        <v>583</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5071,12 +5197,12 @@
     </row>
     <row r="9" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="45" t="s">
-        <v>560</v>
+        <v>584</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="46" t="s">
-        <v>561</v>
+        <v>585</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5084,7 +5210,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="47" t="s">
-        <v>562</v>
+        <v>586</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5092,22 +5218,22 @@
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="49" t="s">
-        <v>563</v>
+        <v>587</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>564</v>
+        <v>588</v>
       </c>
       <c r="C14" s="50"/>
       <c r="D14" s="50" t="s">
-        <v>565</v>
+        <v>589</v>
       </c>
       <c r="E14" s="50"/>
       <c r="F14" s="50" t="s">
-        <v>566</v>
+        <v>590</v>
       </c>
       <c r="G14" s="50"/>
       <c r="H14" s="50" t="s">
-        <v>567</v>
+        <v>591</v>
       </c>
       <c r="I14" s="50"/>
       <c r="J14" s="50" t="s">
@@ -5123,19 +5249,19 @@
       </c>
       <c r="O14" s="50"/>
       <c r="P14" s="50" t="s">
-        <v>568</v>
+        <v>592</v>
       </c>
       <c r="Q14" s="50"/>
       <c r="R14" s="50" t="s">
-        <v>569</v>
+        <v>593</v>
       </c>
       <c r="S14" s="50"/>
       <c r="T14" s="50" t="s">
-        <v>570</v>
+        <v>594</v>
       </c>
       <c r="U14" s="50"/>
       <c r="V14" s="50" t="s">
-        <v>571</v>
+        <v>595</v>
       </c>
       <c r="W14" s="50"/>
       <c r="X14" s="51" t="s">
@@ -5220,7 +5346,7 @@
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="54" t="s">
-        <v>572</v>
+        <v>596</v>
       </c>
       <c r="B16" s="54"/>
       <c r="C16" s="54"/>
@@ -5249,7 +5375,7 @@
     </row>
     <row r="17" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="55" t="s">
-        <v>573</v>
+        <v>597</v>
       </c>
       <c r="B17" s="56"/>
       <c r="C17" s="56"/>
@@ -5278,7 +5404,7 @@
     </row>
     <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="55" t="s">
-        <v>574</v>
+        <v>598</v>
       </c>
       <c r="B18" s="56"/>
       <c r="C18" s="56"/>
@@ -5307,7 +5433,7 @@
     </row>
     <row r="19" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="55" t="s">
-        <v>575</v>
+        <v>599</v>
       </c>
       <c r="B19" s="56"/>
       <c r="C19" s="56"/>
@@ -5390,7 +5516,7 @@
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="54" t="s">
-        <v>576</v>
+        <v>600</v>
       </c>
       <c r="B22" s="54"/>
       <c r="C22" s="54"/>
@@ -5419,7 +5545,7 @@
     </row>
     <row r="23" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="55" t="s">
-        <v>577</v>
+        <v>601</v>
       </c>
       <c r="B23" s="56"/>
       <c r="C23" s="56"/>
@@ -5448,7 +5574,7 @@
     </row>
     <row r="24" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="55" t="s">
-        <v>578</v>
+        <v>602</v>
       </c>
       <c r="B24" s="56"/>
       <c r="C24" s="56"/>
@@ -5477,7 +5603,7 @@
     </row>
     <row r="25" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="55" t="s">
-        <v>579</v>
+        <v>603</v>
       </c>
       <c r="B25" s="56"/>
       <c r="C25" s="56"/>
@@ -5506,7 +5632,7 @@
     </row>
     <row r="26" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="55" t="s">
-        <v>580</v>
+        <v>604</v>
       </c>
       <c r="B26" s="56"/>
       <c r="C26" s="56"/>
@@ -5589,7 +5715,7 @@
     </row>
     <row r="29" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="58" t="s">
-        <v>581</v>
+        <v>605</v>
       </c>
       <c r="B29" s="56"/>
       <c r="C29" s="56"/>
@@ -5618,7 +5744,7 @@
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="54" t="s">
-        <v>582</v>
+        <v>606</v>
       </c>
       <c r="B30" s="54"/>
       <c r="C30" s="54"/>
@@ -5647,7 +5773,7 @@
     </row>
     <row r="31" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="55" t="s">
-        <v>583</v>
+        <v>607</v>
       </c>
       <c r="B31" s="56"/>
       <c r="C31" s="56"/>
@@ -5676,7 +5802,7 @@
     </row>
     <row r="32" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="55" t="s">
-        <v>584</v>
+        <v>608</v>
       </c>
       <c r="B32" s="56"/>
       <c r="C32" s="56"/>
@@ -5759,7 +5885,7 @@
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="54" t="s">
-        <v>585</v>
+        <v>609</v>
       </c>
       <c r="B35" s="54"/>
       <c r="C35" s="54"/>
@@ -5869,7 +5995,7 @@
     </row>
     <row r="39" customFormat="false" ht="66.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="58" t="s">
-        <v>586</v>
+        <v>610</v>
       </c>
       <c r="B39" s="56"/>
       <c r="C39" s="56"/>
@@ -5898,7 +6024,7 @@
     </row>
     <row r="40" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="58" t="s">
-        <v>587</v>
+        <v>611</v>
       </c>
       <c r="B40" s="56"/>
       <c r="C40" s="56"/>
@@ -5927,7 +6053,7 @@
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="54" t="s">
-        <v>588</v>
+        <v>612</v>
       </c>
       <c r="B41" s="54"/>
       <c r="C41" s="54"/>
@@ -5956,7 +6082,7 @@
     </row>
     <row r="42" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="55" t="s">
-        <v>589</v>
+        <v>613</v>
       </c>
       <c r="B42" s="56"/>
       <c r="C42" s="56"/>
@@ -5985,7 +6111,7 @@
     </row>
     <row r="43" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="55" t="s">
-        <v>590</v>
+        <v>614</v>
       </c>
       <c r="B43" s="56"/>
       <c r="C43" s="56"/>
@@ -6014,7 +6140,7 @@
     </row>
     <row r="44" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="55" t="s">
-        <v>591</v>
+        <v>615</v>
       </c>
       <c r="B44" s="56"/>
       <c r="C44" s="56"/>
@@ -6097,7 +6223,7 @@
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="54" t="s">
-        <v>592</v>
+        <v>616</v>
       </c>
       <c r="B47" s="54"/>
       <c r="C47" s="54"/>
@@ -6180,7 +6306,7 @@
     </row>
     <row r="50" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="55" t="s">
-        <v>593</v>
+        <v>617</v>
       </c>
       <c r="B50" s="56"/>
       <c r="C50" s="56"/>
@@ -6209,7 +6335,7 @@
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="54" t="s">
-        <v>594</v>
+        <v>618</v>
       </c>
       <c r="B51" s="54"/>
       <c r="C51" s="54"/>
@@ -6238,7 +6364,7 @@
     </row>
     <row r="52" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="59" t="s">
-        <v>595</v>
+        <v>619</v>
       </c>
       <c r="B52" s="56"/>
       <c r="C52" s="56"/>
@@ -6267,7 +6393,7 @@
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="59" t="s">
-        <v>596</v>
+        <v>620</v>
       </c>
       <c r="B53" s="56"/>
       <c r="C53" s="56"/>
@@ -6296,7 +6422,7 @@
     </row>
     <row r="54" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="59" t="s">
-        <v>597</v>
+        <v>621</v>
       </c>
       <c r="B54" s="56"/>
       <c r="C54" s="56"/>
@@ -6352,7 +6478,7 @@
     </row>
     <row r="56" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="60" t="s">
-        <v>598</v>
+        <v>622</v>
       </c>
       <c r="B56" s="56"/>
       <c r="C56" s="56"/>
@@ -6381,7 +6507,7 @@
     </row>
     <row r="57" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="61" t="s">
-        <v>599</v>
+        <v>623</v>
       </c>
       <c r="B57" s="62"/>
       <c r="C57" s="62"/>
@@ -6413,7 +6539,7 @@
     </row>
     <row r="59" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="65" t="s">
-        <v>600</v>
+        <v>624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement cd4 < 200 and cv < 1000
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="528" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="469" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="File active" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="697">
   <si>
     <t>Région</t>
   </si>
@@ -1746,82 +1746,226 @@
     <t>Nombre d’adultes et d’enfants infectés par le VIH qui présentent suppression charge virale (&lt;1000 copies/ml) 12 mois après la mise en route du TARV</t>
   </si>
   <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', gender: 1}</t>
+  </si>
+  <si>
+    <t>{key:'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START'}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CV_INF_1000_WITHIN_12_MONTH_AFTER_ARV_START', age_min: 50, gender: 1}</t>
+  </si>
+  <si>
     <t>Nombre de personnes vivant avec le VIH et sous TARV pour lesquelles un résultat de mesure des CD4 est disponible à l'initiation du TARV   au cours de la période de rapportage</t>
   </si>
   <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', gender: 1}</t>
-  </si>
-  <si>
-    <t>{key:'HAD_CD4_AT_ARV_START', age_max: 15}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 15}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START'}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_max: 15, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_max: 15, gender: 1}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 15, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 15, gender: 1}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_max: 1, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_max: 1, gender: 1}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 1, age_max: 4, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 5, age_max: 9, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 5, age_max: 9, gender: 1}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 10, age_max: 14, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 10, age_max: 14, gender: 1}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 15, age_max: 19, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 15, age_max: 19, gender: 1}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 20, age_max: 24, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 20, age_max: 24, gender: 1}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 25, age_max: 49, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 25, age_max: 49, gender: 1}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 50, gender: 0}</t>
-  </si>
-  <si>
-    <t>{key: 'HAD_CD4_AT_ARV_START', age_min: 50, gender: 1}</t>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', gender: 1}</t>
+  </si>
+  <si>
+    <t>{key:'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_max: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD'}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_max: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'HAD_CD4_AT_ARV_START_DURING_PERIOD', age_min: 50, gender: 1}</t>
   </si>
   <si>
     <t>Nombre de personnes vivant avec le VIH et sous TARV pour lesquelles le taux des CD4 est &lt; 200 cells/μL à l'initiation du TARV  au cours de la période de rapportage</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', gender: 1}</t>
+  </si>
+  <si>
+    <t>{key:'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_max: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 15}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD'}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_max: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_max: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 15, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 15, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_max: 1, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_max: 1, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 1, age_max: 4, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 5, age_max: 9, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 5, age_max: 9, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 10, age_max: 14, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 10, age_max: 14, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 15, age_max: 19, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 15, age_max: 19, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 20, age_max: 24, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 20, age_max: 24, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 25, age_max: 49, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 25, age_max: 49, gender: 1}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 50, gender: 0}</t>
+  </si>
+  <si>
+    <t>{key: 'CD4_INF_200_AT_ARV_START_DURING_PERIOD', age_min: 50, gender: 1}</t>
   </si>
   <si>
     <t>République du Niger</t>
@@ -2205,7 +2349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="20">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -2258,20 +2402,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="double"/>
       <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="double"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="double"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="double"/>
       <top style="thin"/>
       <bottom style="double"/>
       <diagonal/>
@@ -2388,7 +2518,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2533,47 +2663,19 @@
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2583,6 +2685,14 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="8" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2597,23 +2707,19 @@
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2621,27 +2727,23 @@
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2730,15 +2832,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>216000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>128160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>672120</xdr:colOff>
+      <xdr:colOff>698760</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2751,8 +2853,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="189000" y="736920"/>
-          <a:ext cx="483120" cy="359280"/>
+          <a:off x="216000" y="727920"/>
+          <a:ext cx="482760" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2774,8 +2876,8 @@
   </sheetPr>
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39:AB39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38:AB38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4916,85 +5018,85 @@
       <c r="A36" s="18" t="s">
         <v>525</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="15" t="s">
         <v>526</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="15" t="s">
         <v>527</v>
       </c>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="15" t="s">
         <v>528</v>
       </c>
-      <c r="E36" s="36" t="s">
+      <c r="E36" s="15" t="s">
         <v>529</v>
       </c>
-      <c r="F36" s="36" t="s">
+      <c r="F36" s="15" t="s">
         <v>530</v>
       </c>
-      <c r="G36" s="36" t="s">
+      <c r="G36" s="15" t="s">
         <v>531</v>
       </c>
-      <c r="H36" s="36" t="s">
+      <c r="H36" s="15" t="s">
         <v>532</v>
       </c>
-      <c r="I36" s="36" t="s">
+      <c r="I36" s="15" t="s">
         <v>533</v>
       </c>
-      <c r="J36" s="36" t="s">
+      <c r="J36" s="15" t="s">
         <v>534</v>
       </c>
-      <c r="K36" s="37" t="s">
+      <c r="K36" s="16" t="s">
         <v>535</v>
       </c>
-      <c r="L36" s="37" t="s">
+      <c r="L36" s="16" t="s">
         <v>536</v>
       </c>
-      <c r="M36" s="37" t="s">
+      <c r="M36" s="16" t="s">
         <v>537</v>
       </c>
-      <c r="N36" s="37" t="s">
+      <c r="N36" s="16" t="s">
         <v>535</v>
       </c>
-      <c r="O36" s="37" t="s">
+      <c r="O36" s="16" t="s">
         <v>538</v>
       </c>
-      <c r="P36" s="37" t="s">
+      <c r="P36" s="16" t="s">
         <v>539</v>
       </c>
-      <c r="Q36" s="37" t="s">
+      <c r="Q36" s="16" t="s">
         <v>540</v>
       </c>
-      <c r="R36" s="37" t="s">
+      <c r="R36" s="16" t="s">
         <v>541</v>
       </c>
-      <c r="S36" s="37" t="s">
+      <c r="S36" s="16" t="s">
         <v>542</v>
       </c>
-      <c r="T36" s="37" t="s">
+      <c r="T36" s="16" t="s">
         <v>543</v>
       </c>
-      <c r="U36" s="37" t="s">
+      <c r="U36" s="16" t="s">
         <v>544</v>
       </c>
-      <c r="V36" s="37" t="s">
+      <c r="V36" s="16" t="s">
         <v>545</v>
       </c>
-      <c r="W36" s="37" t="s">
+      <c r="W36" s="16" t="s">
         <v>546</v>
       </c>
-      <c r="X36" s="37" t="s">
+      <c r="X36" s="16" t="s">
         <v>547</v>
       </c>
-      <c r="Y36" s="37" t="s">
+      <c r="Y36" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="Z36" s="37" t="s">
+      <c r="Z36" s="16" t="s">
         <v>549</v>
       </c>
-      <c r="AA36" s="37" t="s">
+      <c r="AA36" s="16" t="s">
         <v>526</v>
       </c>
-      <c r="AB36" s="38" t="s">
+      <c r="AB36" s="17" t="s">
         <v>527</v>
       </c>
     </row>
@@ -5002,239 +5104,349 @@
       <c r="A37" s="18" t="s">
         <v>550</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="15" t="s">
         <v>551</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="15" t="s">
         <v>552</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="15" t="s">
         <v>553</v>
       </c>
-      <c r="E37" s="36" t="s">
+      <c r="E37" s="15" t="s">
         <v>554</v>
       </c>
-      <c r="F37" s="36" t="s">
+      <c r="F37" s="15" t="s">
         <v>555</v>
       </c>
-      <c r="G37" s="36" t="s">
+      <c r="G37" s="15" t="s">
         <v>556</v>
       </c>
-      <c r="H37" s="36" t="s">
+      <c r="H37" s="15" t="s">
         <v>557</v>
       </c>
-      <c r="I37" s="36" t="s">
+      <c r="I37" s="15" t="s">
         <v>558</v>
       </c>
-      <c r="J37" s="36" t="s">
+      <c r="J37" s="15" t="s">
         <v>559</v>
       </c>
-      <c r="K37" s="37" t="s">
+      <c r="K37" s="16" t="s">
         <v>560</v>
       </c>
-      <c r="L37" s="37" t="s">
+      <c r="L37" s="16" t="s">
         <v>561</v>
       </c>
-      <c r="M37" s="37" t="s">
+      <c r="M37" s="16" t="s">
         <v>562</v>
       </c>
-      <c r="N37" s="37" t="s">
+      <c r="N37" s="16" t="s">
         <v>560</v>
       </c>
-      <c r="O37" s="37" t="s">
+      <c r="O37" s="16" t="s">
         <v>563</v>
       </c>
-      <c r="P37" s="37" t="s">
+      <c r="P37" s="16" t="s">
         <v>564</v>
       </c>
-      <c r="Q37" s="37" t="s">
+      <c r="Q37" s="16" t="s">
         <v>565</v>
       </c>
-      <c r="R37" s="37" t="s">
+      <c r="R37" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="S37" s="37" t="s">
+      <c r="S37" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="T37" s="37" t="s">
+      <c r="T37" s="16" t="s">
         <v>568</v>
       </c>
-      <c r="U37" s="37" t="s">
+      <c r="U37" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="V37" s="37" t="s">
+      <c r="V37" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="W37" s="37" t="s">
+      <c r="W37" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="X37" s="37" t="s">
+      <c r="X37" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="Y37" s="37" t="s">
+      <c r="Y37" s="16" t="s">
         <v>573</v>
       </c>
-      <c r="Z37" s="37" t="s">
+      <c r="Z37" s="16" t="s">
         <v>574</v>
       </c>
-      <c r="AA37" s="37" t="s">
+      <c r="AA37" s="16" t="s">
         <v>551</v>
       </c>
-      <c r="AB37" s="38" t="s">
+      <c r="AB37" s="17" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="s">
         <v>575</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
-      <c r="O38" s="16"/>
-      <c r="P38" s="16"/>
-      <c r="Q38" s="16"/>
-      <c r="R38" s="16"/>
-      <c r="S38" s="16"/>
-      <c r="T38" s="16"/>
-      <c r="U38" s="16"/>
-      <c r="V38" s="16"/>
-      <c r="W38" s="16"/>
-      <c r="X38" s="16"/>
-      <c r="Y38" s="16"/>
-      <c r="Z38" s="16"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="22"/>
+      <c r="B38" s="15" t="s">
+        <v>576</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>577</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>578</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>582</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>583</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>584</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>586</v>
+      </c>
+      <c r="M38" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="N38" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="O38" s="16" t="s">
+        <v>588</v>
+      </c>
+      <c r="P38" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="Q38" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="R38" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="S38" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="T38" s="16" t="s">
+        <v>593</v>
+      </c>
+      <c r="U38" s="16" t="s">
+        <v>594</v>
+      </c>
+      <c r="V38" s="16" t="s">
+        <v>595</v>
+      </c>
+      <c r="W38" s="16" t="s">
+        <v>596</v>
+      </c>
+      <c r="X38" s="16" t="s">
+        <v>597</v>
+      </c>
+      <c r="Y38" s="16" t="s">
+        <v>598</v>
+      </c>
+      <c r="Z38" s="16" t="s">
+        <v>599</v>
+      </c>
+      <c r="AA38" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="AB38" s="17" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>576</v>
-      </c>
-      <c r="B39" s="36" t="s">
-        <v>577</v>
-      </c>
-      <c r="C39" s="36" t="s">
-        <v>578</v>
-      </c>
-      <c r="D39" s="36" t="s">
-        <v>579</v>
-      </c>
-      <c r="E39" s="36" t="s">
-        <v>580</v>
-      </c>
-      <c r="F39" s="36" t="s">
-        <v>581</v>
-      </c>
-      <c r="G39" s="36" t="s">
-        <v>582</v>
-      </c>
-      <c r="H39" s="36" t="s">
-        <v>583</v>
-      </c>
-      <c r="I39" s="36" t="s">
-        <v>584</v>
-      </c>
-      <c r="J39" s="36" t="s">
-        <v>585</v>
-      </c>
-      <c r="K39" s="37" t="s">
-        <v>586</v>
-      </c>
-      <c r="L39" s="37" t="s">
-        <v>587</v>
-      </c>
-      <c r="M39" s="37" t="s">
-        <v>588</v>
-      </c>
-      <c r="N39" s="37" t="s">
-        <v>586</v>
-      </c>
-      <c r="O39" s="37" t="s">
-        <v>589</v>
-      </c>
-      <c r="P39" s="37" t="s">
-        <v>590</v>
-      </c>
-      <c r="Q39" s="37" t="s">
-        <v>591</v>
-      </c>
-      <c r="R39" s="37" t="s">
-        <v>592</v>
-      </c>
-      <c r="S39" s="37" t="s">
-        <v>593</v>
-      </c>
-      <c r="T39" s="37" t="s">
-        <v>594</v>
-      </c>
-      <c r="U39" s="37" t="s">
-        <v>595</v>
-      </c>
-      <c r="V39" s="37" t="s">
-        <v>596</v>
-      </c>
-      <c r="W39" s="37" t="s">
-        <v>597</v>
-      </c>
-      <c r="X39" s="37" t="s">
-        <v>598</v>
-      </c>
-      <c r="Y39" s="37" t="s">
-        <v>599</v>
-      </c>
-      <c r="Z39" s="37" t="s">
         <v>600</v>
       </c>
-      <c r="AA39" s="37" t="s">
-        <v>577</v>
-      </c>
-      <c r="AB39" s="38" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="39" t="s">
+      <c r="B39" s="15" t="s">
         <v>601</v>
       </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="42"/>
-      <c r="Q40" s="42"/>
-      <c r="R40" s="42"/>
-      <c r="S40" s="42"/>
-      <c r="T40" s="42"/>
-      <c r="U40" s="42"/>
-      <c r="V40" s="42"/>
-      <c r="W40" s="42"/>
-      <c r="X40" s="42"/>
-      <c r="Y40" s="42"/>
-      <c r="Z40" s="42"/>
-      <c r="AA40" s="41"/>
-      <c r="AB40" s="43"/>
+      <c r="C39" s="15" t="s">
+        <v>602</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>603</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>604</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>605</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>607</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>609</v>
+      </c>
+      <c r="K39" s="16" t="s">
+        <v>610</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>611</v>
+      </c>
+      <c r="M39" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="N39" s="16" t="s">
+        <v>610</v>
+      </c>
+      <c r="O39" s="16" t="s">
+        <v>613</v>
+      </c>
+      <c r="P39" s="16" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q39" s="16" t="s">
+        <v>615</v>
+      </c>
+      <c r="R39" s="16" t="s">
+        <v>616</v>
+      </c>
+      <c r="S39" s="16" t="s">
+        <v>617</v>
+      </c>
+      <c r="T39" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="U39" s="16" t="s">
+        <v>619</v>
+      </c>
+      <c r="V39" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="W39" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="X39" s="16" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y39" s="16" t="s">
+        <v>623</v>
+      </c>
+      <c r="Z39" s="16" t="s">
+        <v>624</v>
+      </c>
+      <c r="AA39" s="16" t="s">
+        <v>601</v>
+      </c>
+      <c r="AB39" s="17" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="36" t="s">
+        <v>625</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>626</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>627</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>628</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>629</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>630</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>631</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>632</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>633</v>
+      </c>
+      <c r="J40" s="15" t="s">
+        <v>634</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>636</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>637</v>
+      </c>
+      <c r="N40" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="O40" s="16" t="s">
+        <v>638</v>
+      </c>
+      <c r="P40" s="16" t="s">
+        <v>639</v>
+      </c>
+      <c r="Q40" s="16" t="s">
+        <v>640</v>
+      </c>
+      <c r="R40" s="16" t="s">
+        <v>641</v>
+      </c>
+      <c r="S40" s="16" t="s">
+        <v>642</v>
+      </c>
+      <c r="T40" s="16" t="s">
+        <v>643</v>
+      </c>
+      <c r="U40" s="16" t="s">
+        <v>644</v>
+      </c>
+      <c r="V40" s="16" t="s">
+        <v>645</v>
+      </c>
+      <c r="W40" s="16" t="s">
+        <v>646</v>
+      </c>
+      <c r="X40" s="16" t="s">
+        <v>647</v>
+      </c>
+      <c r="Y40" s="16" t="s">
+        <v>648</v>
+      </c>
+      <c r="Z40" s="16" t="s">
+        <v>649</v>
+      </c>
+      <c r="AA40" s="16" t="s">
+        <v>626</v>
+      </c>
+      <c r="AB40" s="17" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="22">
@@ -5279,7 +5491,7 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B39:AB39 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B38:AB38 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5289,1383 +5501,1383 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
-        <v>602</v>
+      <c r="A1" s="37" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
-        <v>603</v>
+      <c r="A2" s="37" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
-        <v>604</v>
+      <c r="A3" s="37" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
-        <v>605</v>
+      <c r="A4" s="37" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
-        <v>606</v>
+      <c r="A6" s="37" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44" t="s">
-        <v>607</v>
+      <c r="A7" s="37" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44"/>
+      <c r="A8" s="37"/>
     </row>
     <row r="9" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="s">
-        <v>608</v>
+      <c r="A9" s="38" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="46" t="s">
-        <v>609</v>
+      <c r="A10" s="39" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47"/>
+      <c r="A11" s="40"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="47" t="s">
-        <v>610</v>
+      <c r="A12" s="40" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="48"/>
+      <c r="A13" s="41"/>
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="49" t="s">
-        <v>611</v>
-      </c>
-      <c r="B14" s="50" t="s">
-        <v>612</v>
-      </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50" t="s">
-        <v>613</v>
-      </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50" t="s">
-        <v>614</v>
-      </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50" t="s">
-        <v>615</v>
-      </c>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50" t="s">
+      <c r="A14" s="42" t="s">
+        <v>659</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>660</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43" t="s">
+        <v>661</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43" t="s">
+        <v>662</v>
+      </c>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43" t="s">
+        <v>663</v>
+      </c>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50" t="s">
+      <c r="K14" s="43"/>
+      <c r="L14" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50" t="s">
+      <c r="M14" s="43"/>
+      <c r="N14" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50" t="s">
-        <v>616</v>
-      </c>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="50" t="s">
-        <v>617</v>
-      </c>
-      <c r="S14" s="50"/>
-      <c r="T14" s="50" t="s">
-        <v>618</v>
-      </c>
-      <c r="U14" s="50"/>
-      <c r="V14" s="50" t="s">
-        <v>619</v>
-      </c>
-      <c r="W14" s="50"/>
-      <c r="X14" s="51" t="s">
+      <c r="O14" s="43"/>
+      <c r="P14" s="43" t="s">
+        <v>664</v>
+      </c>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43" t="s">
+        <v>665</v>
+      </c>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43" t="s">
+        <v>666</v>
+      </c>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43" t="s">
+        <v>667</v>
+      </c>
+      <c r="W14" s="43"/>
+      <c r="X14" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="Y14" s="51"/>
+      <c r="Y14" s="44"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="49"/>
-      <c r="B15" s="52" t="s">
+      <c r="A15" s="42"/>
+      <c r="B15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="52" t="s">
+      <c r="G15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="52" t="s">
+      <c r="H15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="52" t="s">
+      <c r="I15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="52" t="s">
+      <c r="J15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="52" t="s">
+      <c r="K15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="L15" s="52" t="s">
+      <c r="L15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="M15" s="52" t="s">
+      <c r="M15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="N15" s="52" t="s">
+      <c r="N15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="O15" s="52" t="s">
+      <c r="O15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="52" t="s">
+      <c r="P15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="Q15" s="52" t="s">
+      <c r="Q15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="R15" s="52" t="s">
+      <c r="R15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="S15" s="52" t="s">
+      <c r="S15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="T15" s="52" t="s">
+      <c r="T15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="U15" s="52" t="s">
+      <c r="U15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="V15" s="52" t="s">
+      <c r="V15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="W15" s="52" t="s">
+      <c r="W15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="X15" s="52" t="s">
+      <c r="X15" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="Y15" s="53" t="s">
+      <c r="Y15" s="46" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="54" t="s">
-        <v>620</v>
-      </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="54"/>
-      <c r="Q16" s="54"/>
-      <c r="R16" s="54"/>
-      <c r="S16" s="54"/>
-      <c r="T16" s="54"/>
-      <c r="U16" s="54"/>
-      <c r="V16" s="54"/>
-      <c r="W16" s="54"/>
-      <c r="X16" s="54"/>
-      <c r="Y16" s="54"/>
+      <c r="A16" s="47" t="s">
+        <v>668</v>
+      </c>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="47"/>
     </row>
     <row r="17" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="55" t="s">
-        <v>621</v>
-      </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="56"/>
-      <c r="T17" s="56"/>
-      <c r="U17" s="56"/>
-      <c r="V17" s="56"/>
-      <c r="W17" s="56"/>
-      <c r="X17" s="56"/>
-      <c r="Y17" s="57"/>
+      <c r="A17" s="48" t="s">
+        <v>669</v>
+      </c>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="49"/>
+      <c r="V17" s="49"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="50"/>
     </row>
     <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="55" t="s">
-        <v>622</v>
-      </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="56"/>
-      <c r="P18" s="56"/>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="56"/>
-      <c r="S18" s="56"/>
-      <c r="T18" s="56"/>
-      <c r="U18" s="56"/>
-      <c r="V18" s="56"/>
-      <c r="W18" s="56"/>
-      <c r="X18" s="56"/>
-      <c r="Y18" s="57"/>
+      <c r="A18" s="48" t="s">
+        <v>670</v>
+      </c>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="49"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="49"/>
+      <c r="Y18" s="50"/>
     </row>
     <row r="19" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="55" t="s">
-        <v>623</v>
-      </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="56"/>
-      <c r="S19" s="56"/>
-      <c r="T19" s="56"/>
-      <c r="U19" s="56"/>
-      <c r="V19" s="56"/>
-      <c r="W19" s="56"/>
-      <c r="X19" s="56"/>
-      <c r="Y19" s="57"/>
+      <c r="A19" s="48" t="s">
+        <v>671</v>
+      </c>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="49"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="49"/>
+      <c r="V19" s="49"/>
+      <c r="W19" s="49"/>
+      <c r="X19" s="49"/>
+      <c r="Y19" s="50"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="55"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
-      <c r="T20" s="56"/>
-      <c r="U20" s="56"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="56"/>
-      <c r="Y20" s="57"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="49"/>
+      <c r="V20" s="49"/>
+      <c r="W20" s="49"/>
+      <c r="X20" s="49"/>
+      <c r="Y20" s="50"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="55"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="56"/>
-      <c r="U21" s="56"/>
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
-      <c r="Y21" s="57"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="49"/>
+      <c r="V21" s="49"/>
+      <c r="W21" s="49"/>
+      <c r="X21" s="49"/>
+      <c r="Y21" s="50"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="54" t="s">
-        <v>624</v>
-      </c>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
-      <c r="P22" s="54"/>
-      <c r="Q22" s="54"/>
-      <c r="R22" s="54"/>
-      <c r="S22" s="54"/>
-      <c r="T22" s="54"/>
-      <c r="U22" s="54"/>
-      <c r="V22" s="54"/>
-      <c r="W22" s="54"/>
-      <c r="X22" s="54"/>
-      <c r="Y22" s="54"/>
+      <c r="A22" s="47" t="s">
+        <v>672</v>
+      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="47"/>
+      <c r="V22" s="47"/>
+      <c r="W22" s="47"/>
+      <c r="X22" s="47"/>
+      <c r="Y22" s="47"/>
     </row>
     <row r="23" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="55" t="s">
-        <v>625</v>
-      </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="56"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="56"/>
-      <c r="U23" s="56"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="56"/>
-      <c r="Y23" s="57"/>
+      <c r="A23" s="48" t="s">
+        <v>673</v>
+      </c>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="49"/>
+      <c r="U23" s="49"/>
+      <c r="V23" s="49"/>
+      <c r="W23" s="49"/>
+      <c r="X23" s="49"/>
+      <c r="Y23" s="50"/>
     </row>
     <row r="24" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="55" t="s">
-        <v>626</v>
-      </c>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="56"/>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="56"/>
-      <c r="S24" s="56"/>
-      <c r="T24" s="56"/>
-      <c r="U24" s="56"/>
-      <c r="V24" s="56"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="56"/>
-      <c r="Y24" s="57"/>
+      <c r="A24" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+      <c r="U24" s="49"/>
+      <c r="V24" s="49"/>
+      <c r="W24" s="49"/>
+      <c r="X24" s="49"/>
+      <c r="Y24" s="50"/>
     </row>
     <row r="25" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="55" t="s">
-        <v>627</v>
-      </c>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="56"/>
-      <c r="S25" s="56"/>
-      <c r="T25" s="56"/>
-      <c r="U25" s="56"/>
-      <c r="V25" s="56"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="56"/>
-      <c r="Y25" s="57"/>
+      <c r="A25" s="48" t="s">
+        <v>675</v>
+      </c>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="49"/>
+      <c r="U25" s="49"/>
+      <c r="V25" s="49"/>
+      <c r="W25" s="49"/>
+      <c r="X25" s="49"/>
+      <c r="Y25" s="50"/>
     </row>
     <row r="26" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="55" t="s">
-        <v>628</v>
-      </c>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="56"/>
-      <c r="R26" s="56"/>
-      <c r="S26" s="56"/>
-      <c r="T26" s="56"/>
-      <c r="U26" s="56"/>
-      <c r="V26" s="56"/>
-      <c r="W26" s="56"/>
-      <c r="X26" s="56"/>
-      <c r="Y26" s="57"/>
+      <c r="A26" s="48" t="s">
+        <v>676</v>
+      </c>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="49"/>
+      <c r="U26" s="49"/>
+      <c r="V26" s="49"/>
+      <c r="W26" s="49"/>
+      <c r="X26" s="49"/>
+      <c r="Y26" s="50"/>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="55"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="56"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="56"/>
-      <c r="S27" s="56"/>
-      <c r="T27" s="56"/>
-      <c r="U27" s="56"/>
-      <c r="V27" s="56"/>
-      <c r="W27" s="56"/>
-      <c r="X27" s="56"/>
-      <c r="Y27" s="57"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="49"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="49"/>
+      <c r="U27" s="49"/>
+      <c r="V27" s="49"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="49"/>
+      <c r="Y27" s="50"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="55"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="56"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="56"/>
-      <c r="T28" s="56"/>
-      <c r="U28" s="56"/>
-      <c r="V28" s="56"/>
-      <c r="W28" s="56"/>
-      <c r="X28" s="56"/>
-      <c r="Y28" s="57"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="49"/>
+      <c r="U28" s="49"/>
+      <c r="V28" s="49"/>
+      <c r="W28" s="49"/>
+      <c r="X28" s="49"/>
+      <c r="Y28" s="50"/>
     </row>
     <row r="29" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="58" t="s">
-        <v>629</v>
-      </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="56"/>
-      <c r="S29" s="56"/>
-      <c r="T29" s="56"/>
-      <c r="U29" s="56"/>
-      <c r="V29" s="56"/>
-      <c r="W29" s="56"/>
-      <c r="X29" s="56"/>
-      <c r="Y29" s="57"/>
+      <c r="A29" s="51" t="s">
+        <v>677</v>
+      </c>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="49"/>
+      <c r="U29" s="49"/>
+      <c r="V29" s="49"/>
+      <c r="W29" s="49"/>
+      <c r="X29" s="49"/>
+      <c r="Y29" s="50"/>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="54" t="s">
-        <v>630</v>
-      </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="54"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="54"/>
-      <c r="T30" s="54"/>
-      <c r="U30" s="54"/>
-      <c r="V30" s="54"/>
-      <c r="W30" s="54"/>
-      <c r="X30" s="54"/>
-      <c r="Y30" s="54"/>
+      <c r="A30" s="47" t="s">
+        <v>678</v>
+      </c>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+      <c r="Q30" s="47"/>
+      <c r="R30" s="47"/>
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="47"/>
+      <c r="V30" s="47"/>
+      <c r="W30" s="47"/>
+      <c r="X30" s="47"/>
+      <c r="Y30" s="47"/>
     </row>
     <row r="31" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="55" t="s">
-        <v>631</v>
-      </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="56"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
-      <c r="X31" s="56"/>
-      <c r="Y31" s="57"/>
+      <c r="A31" s="48" t="s">
+        <v>679</v>
+      </c>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+      <c r="U31" s="49"/>
+      <c r="V31" s="49"/>
+      <c r="W31" s="49"/>
+      <c r="X31" s="49"/>
+      <c r="Y31" s="50"/>
     </row>
     <row r="32" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="55" t="s">
-        <v>632</v>
-      </c>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
-      <c r="Q32" s="56"/>
-      <c r="R32" s="56"/>
-      <c r="S32" s="56"/>
-      <c r="T32" s="56"/>
-      <c r="U32" s="56"/>
-      <c r="V32" s="56"/>
-      <c r="W32" s="56"/>
-      <c r="X32" s="56"/>
-      <c r="Y32" s="57"/>
+      <c r="A32" s="48" t="s">
+        <v>680</v>
+      </c>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="49"/>
+      <c r="U32" s="49"/>
+      <c r="V32" s="49"/>
+      <c r="W32" s="49"/>
+      <c r="X32" s="49"/>
+      <c r="Y32" s="50"/>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="55"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="56"/>
-      <c r="Q33" s="56"/>
-      <c r="R33" s="56"/>
-      <c r="S33" s="56"/>
-      <c r="T33" s="56"/>
-      <c r="U33" s="56"/>
-      <c r="V33" s="56"/>
-      <c r="W33" s="56"/>
-      <c r="X33" s="56"/>
-      <c r="Y33" s="57"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="49"/>
+      <c r="V33" s="49"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="49"/>
+      <c r="Y33" s="50"/>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="55"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
-      <c r="L34" s="56"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="56"/>
-      <c r="O34" s="56"/>
-      <c r="P34" s="56"/>
-      <c r="Q34" s="56"/>
-      <c r="R34" s="56"/>
-      <c r="S34" s="56"/>
-      <c r="T34" s="56"/>
-      <c r="U34" s="56"/>
-      <c r="V34" s="56"/>
-      <c r="W34" s="56"/>
-      <c r="X34" s="56"/>
-      <c r="Y34" s="57"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="49"/>
+      <c r="V34" s="49"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="49"/>
+      <c r="Y34" s="50"/>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="54" t="s">
-        <v>633</v>
-      </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="54"/>
-      <c r="L35" s="54"/>
-      <c r="M35" s="54"/>
-      <c r="N35" s="54"/>
-      <c r="O35" s="54"/>
-      <c r="P35" s="54"/>
-      <c r="Q35" s="54"/>
-      <c r="R35" s="54"/>
-      <c r="S35" s="54"/>
-      <c r="T35" s="54"/>
-      <c r="U35" s="54"/>
-      <c r="V35" s="54"/>
-      <c r="W35" s="54"/>
-      <c r="X35" s="54"/>
-      <c r="Y35" s="54"/>
+      <c r="A35" s="47" t="s">
+        <v>681</v>
+      </c>
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="47"/>
+      <c r="T35" s="47"/>
+      <c r="U35" s="47"/>
+      <c r="V35" s="47"/>
+      <c r="W35" s="47"/>
+      <c r="X35" s="47"/>
+      <c r="Y35" s="47"/>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="55"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="56"/>
-      <c r="M36" s="56"/>
-      <c r="N36" s="56"/>
-      <c r="O36" s="56"/>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56"/>
-      <c r="R36" s="56"/>
-      <c r="S36" s="56"/>
-      <c r="T36" s="56"/>
-      <c r="U36" s="56"/>
-      <c r="V36" s="56"/>
-      <c r="W36" s="56"/>
-      <c r="X36" s="56"/>
-      <c r="Y36" s="57"/>
+      <c r="A36" s="48"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="49"/>
+      <c r="P36" s="49"/>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="49"/>
+      <c r="U36" s="49"/>
+      <c r="V36" s="49"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="49"/>
+      <c r="Y36" s="50"/>
     </row>
     <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="58"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="56"/>
-      <c r="T37" s="56"/>
-      <c r="U37" s="56"/>
-      <c r="V37" s="56"/>
-      <c r="W37" s="56"/>
-      <c r="X37" s="56"/>
-      <c r="Y37" s="57"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="49"/>
+      <c r="U37" s="49"/>
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="50"/>
     </row>
     <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="58"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="56"/>
-      <c r="O38" s="56"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="56"/>
-      <c r="R38" s="56"/>
-      <c r="S38" s="56"/>
-      <c r="T38" s="56"/>
-      <c r="U38" s="56"/>
-      <c r="V38" s="56"/>
-      <c r="W38" s="56"/>
-      <c r="X38" s="56"/>
-      <c r="Y38" s="57"/>
+      <c r="A38" s="51"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="49"/>
+      <c r="R38" s="49"/>
+      <c r="S38" s="49"/>
+      <c r="T38" s="49"/>
+      <c r="U38" s="49"/>
+      <c r="V38" s="49"/>
+      <c r="W38" s="49"/>
+      <c r="X38" s="49"/>
+      <c r="Y38" s="50"/>
     </row>
     <row r="39" customFormat="false" ht="66.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="58" t="s">
-        <v>634</v>
-      </c>
-      <c r="B39" s="56"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="56"/>
-      <c r="R39" s="56"/>
-      <c r="S39" s="56"/>
-      <c r="T39" s="56"/>
-      <c r="U39" s="56"/>
-      <c r="V39" s="56"/>
-      <c r="W39" s="56"/>
-      <c r="X39" s="56"/>
-      <c r="Y39" s="57"/>
+      <c r="A39" s="51" t="s">
+        <v>682</v>
+      </c>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="49"/>
+      <c r="U39" s="49"/>
+      <c r="V39" s="49"/>
+      <c r="W39" s="49"/>
+      <c r="X39" s="49"/>
+      <c r="Y39" s="50"/>
     </row>
     <row r="40" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="58" t="s">
-        <v>635</v>
-      </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="56"/>
-      <c r="N40" s="56"/>
-      <c r="O40" s="56"/>
-      <c r="P40" s="56"/>
-      <c r="Q40" s="56"/>
-      <c r="R40" s="56"/>
-      <c r="S40" s="56"/>
-      <c r="T40" s="56"/>
-      <c r="U40" s="56"/>
-      <c r="V40" s="56"/>
-      <c r="W40" s="56"/>
-      <c r="X40" s="56"/>
-      <c r="Y40" s="57"/>
+      <c r="A40" s="51" t="s">
+        <v>683</v>
+      </c>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="49"/>
+      <c r="U40" s="49"/>
+      <c r="V40" s="49"/>
+      <c r="W40" s="49"/>
+      <c r="X40" s="49"/>
+      <c r="Y40" s="50"/>
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="54" t="s">
-        <v>636</v>
-      </c>
-      <c r="B41" s="54"/>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="54"/>
-      <c r="I41" s="54"/>
-      <c r="J41" s="54"/>
-      <c r="K41" s="54"/>
-      <c r="L41" s="54"/>
-      <c r="M41" s="54"/>
-      <c r="N41" s="54"/>
-      <c r="O41" s="54"/>
-      <c r="P41" s="54"/>
-      <c r="Q41" s="54"/>
-      <c r="R41" s="54"/>
-      <c r="S41" s="54"/>
-      <c r="T41" s="54"/>
-      <c r="U41" s="54"/>
-      <c r="V41" s="54"/>
-      <c r="W41" s="54"/>
-      <c r="X41" s="54"/>
-      <c r="Y41" s="54"/>
+      <c r="A41" s="47" t="s">
+        <v>684</v>
+      </c>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="47"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="47"/>
+      <c r="P41" s="47"/>
+      <c r="Q41" s="47"/>
+      <c r="R41" s="47"/>
+      <c r="S41" s="47"/>
+      <c r="T41" s="47"/>
+      <c r="U41" s="47"/>
+      <c r="V41" s="47"/>
+      <c r="W41" s="47"/>
+      <c r="X41" s="47"/>
+      <c r="Y41" s="47"/>
     </row>
     <row r="42" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="55" t="s">
-        <v>637</v>
-      </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="56"/>
-      <c r="K42" s="56"/>
-      <c r="L42" s="56"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
-      <c r="O42" s="56"/>
-      <c r="P42" s="56"/>
-      <c r="Q42" s="56"/>
-      <c r="R42" s="56"/>
-      <c r="S42" s="56"/>
-      <c r="T42" s="56"/>
-      <c r="U42" s="56"/>
-      <c r="V42" s="56"/>
-      <c r="W42" s="56"/>
-      <c r="X42" s="56"/>
-      <c r="Y42" s="57"/>
+      <c r="A42" s="48" t="s">
+        <v>685</v>
+      </c>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="49"/>
+      <c r="U42" s="49"/>
+      <c r="V42" s="49"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="49"/>
+      <c r="Y42" s="50"/>
     </row>
     <row r="43" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="55" t="s">
-        <v>638</v>
-      </c>
-      <c r="B43" s="56"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="56"/>
-      <c r="J43" s="56"/>
-      <c r="K43" s="56"/>
-      <c r="L43" s="56"/>
-      <c r="M43" s="56"/>
-      <c r="N43" s="56"/>
-      <c r="O43" s="56"/>
-      <c r="P43" s="56"/>
-      <c r="Q43" s="56"/>
-      <c r="R43" s="56"/>
-      <c r="S43" s="56"/>
-      <c r="T43" s="56"/>
-      <c r="U43" s="56"/>
-      <c r="V43" s="56"/>
-      <c r="W43" s="56"/>
-      <c r="X43" s="56"/>
-      <c r="Y43" s="57"/>
+      <c r="A43" s="48" t="s">
+        <v>686</v>
+      </c>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49"/>
+      <c r="O43" s="49"/>
+      <c r="P43" s="49"/>
+      <c r="Q43" s="49"/>
+      <c r="R43" s="49"/>
+      <c r="S43" s="49"/>
+      <c r="T43" s="49"/>
+      <c r="U43" s="49"/>
+      <c r="V43" s="49"/>
+      <c r="W43" s="49"/>
+      <c r="X43" s="49"/>
+      <c r="Y43" s="50"/>
     </row>
     <row r="44" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="55" t="s">
-        <v>639</v>
-      </c>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
-      <c r="O44" s="56"/>
-      <c r="P44" s="56"/>
-      <c r="Q44" s="56"/>
-      <c r="R44" s="56"/>
-      <c r="S44" s="56"/>
-      <c r="T44" s="56"/>
-      <c r="U44" s="56"/>
-      <c r="V44" s="56"/>
-      <c r="W44" s="56"/>
-      <c r="X44" s="56"/>
-      <c r="Y44" s="57"/>
+      <c r="A44" s="48" t="s">
+        <v>687</v>
+      </c>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="49"/>
+      <c r="R44" s="49"/>
+      <c r="S44" s="49"/>
+      <c r="T44" s="49"/>
+      <c r="U44" s="49"/>
+      <c r="V44" s="49"/>
+      <c r="W44" s="49"/>
+      <c r="X44" s="49"/>
+      <c r="Y44" s="50"/>
     </row>
     <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="55"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="56"/>
-      <c r="P45" s="56"/>
-      <c r="Q45" s="56"/>
-      <c r="R45" s="56"/>
-      <c r="S45" s="56"/>
-      <c r="T45" s="56"/>
-      <c r="U45" s="56"/>
-      <c r="V45" s="56"/>
-      <c r="W45" s="56"/>
-      <c r="X45" s="56"/>
-      <c r="Y45" s="57"/>
+      <c r="A45" s="48"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
+      <c r="P45" s="49"/>
+      <c r="Q45" s="49"/>
+      <c r="R45" s="49"/>
+      <c r="S45" s="49"/>
+      <c r="T45" s="49"/>
+      <c r="U45" s="49"/>
+      <c r="V45" s="49"/>
+      <c r="W45" s="49"/>
+      <c r="X45" s="49"/>
+      <c r="Y45" s="50"/>
     </row>
     <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="55"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
-      <c r="O46" s="56"/>
-      <c r="P46" s="56"/>
-      <c r="Q46" s="56"/>
-      <c r="R46" s="56"/>
-      <c r="S46" s="56"/>
-      <c r="T46" s="56"/>
-      <c r="U46" s="56"/>
-      <c r="V46" s="56"/>
-      <c r="W46" s="56"/>
-      <c r="X46" s="56"/>
-      <c r="Y46" s="57"/>
+      <c r="A46" s="48"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+      <c r="L46" s="49"/>
+      <c r="M46" s="49"/>
+      <c r="N46" s="49"/>
+      <c r="O46" s="49"/>
+      <c r="P46" s="49"/>
+      <c r="Q46" s="49"/>
+      <c r="R46" s="49"/>
+      <c r="S46" s="49"/>
+      <c r="T46" s="49"/>
+      <c r="U46" s="49"/>
+      <c r="V46" s="49"/>
+      <c r="W46" s="49"/>
+      <c r="X46" s="49"/>
+      <c r="Y46" s="50"/>
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="54" t="s">
-        <v>640</v>
-      </c>
-      <c r="B47" s="54"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="54"/>
-      <c r="L47" s="54"/>
-      <c r="M47" s="54"/>
-      <c r="N47" s="54"/>
-      <c r="O47" s="54"/>
-      <c r="P47" s="54"/>
-      <c r="Q47" s="54"/>
-      <c r="R47" s="54"/>
-      <c r="S47" s="54"/>
-      <c r="T47" s="54"/>
-      <c r="U47" s="54"/>
-      <c r="V47" s="54"/>
-      <c r="W47" s="54"/>
-      <c r="X47" s="54"/>
-      <c r="Y47" s="54"/>
+      <c r="A47" s="47" t="s">
+        <v>688</v>
+      </c>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+      <c r="M47" s="47"/>
+      <c r="N47" s="47"/>
+      <c r="O47" s="47"/>
+      <c r="P47" s="47"/>
+      <c r="Q47" s="47"/>
+      <c r="R47" s="47"/>
+      <c r="S47" s="47"/>
+      <c r="T47" s="47"/>
+      <c r="U47" s="47"/>
+      <c r="V47" s="47"/>
+      <c r="W47" s="47"/>
+      <c r="X47" s="47"/>
+      <c r="Y47" s="47"/>
     </row>
     <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="55"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="56"/>
-      <c r="J48" s="56"/>
-      <c r="K48" s="56"/>
-      <c r="L48" s="56"/>
-      <c r="M48" s="56"/>
-      <c r="N48" s="56"/>
-      <c r="O48" s="56"/>
-      <c r="P48" s="56"/>
-      <c r="Q48" s="56"/>
-      <c r="R48" s="56"/>
-      <c r="S48" s="56"/>
-      <c r="T48" s="56"/>
-      <c r="U48" s="56"/>
-      <c r="V48" s="56"/>
-      <c r="W48" s="56"/>
-      <c r="X48" s="56"/>
-      <c r="Y48" s="57"/>
+      <c r="A48" s="48"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="49"/>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="49"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="49"/>
+      <c r="O48" s="49"/>
+      <c r="P48" s="49"/>
+      <c r="Q48" s="49"/>
+      <c r="R48" s="49"/>
+      <c r="S48" s="49"/>
+      <c r="T48" s="49"/>
+      <c r="U48" s="49"/>
+      <c r="V48" s="49"/>
+      <c r="W48" s="49"/>
+      <c r="X48" s="49"/>
+      <c r="Y48" s="50"/>
     </row>
     <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="55"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="56"/>
-      <c r="J49" s="56"/>
-      <c r="K49" s="56"/>
-      <c r="L49" s="56"/>
-      <c r="M49" s="56"/>
-      <c r="N49" s="56"/>
-      <c r="O49" s="56"/>
-      <c r="P49" s="56"/>
-      <c r="Q49" s="56"/>
-      <c r="R49" s="56"/>
-      <c r="S49" s="56"/>
-      <c r="T49" s="56"/>
-      <c r="U49" s="56"/>
-      <c r="V49" s="56"/>
-      <c r="W49" s="56"/>
-      <c r="X49" s="56"/>
-      <c r="Y49" s="57"/>
+      <c r="A49" s="48"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="49"/>
+      <c r="J49" s="49"/>
+      <c r="K49" s="49"/>
+      <c r="L49" s="49"/>
+      <c r="M49" s="49"/>
+      <c r="N49" s="49"/>
+      <c r="O49" s="49"/>
+      <c r="P49" s="49"/>
+      <c r="Q49" s="49"/>
+      <c r="R49" s="49"/>
+      <c r="S49" s="49"/>
+      <c r="T49" s="49"/>
+      <c r="U49" s="49"/>
+      <c r="V49" s="49"/>
+      <c r="W49" s="49"/>
+      <c r="X49" s="49"/>
+      <c r="Y49" s="50"/>
     </row>
     <row r="50" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="55" t="s">
-        <v>641</v>
-      </c>
-      <c r="B50" s="56"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="56"/>
-      <c r="I50" s="56"/>
-      <c r="J50" s="56"/>
-      <c r="K50" s="56"/>
-      <c r="L50" s="56"/>
-      <c r="M50" s="56"/>
-      <c r="N50" s="56"/>
-      <c r="O50" s="56"/>
-      <c r="P50" s="56"/>
-      <c r="Q50" s="56"/>
-      <c r="R50" s="56"/>
-      <c r="S50" s="56"/>
-      <c r="T50" s="56"/>
-      <c r="U50" s="56"/>
-      <c r="V50" s="56"/>
-      <c r="W50" s="56"/>
-      <c r="X50" s="56"/>
-      <c r="Y50" s="57"/>
+      <c r="A50" s="48" t="s">
+        <v>689</v>
+      </c>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="49"/>
+      <c r="N50" s="49"/>
+      <c r="O50" s="49"/>
+      <c r="P50" s="49"/>
+      <c r="Q50" s="49"/>
+      <c r="R50" s="49"/>
+      <c r="S50" s="49"/>
+      <c r="T50" s="49"/>
+      <c r="U50" s="49"/>
+      <c r="V50" s="49"/>
+      <c r="W50" s="49"/>
+      <c r="X50" s="49"/>
+      <c r="Y50" s="50"/>
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="54" t="s">
-        <v>642</v>
-      </c>
-      <c r="B51" s="54"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
-      <c r="H51" s="54"/>
-      <c r="I51" s="54"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="54"/>
-      <c r="L51" s="54"/>
-      <c r="M51" s="54"/>
-      <c r="N51" s="54"/>
-      <c r="O51" s="54"/>
-      <c r="P51" s="54"/>
-      <c r="Q51" s="54"/>
-      <c r="R51" s="54"/>
-      <c r="S51" s="54"/>
-      <c r="T51" s="54"/>
-      <c r="U51" s="54"/>
-      <c r="V51" s="54"/>
-      <c r="W51" s="54"/>
-      <c r="X51" s="54"/>
-      <c r="Y51" s="54"/>
+      <c r="A51" s="47" t="s">
+        <v>690</v>
+      </c>
+      <c r="B51" s="47"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="47"/>
+      <c r="I51" s="47"/>
+      <c r="J51" s="47"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="47"/>
+      <c r="M51" s="47"/>
+      <c r="N51" s="47"/>
+      <c r="O51" s="47"/>
+      <c r="P51" s="47"/>
+      <c r="Q51" s="47"/>
+      <c r="R51" s="47"/>
+      <c r="S51" s="47"/>
+      <c r="T51" s="47"/>
+      <c r="U51" s="47"/>
+      <c r="V51" s="47"/>
+      <c r="W51" s="47"/>
+      <c r="X51" s="47"/>
+      <c r="Y51" s="47"/>
     </row>
     <row r="52" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="59" t="s">
-        <v>643</v>
-      </c>
-      <c r="B52" s="56"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="56"/>
-      <c r="L52" s="56"/>
-      <c r="M52" s="56"/>
-      <c r="N52" s="56"/>
-      <c r="O52" s="56"/>
-      <c r="P52" s="56"/>
-      <c r="Q52" s="56"/>
-      <c r="R52" s="56"/>
-      <c r="S52" s="56"/>
-      <c r="T52" s="56"/>
-      <c r="U52" s="56"/>
-      <c r="V52" s="56"/>
-      <c r="W52" s="56"/>
-      <c r="X52" s="56"/>
-      <c r="Y52" s="57"/>
+      <c r="A52" s="52" t="s">
+        <v>691</v>
+      </c>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="49"/>
+      <c r="J52" s="49"/>
+      <c r="K52" s="49"/>
+      <c r="L52" s="49"/>
+      <c r="M52" s="49"/>
+      <c r="N52" s="49"/>
+      <c r="O52" s="49"/>
+      <c r="P52" s="49"/>
+      <c r="Q52" s="49"/>
+      <c r="R52" s="49"/>
+      <c r="S52" s="49"/>
+      <c r="T52" s="49"/>
+      <c r="U52" s="49"/>
+      <c r="V52" s="49"/>
+      <c r="W52" s="49"/>
+      <c r="X52" s="49"/>
+      <c r="Y52" s="50"/>
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="59" t="s">
-        <v>644</v>
-      </c>
-      <c r="B53" s="56"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
-      <c r="H53" s="56"/>
-      <c r="I53" s="56"/>
-      <c r="J53" s="56"/>
-      <c r="K53" s="56"/>
-      <c r="L53" s="56"/>
-      <c r="M53" s="56"/>
-      <c r="N53" s="56"/>
-      <c r="O53" s="56"/>
-      <c r="P53" s="56"/>
-      <c r="Q53" s="56"/>
-      <c r="R53" s="56"/>
-      <c r="S53" s="56"/>
-      <c r="T53" s="56"/>
-      <c r="U53" s="56"/>
-      <c r="V53" s="56"/>
-      <c r="W53" s="56"/>
-      <c r="X53" s="56"/>
-      <c r="Y53" s="57"/>
+      <c r="A53" s="52" t="s">
+        <v>692</v>
+      </c>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="49"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="49"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="49"/>
+      <c r="O53" s="49"/>
+      <c r="P53" s="49"/>
+      <c r="Q53" s="49"/>
+      <c r="R53" s="49"/>
+      <c r="S53" s="49"/>
+      <c r="T53" s="49"/>
+      <c r="U53" s="49"/>
+      <c r="V53" s="49"/>
+      <c r="W53" s="49"/>
+      <c r="X53" s="49"/>
+      <c r="Y53" s="50"/>
     </row>
     <row r="54" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="59" t="s">
-        <v>645</v>
-      </c>
-      <c r="B54" s="56"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="56"/>
-      <c r="I54" s="56"/>
-      <c r="J54" s="56"/>
-      <c r="K54" s="56"/>
-      <c r="L54" s="56"/>
-      <c r="M54" s="56"/>
-      <c r="N54" s="56"/>
-      <c r="O54" s="56"/>
-      <c r="P54" s="56"/>
-      <c r="Q54" s="56"/>
-      <c r="R54" s="56"/>
-      <c r="S54" s="56"/>
-      <c r="T54" s="56"/>
-      <c r="U54" s="56"/>
-      <c r="V54" s="56"/>
-      <c r="W54" s="56"/>
-      <c r="X54" s="56"/>
-      <c r="Y54" s="57"/>
+      <c r="A54" s="52" t="s">
+        <v>693</v>
+      </c>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="49"/>
+      <c r="L54" s="49"/>
+      <c r="M54" s="49"/>
+      <c r="N54" s="49"/>
+      <c r="O54" s="49"/>
+      <c r="P54" s="49"/>
+      <c r="Q54" s="49"/>
+      <c r="R54" s="49"/>
+      <c r="S54" s="49"/>
+      <c r="T54" s="49"/>
+      <c r="U54" s="49"/>
+      <c r="V54" s="49"/>
+      <c r="W54" s="49"/>
+      <c r="X54" s="49"/>
+      <c r="Y54" s="50"/>
     </row>
     <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="55"/>
-      <c r="B55" s="56"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="56"/>
-      <c r="I55" s="56"/>
-      <c r="J55" s="56"/>
-      <c r="K55" s="56"/>
-      <c r="L55" s="56"/>
-      <c r="M55" s="56"/>
-      <c r="N55" s="56"/>
-      <c r="O55" s="56"/>
-      <c r="P55" s="56"/>
-      <c r="Q55" s="56"/>
-      <c r="R55" s="56"/>
-      <c r="S55" s="56"/>
-      <c r="T55" s="56"/>
-      <c r="U55" s="56"/>
-      <c r="V55" s="56"/>
-      <c r="W55" s="56"/>
-      <c r="X55" s="56"/>
-      <c r="Y55" s="57"/>
+      <c r="A55" s="48"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="49"/>
+      <c r="L55" s="49"/>
+      <c r="M55" s="49"/>
+      <c r="N55" s="49"/>
+      <c r="O55" s="49"/>
+      <c r="P55" s="49"/>
+      <c r="Q55" s="49"/>
+      <c r="R55" s="49"/>
+      <c r="S55" s="49"/>
+      <c r="T55" s="49"/>
+      <c r="U55" s="49"/>
+      <c r="V55" s="49"/>
+      <c r="W55" s="49"/>
+      <c r="X55" s="49"/>
+      <c r="Y55" s="50"/>
     </row>
     <row r="56" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="60" t="s">
-        <v>646</v>
-      </c>
-      <c r="B56" s="56"/>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="56"/>
-      <c r="J56" s="56"/>
-      <c r="K56" s="56"/>
-      <c r="L56" s="56"/>
-      <c r="M56" s="56"/>
-      <c r="N56" s="56"/>
-      <c r="O56" s="56"/>
-      <c r="P56" s="56"/>
-      <c r="Q56" s="56"/>
-      <c r="R56" s="56"/>
-      <c r="S56" s="56"/>
-      <c r="T56" s="56"/>
-      <c r="U56" s="56"/>
-      <c r="V56" s="56"/>
-      <c r="W56" s="56"/>
-      <c r="X56" s="56"/>
-      <c r="Y56" s="57"/>
+      <c r="A56" s="53" t="s">
+        <v>694</v>
+      </c>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
+      <c r="L56" s="49"/>
+      <c r="M56" s="49"/>
+      <c r="N56" s="49"/>
+      <c r="O56" s="49"/>
+      <c r="P56" s="49"/>
+      <c r="Q56" s="49"/>
+      <c r="R56" s="49"/>
+      <c r="S56" s="49"/>
+      <c r="T56" s="49"/>
+      <c r="U56" s="49"/>
+      <c r="V56" s="49"/>
+      <c r="W56" s="49"/>
+      <c r="X56" s="49"/>
+      <c r="Y56" s="50"/>
     </row>
     <row r="57" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="61" t="s">
-        <v>647</v>
-      </c>
-      <c r="B57" s="62"/>
-      <c r="C57" s="62"/>
-      <c r="D57" s="62"/>
-      <c r="E57" s="62"/>
-      <c r="F57" s="62"/>
-      <c r="G57" s="62"/>
-      <c r="H57" s="62"/>
-      <c r="I57" s="62"/>
-      <c r="J57" s="62"/>
-      <c r="K57" s="62"/>
-      <c r="L57" s="62"/>
-      <c r="M57" s="62"/>
-      <c r="N57" s="62"/>
-      <c r="O57" s="62"/>
-      <c r="P57" s="62"/>
-      <c r="Q57" s="62"/>
-      <c r="R57" s="62"/>
-      <c r="S57" s="62"/>
-      <c r="T57" s="62"/>
-      <c r="U57" s="62"/>
-      <c r="V57" s="62"/>
-      <c r="W57" s="62"/>
-      <c r="X57" s="62"/>
-      <c r="Y57" s="63"/>
+      <c r="A57" s="54" t="s">
+        <v>695</v>
+      </c>
+      <c r="B57" s="55"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="55"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="55"/>
+      <c r="L57" s="55"/>
+      <c r="M57" s="55"/>
+      <c r="N57" s="55"/>
+      <c r="O57" s="55"/>
+      <c r="P57" s="55"/>
+      <c r="Q57" s="55"/>
+      <c r="R57" s="55"/>
+      <c r="S57" s="55"/>
+      <c r="T57" s="55"/>
+      <c r="U57" s="55"/>
+      <c r="V57" s="55"/>
+      <c r="W57" s="55"/>
+      <c r="X57" s="55"/>
+      <c r="Y57" s="56"/>
     </row>
     <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="64"/>
+      <c r="A58" s="57"/>
     </row>
     <row r="59" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="65" t="s">
-        <v>648</v>
+      <c r="A59" s="58" t="s">
+        <v>696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement aggregation indicator maker
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -3226,15 +3226,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>405000</xdr:colOff>
+      <xdr:colOff>432000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>885240</xdr:colOff>
+      <xdr:colOff>911880</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3247,8 +3247,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="405000" y="664920"/>
-          <a:ext cx="480240" cy="356400"/>
+          <a:off x="432000" y="655920"/>
+          <a:ext cx="479880" cy="356040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
Aggregation indicators loading implemented
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -3271,7 +3271,7 @@
   <dimension ref="A1:AD65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B41" activeCellId="1" sqref="A7 B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6212,7 +6212,7 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fix typo in template
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -177,7 +177,7 @@
     <t>{key: 'PREVIOUS_ACTIVE_LIST', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre d’adultes et d’enfants  chez qui on a initié la TARV au cours de la période de raportage (B)</t>
+    <t>Nombre d’adultes et d’enfants  chez qui on a initié la TARV au cours de la période de rapportage (B)</t>
   </si>
   <si>
     <t>{key: 'ARV_STARTED', gender: 0}</t>
@@ -258,7 +258,7 @@
     <t>{key: 'ARV_STARTED', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre d’adultes et d’enfants déjà sous TARV  reçus dans le centre en provenance d'un autre centre de traitement au cours dau cours de la période de raportage (C)</t>
+    <t>Nombre d’adultes et d’enfants déjà sous TARV  reçus dans le centre en provenance d'un autre centre de traitement au cours dau cours de la période de rapportage (C)</t>
   </si>
   <si>
     <t>{key: 'ARV_INCOMING_TRANSFER', gender: 0}</t>
@@ -339,7 +339,7 @@
     <t>{key: 'ARV_INCOMING_TRANSFER', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre d’adultes et d’enfants déjà sous TARV  mais perdus de vue dans le centre et qui ont repris le traitement au cours au cours de la période de raportage (D)</t>
+    <t>Nombre d’adultes et d’enfants déjà sous TARV  mais perdus de vue dans le centre et qui ont repris le traitement au cours au cours de la période de rapportage (D)</t>
   </si>
   <si>
     <t>{key: 'ARV_LOST_BACK', gender: 0}</t>
@@ -420,7 +420,7 @@
     <t>{key: 'ARV_LOST_BACK', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre d’adultes et d’enfants déjà sous TARV  et ayant arrêté le traitement mais qui ont repris au cours au cours de la période de raportage (E)</t>
+    <t>Nombre d’adultes et d’enfants déjà sous TARV  et ayant arrêté le traitement mais qui ont repris au cours au cours de la période de rapportage (E)</t>
   </si>
   <si>
     <t>{key: 'ARV_RESTARTED', gender: 0}</t>
@@ -582,7 +582,7 @@
     <t>{key: 'ARV_RECEIVED', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux perdus de vue au cours au cours de la période de raportage (G)</t>
+    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux perdus de vue au cours au cours de la période de rapportage (G)</t>
   </si>
   <si>
     <t>{key: 'ARV_LOST', gender: 0}</t>
@@ -663,7 +663,7 @@
     <t>{key: 'ARV_LOST', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux Décédés au cours au cours de la période de raportage (H)</t>
+    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux Décédés au cours au cours de la période de rapportage (H)</t>
   </si>
   <si>
     <t>{key: 'ARV_DEAD', gender: 0}</t>
@@ -744,7 +744,7 @@
     <t>{key: 'ARV_DEAD', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux Ayant arrêté le traitement au cours au cours de la période de raportage (I)</t>
+    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux Ayant arrêté le traitement au cours au cours de la période de rapportage (I)</t>
   </si>
   <si>
     <t>{key: 'ARV_STOPPED', gender: 0}</t>
@@ -825,7 +825,7 @@
     <t>{key: 'ARV_STOPPED', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux transférés au cours au cours de la période de raportage (J)</t>
+    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux transférés au cours au cours de la période de rapportage (J)</t>
   </si>
   <si>
     <t>{key: 'ARV_TRANSFERRED', gender: 0}</t>
@@ -987,7 +987,7 @@
     <t>{key: 'ACTIVE_LIST', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre de personnes infectées par le VIH, qui répondent aux critères d’éligibilité à la prophylaxie au cotrimoxazole au cours au cours de la période de raportage</t>
+    <t>Nombre de personnes infectées par le VIH, qui répondent aux critères d’éligibilité à la prophylaxie au cotrimoxazole au cours au cours de la période de rapportage</t>
   </si>
   <si>
     <t>{key: 'CTX_ELIGIBLE', gender: 0}</t>
@@ -1068,7 +1068,7 @@
     <t>{key: 'CTX_ELIGIBLE', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre de personnes  VIH, qui reçoivent  du cotrimoxazole au cours au cours de la période de raportage</t>
+    <t>Nombre de personnes  VIH, qui reçoivent  du cotrimoxazole au cours au cours de la période de rapportage</t>
   </si>
   <si>
     <t>{key: 'UNDER_CTX', gender: 0}</t>
@@ -3206,15 +3206,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>486000</xdr:colOff>
+      <xdr:colOff>513000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>965160</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:colOff>991800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>183960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3227,8 +3227,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="486000" y="637920"/>
-          <a:ext cx="479160" cy="355320"/>
+          <a:off x="513000" y="628920"/>
+          <a:ext cx="478800" cy="354960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3251,7 +3251,7 @@
   <dimension ref="A1:AD65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6192,7 +6192,7 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fix default report template and ctx eligible indicator
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="89" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="79" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="File active" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="829">
   <si>
     <t>Région</t>
   </si>
@@ -258,7 +258,7 @@
     <t>{key: 'ARV_STARTED', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre d’adultes et d’enfants déjà sous TARV  reçus dans le centre en provenance d'un autre centre de traitement au cours dau cours de la période de rapportage (C)</t>
+    <t>Nombre d’adultes et d’enfants déjà sous TARV  reçus dans le centre en provenance d'un autre centre de traitement au cours de la période de rapportage (C)</t>
   </si>
   <si>
     <t>{key: 'ARV_INCOMING_TRANSFER', gender: 0}</t>
@@ -339,9 +339,6 @@
     <t>{key: 'ARV_INCOMING_TRANSFER', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre d’adultes et d’enfants déjà sous TARV  mais perdus de vue dans le centre et qui ont repris le traitement au cours au cours de la période de rapportage (D)</t>
-  </si>
-  <si>
     <t>{key: 'ARV_LOST_BACK', gender: 0}</t>
   </si>
   <si>
@@ -420,7 +417,7 @@
     <t>{key: 'ARV_LOST_BACK', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre d’adultes et d’enfants déjà sous TARV  et ayant arrêté le traitement mais qui ont repris au cours au cours de la période de rapportage (E)</t>
+    <t>Nombre d’adultes et d’enfants déjà sous TARV  et ayant arrêté le traitement mais qui ont repris au cours de la période de rapportage (E)</t>
   </si>
   <si>
     <t>{key: 'ARV_RESTARTED', gender: 0}</t>
@@ -582,7 +579,7 @@
     <t>{key: 'ARV_RECEIVED', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux perdus de vue au cours au cours de la période de rapportage (G)</t>
+    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux perdus de vue au cours de la période de rapportage (G)</t>
   </si>
   <si>
     <t>{key: 'ARV_LOST', gender: 0}</t>
@@ -663,7 +660,7 @@
     <t>{key: 'ARV_LOST', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux Décédés au cours au cours de la période de rapportage (H)</t>
+    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux Décédés au cours de la période de rapportage (H)</t>
   </si>
   <si>
     <t>{key: 'ARV_DEAD', gender: 0}</t>
@@ -744,7 +741,7 @@
     <t>{key: 'ARV_DEAD', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux Ayant arrêté le traitement au cours au cours de la période de rapportage (I)</t>
+    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux Ayant arrêté le traitement au cours de la période de rapportage (I)</t>
   </si>
   <si>
     <t>{key: 'ARV_STOPPED', gender: 0}</t>
@@ -825,7 +822,7 @@
     <t>{key: 'ARV_STOPPED', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux transférés au cours au cours de la période de rapportage (J)</t>
+    <t>Nombre Total d’adultes et d’enfants sous antirétroviraux transférés au cours de la période de rapportage (J)</t>
   </si>
   <si>
     <t>{key: 'ARV_TRANSFERRED', gender: 0}</t>
@@ -987,7 +984,7 @@
     <t>{key: 'ACTIVE_LIST', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre de personnes infectées par le VIH, qui répondent aux critères d’éligibilité à la prophylaxie au cotrimoxazole au cours au cours de la période de rapportage</t>
+    <t>Nombre de personnes infectées par le VIH, qui répondent aux critères d’éligibilité à la prophylaxie au cotrimoxazole de la période de rapportage et ne sont pas sous TARV</t>
   </si>
   <si>
     <t>{key: 'CTX_ELIGIBLE', gender: 0}</t>
@@ -1068,7 +1065,7 @@
     <t>{key: 'CTX_ELIGIBLE', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre de personnes  VIH, qui reçoivent  du cotrimoxazole au cours au cours de la période de rapportage</t>
+    <t>Nombre de personnes  VIH, qui reçoivent  du cotrimoxazole au cours de la période de rapportage</t>
   </si>
   <si>
     <t>{key: 'UNDER_CTX', gender: 0}</t>
@@ -3206,15 +3203,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>513000</xdr:colOff>
+      <xdr:colOff>567000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>991800</xdr:colOff>
+      <xdr:colOff>1045080</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>183960</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3227,8 +3224,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="513000" y="628920"/>
-          <a:ext cx="478800" cy="354960"/>
+          <a:off x="567000" y="610920"/>
+          <a:ext cx="478080" cy="354240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3250,13 +3247,13 @@
   </sheetPr>
   <dimension ref="A1:AD65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A:A"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.3036437246964"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.0728744939271"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.2834008097166"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.417004048583"/>
@@ -3814,1571 +3811,1571 @@
     </row>
     <row r="14" s="19" customFormat="true" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="C14" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="F14" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="G14" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="H14" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="I14" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="K14" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="L14" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="M14" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="M14" s="16" t="s">
+      <c r="N14" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="N14" s="16" t="s">
+      <c r="O14" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="O14" s="16" t="s">
+      <c r="P14" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q14" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="P14" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q14" s="16" t="s">
+      <c r="R14" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="R14" s="16" t="s">
+      <c r="S14" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="S14" s="16" t="s">
+      <c r="T14" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T14" s="16" t="s">
+      <c r="U14" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="U14" s="16" t="s">
+      <c r="V14" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="V14" s="16" t="s">
+      <c r="W14" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="W14" s="16" t="s">
+      <c r="X14" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="X14" s="16" t="s">
+      <c r="Y14" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="Y14" s="16" t="s">
+      <c r="Z14" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="Z14" s="16" t="s">
+      <c r="AA14" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="AA14" s="16" t="s">
+      <c r="AB14" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="AB14" s="16" t="s">
-        <v>133</v>
-      </c>
       <c r="AC14" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD14" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="AD14" s="17" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="C15" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="E15" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="F15" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="G15" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="H15" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="I15" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="J15" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="K15" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="L15" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="M15" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="M15" s="16" t="s">
+      <c r="N15" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="N15" s="16" t="s">
+      <c r="O15" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="O15" s="16" t="s">
+      <c r="P15" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q15" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="P15" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q15" s="16" t="s">
+      <c r="R15" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="R15" s="16" t="s">
+      <c r="S15" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="S15" s="16" t="s">
+      <c r="T15" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="T15" s="16" t="s">
+      <c r="U15" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="U15" s="16" t="s">
+      <c r="V15" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="V15" s="16" t="s">
+      <c r="W15" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="W15" s="16" t="s">
+      <c r="X15" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="X15" s="16" t="s">
+      <c r="Y15" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="Y15" s="16" t="s">
+      <c r="Z15" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="Z15" s="16" t="s">
+      <c r="AA15" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="AA15" s="16" t="s">
+      <c r="AB15" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="AB15" s="16" t="s">
-        <v>160</v>
-      </c>
       <c r="AC15" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD15" s="17" t="s">
         <v>135</v>
-      </c>
-      <c r="AD15" s="17" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="C16" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="D16" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="F16" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="G16" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="H16" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="I16" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="J16" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="K16" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="L16" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="L16" s="23" t="s">
+      <c r="M16" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="N16" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="N16" s="21" t="s">
+      <c r="O16" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="O16" s="21" t="s">
+      <c r="P16" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q16" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="P16" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q16" s="21" t="s">
+      <c r="R16" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="R16" s="21" t="s">
+      <c r="S16" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="S16" s="21" t="s">
+      <c r="T16" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="T16" s="21" t="s">
+      <c r="U16" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="U16" s="21" t="s">
+      <c r="V16" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="V16" s="21" t="s">
+      <c r="W16" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="W16" s="21" t="s">
+      <c r="X16" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="X16" s="21" t="s">
+      <c r="Y16" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="Y16" s="21" t="s">
+      <c r="Z16" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="Z16" s="21" t="s">
+      <c r="AA16" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="AA16" s="21" t="s">
+      <c r="AB16" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="AB16" s="21" t="s">
-        <v>187</v>
-      </c>
       <c r="AC16" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD16" s="24" t="s">
         <v>162</v>
-      </c>
-      <c r="AD16" s="24" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="C17" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="E17" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="F17" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="G17" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="H17" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="I17" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="J17" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="K17" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="L17" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="M17" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="N17" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="N17" s="16" t="s">
+      <c r="O17" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="O17" s="16" t="s">
+      <c r="P17" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q17" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="P17" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q17" s="16" t="s">
+      <c r="R17" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="R17" s="16" t="s">
+      <c r="S17" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="S17" s="16" t="s">
+      <c r="T17" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="T17" s="16" t="s">
+      <c r="U17" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="U17" s="16" t="s">
+      <c r="V17" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="V17" s="16" t="s">
+      <c r="W17" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="W17" s="16" t="s">
+      <c r="X17" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="X17" s="16" t="s">
+      <c r="Y17" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="Y17" s="16" t="s">
+      <c r="Z17" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="Z17" s="16" t="s">
+      <c r="AA17" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="AA17" s="16" t="s">
+      <c r="AB17" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="AB17" s="16" t="s">
-        <v>214</v>
-      </c>
       <c r="AC17" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD17" s="17" t="s">
         <v>189</v>
-      </c>
-      <c r="AD17" s="17" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="C18" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="E18" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="F18" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="G18" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="H18" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="I18" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="J18" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="K18" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="L18" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="M18" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="M18" s="16" t="s">
+      <c r="N18" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="N18" s="16" t="s">
+      <c r="O18" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="O18" s="16" t="s">
+      <c r="P18" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q18" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="P18" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q18" s="16" t="s">
+      <c r="R18" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="R18" s="16" t="s">
+      <c r="S18" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="S18" s="16" t="s">
+      <c r="T18" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="T18" s="16" t="s">
+      <c r="U18" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="U18" s="16" t="s">
+      <c r="V18" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="V18" s="16" t="s">
+      <c r="W18" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="W18" s="16" t="s">
+      <c r="X18" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="X18" s="16" t="s">
+      <c r="Y18" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="Y18" s="16" t="s">
+      <c r="Z18" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="Z18" s="16" t="s">
+      <c r="AA18" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="AA18" s="16" t="s">
+      <c r="AB18" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="AB18" s="16" t="s">
-        <v>241</v>
-      </c>
       <c r="AC18" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD18" s="17" t="s">
         <v>216</v>
-      </c>
-      <c r="AD18" s="17" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="C19" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="E19" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="F19" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="G19" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="H19" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="I19" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="J19" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="K19" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="L19" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="M19" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="N19" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="N19" s="16" t="s">
+      <c r="O19" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="O19" s="16" t="s">
+      <c r="P19" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q19" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="P19" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q19" s="16" t="s">
+      <c r="R19" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="R19" s="16" t="s">
+      <c r="S19" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="S19" s="16" t="s">
+      <c r="T19" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="T19" s="16" t="s">
+      <c r="U19" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="U19" s="16" t="s">
+      <c r="V19" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="V19" s="16" t="s">
+      <c r="W19" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="W19" s="16" t="s">
+      <c r="X19" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="X19" s="16" t="s">
+      <c r="Y19" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="Y19" s="16" t="s">
+      <c r="Z19" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="Z19" s="16" t="s">
+      <c r="AA19" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="AA19" s="16" t="s">
+      <c r="AB19" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="AB19" s="16" t="s">
-        <v>268</v>
-      </c>
       <c r="AC19" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="AD19" s="17" t="s">
         <v>243</v>
-      </c>
-      <c r="AD19" s="17" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="D20" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="E20" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="F20" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="G20" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="H20" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="I20" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="J20" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="K20" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="L20" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="M20" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="M20" s="16" t="s">
+      <c r="N20" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="N20" s="16" t="s">
+      <c r="O20" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="O20" s="16" t="s">
+      <c r="P20" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q20" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="P20" s="16" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q20" s="16" t="s">
+      <c r="R20" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="R20" s="16" t="s">
+      <c r="S20" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="S20" s="16" t="s">
+      <c r="T20" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="T20" s="16" t="s">
+      <c r="U20" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="U20" s="16" t="s">
+      <c r="V20" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="V20" s="16" t="s">
+      <c r="W20" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="W20" s="16" t="s">
+      <c r="X20" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="X20" s="16" t="s">
+      <c r="Y20" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="Y20" s="16" t="s">
+      <c r="Z20" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="Z20" s="16" t="s">
+      <c r="AA20" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="AA20" s="16" t="s">
+      <c r="AB20" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="AB20" s="16" t="s">
-        <v>295</v>
-      </c>
       <c r="AC20" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="AD20" s="17" t="s">
         <v>270</v>
-      </c>
-      <c r="AD20" s="17" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="C21" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="D21" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="E21" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="F21" s="26" t="s">
         <v>300</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="G21" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="H21" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="I21" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="I21" s="23" t="s">
+      <c r="J21" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="K21" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="K21" s="23" t="s">
+      <c r="L21" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="L21" s="23" t="s">
+      <c r="M21" s="27" t="s">
         <v>307</v>
       </c>
-      <c r="M21" s="27" t="s">
+      <c r="N21" s="27" t="s">
         <v>308</v>
       </c>
-      <c r="N21" s="27" t="s">
+      <c r="O21" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="O21" s="27" t="s">
+      <c r="P21" s="27" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q21" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="P21" s="27" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q21" s="27" t="s">
+      <c r="R21" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="R21" s="27" t="s">
+      <c r="S21" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="S21" s="27" t="s">
+      <c r="T21" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="T21" s="27" t="s">
+      <c r="U21" s="27" t="s">
         <v>314</v>
       </c>
-      <c r="U21" s="27" t="s">
+      <c r="V21" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="V21" s="27" t="s">
+      <c r="W21" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="W21" s="27" t="s">
+      <c r="X21" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="X21" s="27" t="s">
+      <c r="Y21" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="Y21" s="27" t="s">
+      <c r="Z21" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="Z21" s="27" t="s">
+      <c r="AA21" s="27" t="s">
         <v>320</v>
       </c>
-      <c r="AA21" s="27" t="s">
+      <c r="AB21" s="27" t="s">
         <v>321</v>
       </c>
-      <c r="AB21" s="27" t="s">
-        <v>322</v>
-      </c>
       <c r="AC21" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="AD21" s="28" t="s">
         <v>297</v>
-      </c>
-      <c r="AD21" s="28" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="C22" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="D22" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="E22" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="F22" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="G22" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="H22" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="I22" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="J22" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="K22" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="K22" s="15" t="s">
+      <c r="L22" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="L22" s="15" t="s">
+      <c r="M22" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="M22" s="16" t="s">
+      <c r="N22" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="N22" s="16" t="s">
+      <c r="O22" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="O22" s="16" t="s">
+      <c r="P22" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q22" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="P22" s="16" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q22" s="16" t="s">
+      <c r="R22" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="R22" s="16" t="s">
+      <c r="S22" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="S22" s="16" t="s">
+      <c r="T22" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="T22" s="16" t="s">
+      <c r="U22" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="U22" s="16" t="s">
+      <c r="V22" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="V22" s="16" t="s">
+      <c r="W22" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="W22" s="16" t="s">
+      <c r="X22" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="X22" s="16" t="s">
+      <c r="Y22" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="Y22" s="16" t="s">
+      <c r="Z22" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="Z22" s="16" t="s">
+      <c r="AA22" s="16" t="s">
         <v>347</v>
       </c>
-      <c r="AA22" s="16" t="s">
+      <c r="AB22" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="AB22" s="16" t="s">
-        <v>349</v>
-      </c>
       <c r="AC22" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="AD22" s="17" t="s">
         <v>324</v>
-      </c>
-      <c r="AD22" s="17" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="C23" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="D23" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="E23" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="F23" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="G23" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="H23" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="I23" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="J23" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="K23" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="L23" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="L23" s="15" t="s">
+      <c r="M23" s="16" t="s">
         <v>361</v>
       </c>
-      <c r="M23" s="16" t="s">
+      <c r="N23" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="N23" s="16" t="s">
+      <c r="O23" s="16" t="s">
         <v>363</v>
       </c>
-      <c r="O23" s="16" t="s">
+      <c r="P23" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q23" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="P23" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="Q23" s="16" t="s">
+      <c r="R23" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="R23" s="16" t="s">
+      <c r="S23" s="16" t="s">
         <v>366</v>
       </c>
-      <c r="S23" s="16" t="s">
+      <c r="T23" s="16" t="s">
         <v>367</v>
       </c>
-      <c r="T23" s="16" t="s">
+      <c r="U23" s="16" t="s">
         <v>368</v>
       </c>
-      <c r="U23" s="16" t="s">
+      <c r="V23" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="V23" s="16" t="s">
+      <c r="W23" s="16" t="s">
         <v>370</v>
       </c>
-      <c r="W23" s="16" t="s">
+      <c r="X23" s="16" t="s">
         <v>371</v>
       </c>
-      <c r="X23" s="16" t="s">
+      <c r="Y23" s="16" t="s">
         <v>372</v>
       </c>
-      <c r="Y23" s="16" t="s">
+      <c r="Z23" s="16" t="s">
         <v>373</v>
       </c>
-      <c r="Z23" s="16" t="s">
+      <c r="AA23" s="16" t="s">
         <v>374</v>
       </c>
-      <c r="AA23" s="16" t="s">
+      <c r="AB23" s="16" t="s">
         <v>375</v>
       </c>
-      <c r="AB23" s="16" t="s">
-        <v>376</v>
-      </c>
       <c r="AC23" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="AD23" s="17" t="s">
         <v>351</v>
-      </c>
-      <c r="AD23" s="17" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="24" s="19" customFormat="true" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="B24" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="C24" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="D24" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="E24" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="F24" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="G24" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="H24" s="15" t="s">
         <v>383</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="I24" s="15" t="s">
         <v>384</v>
       </c>
-      <c r="I24" s="15" t="s">
+      <c r="J24" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="J24" s="15" t="s">
+      <c r="K24" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="K24" s="15" t="s">
+      <c r="L24" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="L24" s="15" t="s">
+      <c r="M24" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="M24" s="16" t="s">
+      <c r="N24" s="16" t="s">
         <v>389</v>
       </c>
-      <c r="N24" s="16" t="s">
+      <c r="O24" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="O24" s="16" t="s">
+      <c r="P24" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q24" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="P24" s="16" t="s">
-        <v>389</v>
-      </c>
-      <c r="Q24" s="16" t="s">
+      <c r="R24" s="16" t="s">
         <v>392</v>
       </c>
-      <c r="R24" s="16" t="s">
+      <c r="S24" s="16" t="s">
         <v>393</v>
       </c>
-      <c r="S24" s="16" t="s">
+      <c r="T24" s="16" t="s">
         <v>394</v>
       </c>
-      <c r="T24" s="16" t="s">
+      <c r="U24" s="16" t="s">
         <v>395</v>
       </c>
-      <c r="U24" s="16" t="s">
+      <c r="V24" s="16" t="s">
         <v>396</v>
       </c>
-      <c r="V24" s="16" t="s">
+      <c r="W24" s="16" t="s">
         <v>397</v>
       </c>
-      <c r="W24" s="16" t="s">
+      <c r="X24" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="X24" s="16" t="s">
+      <c r="Y24" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="Y24" s="16" t="s">
+      <c r="Z24" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="Z24" s="16" t="s">
+      <c r="AA24" s="16" t="s">
         <v>401</v>
       </c>
-      <c r="AA24" s="16" t="s">
+      <c r="AB24" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="AB24" s="16" t="s">
-        <v>403</v>
-      </c>
       <c r="AC24" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="AD24" s="17" t="s">
         <v>378</v>
-      </c>
-      <c r="AD24" s="17" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="25" s="19" customFormat="true" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="C25" s="15" t="s">
         <v>405</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="D25" s="15" t="s">
         <v>406</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="E25" s="15" t="s">
         <v>407</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>408</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="G25" s="15" t="s">
         <v>409</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="H25" s="15" t="s">
         <v>410</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="I25" s="15" t="s">
         <v>411</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="J25" s="15" t="s">
         <v>412</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="K25" s="15" t="s">
         <v>413</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="L25" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="L25" s="15" t="s">
+      <c r="M25" s="16" t="s">
         <v>415</v>
       </c>
-      <c r="M25" s="16" t="s">
+      <c r="N25" s="16" t="s">
         <v>416</v>
       </c>
-      <c r="N25" s="16" t="s">
+      <c r="O25" s="16" t="s">
         <v>417</v>
       </c>
-      <c r="O25" s="16" t="s">
+      <c r="P25" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q25" s="16" t="s">
         <v>418</v>
       </c>
-      <c r="P25" s="16" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q25" s="16" t="s">
+      <c r="R25" s="16" t="s">
         <v>419</v>
       </c>
-      <c r="R25" s="16" t="s">
+      <c r="S25" s="16" t="s">
         <v>420</v>
       </c>
-      <c r="S25" s="16" t="s">
+      <c r="T25" s="16" t="s">
         <v>421</v>
       </c>
-      <c r="T25" s="16" t="s">
+      <c r="U25" s="16" t="s">
         <v>422</v>
       </c>
-      <c r="U25" s="16" t="s">
+      <c r="V25" s="16" t="s">
         <v>423</v>
       </c>
-      <c r="V25" s="16" t="s">
+      <c r="W25" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="W25" s="16" t="s">
+      <c r="X25" s="16" t="s">
         <v>425</v>
       </c>
-      <c r="X25" s="16" t="s">
+      <c r="Y25" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="Y25" s="16" t="s">
+      <c r="Z25" s="16" t="s">
         <v>427</v>
       </c>
-      <c r="Z25" s="16" t="s">
+      <c r="AA25" s="16" t="s">
         <v>428</v>
       </c>
-      <c r="AA25" s="16" t="s">
+      <c r="AB25" s="16" t="s">
         <v>429</v>
       </c>
-      <c r="AB25" s="16" t="s">
-        <v>430</v>
-      </c>
       <c r="AC25" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="AD25" s="17" t="s">
         <v>405</v>
-      </c>
-      <c r="AD25" s="17" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="26" s="19" customFormat="true" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>431</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="C26" s="15" t="s">
         <v>432</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="D26" s="15" t="s">
         <v>433</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="E26" s="15" t="s">
         <v>434</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="F26" s="15" t="s">
         <v>435</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="G26" s="15" t="s">
         <v>436</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="H26" s="15" t="s">
         <v>437</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="I26" s="15" t="s">
         <v>438</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="J26" s="15" t="s">
         <v>439</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="K26" s="15" t="s">
         <v>440</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="L26" s="15" t="s">
         <v>441</v>
       </c>
-      <c r="L26" s="15" t="s">
+      <c r="M26" s="16" t="s">
         <v>442</v>
       </c>
-      <c r="M26" s="16" t="s">
+      <c r="N26" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="N26" s="16" t="s">
+      <c r="O26" s="16" t="s">
         <v>444</v>
       </c>
-      <c r="O26" s="16" t="s">
+      <c r="P26" s="16" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q26" s="16" t="s">
         <v>445</v>
       </c>
-      <c r="P26" s="16" t="s">
-        <v>443</v>
-      </c>
-      <c r="Q26" s="16" t="s">
+      <c r="R26" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="R26" s="16" t="s">
+      <c r="S26" s="16" t="s">
         <v>447</v>
       </c>
-      <c r="S26" s="16" t="s">
+      <c r="T26" s="16" t="s">
         <v>448</v>
       </c>
-      <c r="T26" s="16" t="s">
+      <c r="U26" s="16" t="s">
         <v>449</v>
       </c>
-      <c r="U26" s="16" t="s">
+      <c r="V26" s="16" t="s">
         <v>450</v>
       </c>
-      <c r="V26" s="16" t="s">
+      <c r="W26" s="16" t="s">
         <v>451</v>
       </c>
-      <c r="W26" s="16" t="s">
+      <c r="X26" s="16" t="s">
         <v>452</v>
       </c>
-      <c r="X26" s="16" t="s">
+      <c r="Y26" s="16" t="s">
         <v>453</v>
       </c>
-      <c r="Y26" s="16" t="s">
+      <c r="Z26" s="16" t="s">
         <v>454</v>
       </c>
-      <c r="Z26" s="16" t="s">
+      <c r="AA26" s="16" t="s">
         <v>455</v>
       </c>
-      <c r="AA26" s="16" t="s">
+      <c r="AB26" s="16" t="s">
         <v>456</v>
       </c>
-      <c r="AB26" s="16" t="s">
-        <v>457</v>
-      </c>
       <c r="AC26" s="16" t="s">
+        <v>431</v>
+      </c>
+      <c r="AD26" s="17" t="s">
         <v>432</v>
-      </c>
-      <c r="AD26" s="17" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="27" s="19" customFormat="true" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>458</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="C27" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="15" t="s">
         <v>460</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="E27" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="F27" s="15" t="s">
         <v>462</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="G27" s="15" t="s">
         <v>463</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="H27" s="15" t="s">
         <v>464</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="I27" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="J27" s="15" t="s">
         <v>466</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="K27" s="15" t="s">
         <v>467</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="L27" s="15" t="s">
         <v>468</v>
       </c>
-      <c r="L27" s="15" t="s">
+      <c r="M27" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="M27" s="16" t="s">
+      <c r="N27" s="16" t="s">
         <v>470</v>
       </c>
-      <c r="N27" s="16" t="s">
+      <c r="O27" s="16" t="s">
         <v>471</v>
       </c>
-      <c r="O27" s="16" t="s">
+      <c r="P27" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q27" s="16" t="s">
         <v>472</v>
       </c>
-      <c r="P27" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="Q27" s="16" t="s">
+      <c r="R27" s="16" t="s">
         <v>473</v>
       </c>
-      <c r="R27" s="16" t="s">
+      <c r="S27" s="16" t="s">
         <v>474</v>
       </c>
-      <c r="S27" s="16" t="s">
+      <c r="T27" s="16" t="s">
         <v>475</v>
       </c>
-      <c r="T27" s="16" t="s">
+      <c r="U27" s="16" t="s">
         <v>476</v>
       </c>
-      <c r="U27" s="16" t="s">
+      <c r="V27" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="V27" s="16" t="s">
+      <c r="W27" s="16" t="s">
         <v>478</v>
       </c>
-      <c r="W27" s="16" t="s">
+      <c r="X27" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="X27" s="16" t="s">
+      <c r="Y27" s="16" t="s">
         <v>480</v>
       </c>
-      <c r="Y27" s="16" t="s">
+      <c r="Z27" s="16" t="s">
         <v>481</v>
       </c>
-      <c r="Z27" s="16" t="s">
+      <c r="AA27" s="16" t="s">
         <v>482</v>
       </c>
-      <c r="AA27" s="16" t="s">
+      <c r="AB27" s="16" t="s">
         <v>483</v>
       </c>
-      <c r="AB27" s="16" t="s">
-        <v>484</v>
-      </c>
       <c r="AC27" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="AD27" s="17" t="s">
         <v>459</v>
-      </c>
-      <c r="AD27" s="17" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="63.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>485</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="C28" s="15" t="s">
         <v>486</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="D28" s="15" t="s">
         <v>487</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="E28" s="15" t="s">
         <v>488</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="F28" s="15" t="s">
         <v>489</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="G28" s="15" t="s">
         <v>490</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="H28" s="15" t="s">
         <v>491</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="I28" s="15" t="s">
         <v>492</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="J28" s="15" t="s">
         <v>493</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="K28" s="15" t="s">
         <v>494</v>
       </c>
-      <c r="K28" s="15" t="s">
+      <c r="L28" s="15" t="s">
         <v>495</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="M28" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="M28" s="16" t="s">
+      <c r="N28" s="16" t="s">
         <v>497</v>
       </c>
-      <c r="N28" s="16" t="s">
+      <c r="O28" s="16" t="s">
         <v>498</v>
       </c>
-      <c r="O28" s="16" t="s">
+      <c r="P28" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q28" s="16" t="s">
         <v>499</v>
       </c>
-      <c r="P28" s="16" t="s">
-        <v>497</v>
-      </c>
-      <c r="Q28" s="16" t="s">
+      <c r="R28" s="16" t="s">
         <v>500</v>
       </c>
-      <c r="R28" s="16" t="s">
+      <c r="S28" s="16" t="s">
         <v>501</v>
       </c>
-      <c r="S28" s="16" t="s">
+      <c r="T28" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="T28" s="16" t="s">
+      <c r="U28" s="16" t="s">
         <v>503</v>
       </c>
-      <c r="U28" s="16" t="s">
+      <c r="V28" s="16" t="s">
         <v>504</v>
       </c>
-      <c r="V28" s="16" t="s">
+      <c r="W28" s="16" t="s">
         <v>505</v>
       </c>
-      <c r="W28" s="16" t="s">
+      <c r="X28" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="X28" s="16" t="s">
+      <c r="Y28" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="Y28" s="16" t="s">
+      <c r="Z28" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="Z28" s="16" t="s">
+      <c r="AA28" s="16" t="s">
         <v>509</v>
       </c>
-      <c r="AA28" s="16" t="s">
+      <c r="AB28" s="16" t="s">
         <v>510</v>
       </c>
-      <c r="AB28" s="16" t="s">
-        <v>511</v>
-      </c>
       <c r="AC28" s="16" t="s">
+        <v>485</v>
+      </c>
+      <c r="AD28" s="17" t="s">
         <v>486</v>
-      </c>
-      <c r="AD28" s="17" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="58.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
+        <v>511</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>512</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="C29" s="15" t="s">
         <v>513</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="D29" s="15" t="s">
         <v>514</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="E29" s="15" t="s">
         <v>515</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="F29" s="15" t="s">
         <v>516</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="G29" s="15" t="s">
         <v>517</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="H29" s="15" t="s">
         <v>518</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="I29" s="15" t="s">
         <v>519</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="J29" s="15" t="s">
         <v>520</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="K29" s="15" t="s">
         <v>521</v>
       </c>
-      <c r="K29" s="15" t="s">
+      <c r="L29" s="15" t="s">
         <v>522</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="M29" s="16" t="s">
         <v>523</v>
       </c>
-      <c r="M29" s="16" t="s">
+      <c r="N29" s="16" t="s">
         <v>524</v>
       </c>
-      <c r="N29" s="16" t="s">
+      <c r="O29" s="16" t="s">
         <v>525</v>
       </c>
-      <c r="O29" s="16" t="s">
+      <c r="P29" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="Q29" s="16" t="s">
         <v>526</v>
       </c>
-      <c r="P29" s="16" t="s">
-        <v>524</v>
-      </c>
-      <c r="Q29" s="16" t="s">
+      <c r="R29" s="16" t="s">
         <v>527</v>
       </c>
-      <c r="R29" s="16" t="s">
+      <c r="S29" s="16" t="s">
         <v>528</v>
       </c>
-      <c r="S29" s="16" t="s">
+      <c r="T29" s="16" t="s">
         <v>529</v>
       </c>
-      <c r="T29" s="16" t="s">
+      <c r="U29" s="16" t="s">
         <v>530</v>
       </c>
-      <c r="U29" s="16" t="s">
+      <c r="V29" s="16" t="s">
         <v>531</v>
       </c>
-      <c r="V29" s="16" t="s">
+      <c r="W29" s="16" t="s">
         <v>532</v>
       </c>
-      <c r="W29" s="16" t="s">
+      <c r="X29" s="16" t="s">
         <v>533</v>
       </c>
-      <c r="X29" s="16" t="s">
+      <c r="Y29" s="16" t="s">
         <v>534</v>
       </c>
-      <c r="Y29" s="16" t="s">
+      <c r="Z29" s="16" t="s">
         <v>535</v>
       </c>
-      <c r="Z29" s="16" t="s">
+      <c r="AA29" s="16" t="s">
         <v>536</v>
       </c>
-      <c r="AA29" s="16" t="s">
+      <c r="AB29" s="16" t="s">
         <v>537</v>
       </c>
-      <c r="AB29" s="16" t="s">
-        <v>538</v>
-      </c>
       <c r="AC29" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="AD29" s="17" t="s">
         <v>513</v>
-      </c>
-      <c r="AD29" s="17" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="65.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
+        <v>538</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>539</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="C30" s="15" t="s">
         <v>540</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="D30" s="15" t="s">
         <v>541</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="E30" s="15" t="s">
         <v>542</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="F30" s="15" t="s">
         <v>543</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="G30" s="15" t="s">
         <v>544</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="H30" s="15" t="s">
         <v>545</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="I30" s="15" t="s">
         <v>546</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="J30" s="15" t="s">
         <v>547</v>
       </c>
-      <c r="J30" s="15" t="s">
+      <c r="K30" s="15" t="s">
         <v>548</v>
       </c>
-      <c r="K30" s="15" t="s">
+      <c r="L30" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="M30" s="16" t="s">
         <v>550</v>
       </c>
-      <c r="M30" s="16" t="s">
+      <c r="N30" s="16" t="s">
         <v>551</v>
       </c>
-      <c r="N30" s="16" t="s">
+      <c r="O30" s="16" t="s">
         <v>552</v>
       </c>
-      <c r="O30" s="16" t="s">
+      <c r="P30" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q30" s="16" t="s">
         <v>553</v>
       </c>
-      <c r="P30" s="16" t="s">
-        <v>551</v>
-      </c>
-      <c r="Q30" s="16" t="s">
+      <c r="R30" s="16" t="s">
         <v>554</v>
       </c>
-      <c r="R30" s="16" t="s">
+      <c r="S30" s="16" t="s">
         <v>555</v>
       </c>
-      <c r="S30" s="16" t="s">
+      <c r="T30" s="16" t="s">
         <v>556</v>
       </c>
-      <c r="T30" s="16" t="s">
+      <c r="U30" s="16" t="s">
         <v>557</v>
       </c>
-      <c r="U30" s="16" t="s">
+      <c r="V30" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="V30" s="16" t="s">
+      <c r="W30" s="16" t="s">
         <v>559</v>
       </c>
-      <c r="W30" s="16" t="s">
+      <c r="X30" s="16" t="s">
         <v>560</v>
       </c>
-      <c r="X30" s="16" t="s">
+      <c r="Y30" s="16" t="s">
         <v>561</v>
       </c>
-      <c r="Y30" s="16" t="s">
+      <c r="Z30" s="16" t="s">
         <v>562</v>
       </c>
-      <c r="Z30" s="16" t="s">
+      <c r="AA30" s="16" t="s">
         <v>563</v>
       </c>
-      <c r="AA30" s="16" t="s">
+      <c r="AB30" s="16" t="s">
         <v>564</v>
       </c>
-      <c r="AB30" s="16" t="s">
-        <v>565</v>
-      </c>
       <c r="AC30" s="16" t="s">
+        <v>539</v>
+      </c>
+      <c r="AD30" s="17" t="s">
         <v>540</v>
-      </c>
-      <c r="AD30" s="17" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="70.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -5412,738 +5409,738 @@
     </row>
     <row r="32" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
+        <v>566</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>567</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="C32" s="15" t="s">
         <v>568</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="D32" s="15" t="s">
         <v>569</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="E32" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="F32" s="15" t="s">
         <v>571</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="G32" s="15" t="s">
         <v>572</v>
       </c>
-      <c r="G32" s="15" t="s">
+      <c r="H32" s="15" t="s">
         <v>573</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="I32" s="15" t="s">
         <v>574</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="J32" s="15" t="s">
         <v>575</v>
       </c>
-      <c r="J32" s="15" t="s">
+      <c r="K32" s="15" t="s">
         <v>576</v>
       </c>
-      <c r="K32" s="15" t="s">
+      <c r="L32" s="15" t="s">
         <v>577</v>
       </c>
-      <c r="L32" s="15" t="s">
+      <c r="M32" s="16" t="s">
         <v>578</v>
       </c>
-      <c r="M32" s="16" t="s">
+      <c r="N32" s="16" t="s">
         <v>579</v>
       </c>
-      <c r="N32" s="16" t="s">
+      <c r="O32" s="16" t="s">
         <v>580</v>
       </c>
-      <c r="O32" s="16" t="s">
+      <c r="P32" s="16" t="s">
+        <v>578</v>
+      </c>
+      <c r="Q32" s="16" t="s">
         <v>581</v>
       </c>
-      <c r="P32" s="16" t="s">
-        <v>579</v>
-      </c>
-      <c r="Q32" s="16" t="s">
+      <c r="R32" s="16" t="s">
         <v>582</v>
       </c>
-      <c r="R32" s="16" t="s">
+      <c r="S32" s="16" t="s">
         <v>583</v>
       </c>
-      <c r="S32" s="16" t="s">
+      <c r="T32" s="16" t="s">
         <v>584</v>
       </c>
-      <c r="T32" s="16" t="s">
+      <c r="U32" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="U32" s="16" t="s">
+      <c r="V32" s="16" t="s">
         <v>586</v>
       </c>
-      <c r="V32" s="16" t="s">
+      <c r="W32" s="16" t="s">
         <v>587</v>
       </c>
-      <c r="W32" s="16" t="s">
+      <c r="X32" s="16" t="s">
         <v>588</v>
       </c>
-      <c r="X32" s="16" t="s">
+      <c r="Y32" s="16" t="s">
         <v>589</v>
       </c>
-      <c r="Y32" s="16" t="s">
+      <c r="Z32" s="16" t="s">
         <v>590</v>
       </c>
-      <c r="Z32" s="16" t="s">
+      <c r="AA32" s="16" t="s">
         <v>591</v>
       </c>
-      <c r="AA32" s="16" t="s">
+      <c r="AB32" s="16" t="s">
         <v>592</v>
       </c>
-      <c r="AB32" s="16" t="s">
-        <v>593</v>
-      </c>
       <c r="AC32" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="AD32" s="17" t="s">
         <v>568</v>
-      </c>
-      <c r="AD32" s="17" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>594</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="C33" s="15" t="s">
         <v>595</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="D33" s="15" t="s">
         <v>596</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="E33" s="15" t="s">
         <v>597</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="F33" s="15" t="s">
         <v>598</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="G33" s="15" t="s">
         <v>599</v>
       </c>
-      <c r="G33" s="15" t="s">
+      <c r="H33" s="15" t="s">
         <v>600</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="I33" s="15" t="s">
         <v>601</v>
       </c>
-      <c r="I33" s="15" t="s">
+      <c r="J33" s="15" t="s">
         <v>602</v>
       </c>
-      <c r="J33" s="15" t="s">
+      <c r="K33" s="15" t="s">
         <v>603</v>
       </c>
-      <c r="K33" s="15" t="s">
+      <c r="L33" s="15" t="s">
         <v>604</v>
       </c>
-      <c r="L33" s="15" t="s">
+      <c r="M33" s="16" t="s">
         <v>605</v>
       </c>
-      <c r="M33" s="16" t="s">
+      <c r="N33" s="16" t="s">
         <v>606</v>
       </c>
-      <c r="N33" s="16" t="s">
+      <c r="O33" s="16" t="s">
         <v>607</v>
       </c>
-      <c r="O33" s="16" t="s">
+      <c r="P33" s="16" t="s">
+        <v>605</v>
+      </c>
+      <c r="Q33" s="16" t="s">
         <v>608</v>
       </c>
-      <c r="P33" s="16" t="s">
-        <v>606</v>
-      </c>
-      <c r="Q33" s="16" t="s">
+      <c r="R33" s="16" t="s">
         <v>609</v>
       </c>
-      <c r="R33" s="16" t="s">
+      <c r="S33" s="16" t="s">
         <v>610</v>
       </c>
-      <c r="S33" s="16" t="s">
+      <c r="T33" s="16" t="s">
         <v>611</v>
       </c>
-      <c r="T33" s="16" t="s">
+      <c r="U33" s="16" t="s">
         <v>612</v>
       </c>
-      <c r="U33" s="16" t="s">
+      <c r="V33" s="16" t="s">
         <v>613</v>
       </c>
-      <c r="V33" s="16" t="s">
+      <c r="W33" s="16" t="s">
         <v>614</v>
       </c>
-      <c r="W33" s="16" t="s">
+      <c r="X33" s="16" t="s">
         <v>615</v>
       </c>
-      <c r="X33" s="16" t="s">
+      <c r="Y33" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="Y33" s="16" t="s">
+      <c r="Z33" s="16" t="s">
         <v>617</v>
       </c>
-      <c r="Z33" s="16" t="s">
+      <c r="AA33" s="16" t="s">
         <v>618</v>
       </c>
-      <c r="AA33" s="16" t="s">
+      <c r="AB33" s="16" t="s">
         <v>619</v>
       </c>
-      <c r="AB33" s="16" t="s">
-        <v>620</v>
-      </c>
       <c r="AC33" s="16" t="s">
+        <v>594</v>
+      </c>
+      <c r="AD33" s="17" t="s">
         <v>595</v>
-      </c>
-      <c r="AD33" s="17" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="54.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="25" t="s">
+        <v>620</v>
+      </c>
+      <c r="B34" s="26" t="s">
         <v>621</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="C34" s="26" t="s">
         <v>622</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="D34" s="26" t="s">
         <v>623</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="E34" s="26" t="s">
         <v>624</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="F34" s="26" t="s">
         <v>625</v>
       </c>
-      <c r="F34" s="26" t="s">
+      <c r="G34" s="26" t="s">
         <v>626</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="H34" s="26" t="s">
         <v>627</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="I34" s="26" t="s">
         <v>628</v>
       </c>
-      <c r="I34" s="26" t="s">
+      <c r="J34" s="26" t="s">
         <v>629</v>
       </c>
-      <c r="J34" s="26" t="s">
+      <c r="K34" s="26" t="s">
         <v>630</v>
       </c>
-      <c r="K34" s="26" t="s">
+      <c r="L34" s="26" t="s">
         <v>631</v>
       </c>
-      <c r="L34" s="26" t="s">
+      <c r="M34" s="27" t="s">
         <v>632</v>
       </c>
-      <c r="M34" s="27" t="s">
+      <c r="N34" s="27" t="s">
         <v>633</v>
       </c>
-      <c r="N34" s="27" t="s">
+      <c r="O34" s="27" t="s">
         <v>634</v>
       </c>
-      <c r="O34" s="27" t="s">
+      <c r="P34" s="27" t="s">
+        <v>632</v>
+      </c>
+      <c r="Q34" s="27" t="s">
         <v>635</v>
       </c>
-      <c r="P34" s="27" t="s">
-        <v>633</v>
-      </c>
-      <c r="Q34" s="27" t="s">
+      <c r="R34" s="27" t="s">
         <v>636</v>
       </c>
-      <c r="R34" s="27" t="s">
+      <c r="S34" s="27" t="s">
         <v>637</v>
       </c>
-      <c r="S34" s="27" t="s">
+      <c r="T34" s="27" t="s">
         <v>638</v>
       </c>
-      <c r="T34" s="27" t="s">
+      <c r="U34" s="27" t="s">
         <v>639</v>
       </c>
-      <c r="U34" s="27" t="s">
+      <c r="V34" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="V34" s="27" t="s">
+      <c r="W34" s="27" t="s">
         <v>641</v>
       </c>
-      <c r="W34" s="27" t="s">
+      <c r="X34" s="27" t="s">
         <v>642</v>
       </c>
-      <c r="X34" s="27" t="s">
+      <c r="Y34" s="27" t="s">
         <v>643</v>
       </c>
-      <c r="Y34" s="27" t="s">
+      <c r="Z34" s="27" t="s">
         <v>644</v>
       </c>
-      <c r="Z34" s="27" t="s">
+      <c r="AA34" s="27" t="s">
         <v>645</v>
       </c>
-      <c r="AA34" s="27" t="s">
+      <c r="AB34" s="27" t="s">
         <v>646</v>
       </c>
-      <c r="AB34" s="27" t="s">
-        <v>647</v>
-      </c>
       <c r="AC34" s="27" t="s">
+        <v>621</v>
+      </c>
+      <c r="AD34" s="28" t="s">
         <v>622</v>
-      </c>
-      <c r="AD34" s="28" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="18" t="s">
+        <v>647</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>648</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="C35" s="15" t="s">
         <v>649</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="D35" s="15" t="s">
         <v>650</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="E35" s="15" t="s">
         <v>651</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="F35" s="15" t="s">
         <v>652</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="G35" s="15" t="s">
         <v>653</v>
       </c>
-      <c r="G35" s="15" t="s">
+      <c r="H35" s="15" t="s">
         <v>654</v>
       </c>
-      <c r="H35" s="15" t="s">
+      <c r="I35" s="15" t="s">
         <v>655</v>
       </c>
-      <c r="I35" s="15" t="s">
+      <c r="J35" s="15" t="s">
         <v>656</v>
       </c>
-      <c r="J35" s="15" t="s">
+      <c r="K35" s="15" t="s">
         <v>657</v>
       </c>
-      <c r="K35" s="15" t="s">
+      <c r="L35" s="15" t="s">
         <v>658</v>
       </c>
-      <c r="L35" s="15" t="s">
+      <c r="M35" s="16" t="s">
         <v>659</v>
       </c>
-      <c r="M35" s="16" t="s">
+      <c r="N35" s="16" t="s">
         <v>660</v>
       </c>
-      <c r="N35" s="16" t="s">
+      <c r="O35" s="16" t="s">
         <v>661</v>
       </c>
-      <c r="O35" s="16" t="s">
+      <c r="P35" s="16" t="s">
+        <v>659</v>
+      </c>
+      <c r="Q35" s="16" t="s">
         <v>662</v>
       </c>
-      <c r="P35" s="16" t="s">
-        <v>660</v>
-      </c>
-      <c r="Q35" s="16" t="s">
+      <c r="R35" s="16" t="s">
         <v>663</v>
       </c>
-      <c r="R35" s="16" t="s">
+      <c r="S35" s="16" t="s">
         <v>664</v>
       </c>
-      <c r="S35" s="16" t="s">
+      <c r="T35" s="16" t="s">
         <v>665</v>
       </c>
-      <c r="T35" s="16" t="s">
+      <c r="U35" s="16" t="s">
         <v>666</v>
       </c>
-      <c r="U35" s="16" t="s">
+      <c r="V35" s="16" t="s">
         <v>667</v>
       </c>
-      <c r="V35" s="16" t="s">
+      <c r="W35" s="16" t="s">
         <v>668</v>
       </c>
-      <c r="W35" s="16" t="s">
+      <c r="X35" s="16" t="s">
         <v>669</v>
       </c>
-      <c r="X35" s="16" t="s">
+      <c r="Y35" s="16" t="s">
         <v>670</v>
       </c>
-      <c r="Y35" s="16" t="s">
+      <c r="Z35" s="16" t="s">
         <v>671</v>
       </c>
-      <c r="Z35" s="16" t="s">
+      <c r="AA35" s="16" t="s">
         <v>672</v>
       </c>
-      <c r="AA35" s="16" t="s">
+      <c r="AB35" s="16" t="s">
         <v>673</v>
       </c>
-      <c r="AB35" s="16" t="s">
-        <v>674</v>
-      </c>
       <c r="AC35" s="16" t="s">
+        <v>648</v>
+      </c>
+      <c r="AD35" s="17" t="s">
         <v>649</v>
-      </c>
-      <c r="AD35" s="17" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="s">
+        <v>674</v>
+      </c>
+      <c r="B36" s="15" t="s">
         <v>675</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="C36" s="15" t="s">
         <v>676</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="D36" s="15" t="s">
         <v>677</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="E36" s="15" t="s">
         <v>678</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="F36" s="15" t="s">
         <v>679</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="G36" s="15" t="s">
         <v>680</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="H36" s="15" t="s">
         <v>681</v>
       </c>
-      <c r="H36" s="15" t="s">
+      <c r="I36" s="15" t="s">
         <v>682</v>
       </c>
-      <c r="I36" s="15" t="s">
+      <c r="J36" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="J36" s="15" t="s">
+      <c r="K36" s="15" t="s">
         <v>684</v>
       </c>
-      <c r="K36" s="15" t="s">
+      <c r="L36" s="15" t="s">
         <v>685</v>
       </c>
-      <c r="L36" s="15" t="s">
+      <c r="M36" s="16" t="s">
         <v>686</v>
       </c>
-      <c r="M36" s="16" t="s">
+      <c r="N36" s="16" t="s">
         <v>687</v>
       </c>
-      <c r="N36" s="16" t="s">
+      <c r="O36" s="16" t="s">
         <v>688</v>
       </c>
-      <c r="O36" s="16" t="s">
+      <c r="P36" s="16" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q36" s="16" t="s">
         <v>689</v>
       </c>
-      <c r="P36" s="16" t="s">
-        <v>687</v>
-      </c>
-      <c r="Q36" s="16" t="s">
+      <c r="R36" s="16" t="s">
         <v>690</v>
       </c>
-      <c r="R36" s="16" t="s">
+      <c r="S36" s="16" t="s">
         <v>691</v>
       </c>
-      <c r="S36" s="16" t="s">
+      <c r="T36" s="16" t="s">
         <v>692</v>
       </c>
-      <c r="T36" s="16" t="s">
+      <c r="U36" s="16" t="s">
         <v>693</v>
       </c>
-      <c r="U36" s="16" t="s">
+      <c r="V36" s="16" t="s">
         <v>694</v>
       </c>
-      <c r="V36" s="16" t="s">
+      <c r="W36" s="16" t="s">
         <v>695</v>
       </c>
-      <c r="W36" s="16" t="s">
+      <c r="X36" s="16" t="s">
         <v>696</v>
       </c>
-      <c r="X36" s="16" t="s">
+      <c r="Y36" s="16" t="s">
         <v>697</v>
       </c>
-      <c r="Y36" s="16" t="s">
+      <c r="Z36" s="16" t="s">
         <v>698</v>
       </c>
-      <c r="Z36" s="16" t="s">
+      <c r="AA36" s="16" t="s">
         <v>699</v>
       </c>
-      <c r="AA36" s="16" t="s">
+      <c r="AB36" s="16" t="s">
         <v>700</v>
       </c>
-      <c r="AB36" s="16" t="s">
-        <v>701</v>
-      </c>
       <c r="AC36" s="16" t="s">
+        <v>675</v>
+      </c>
+      <c r="AD36" s="17" t="s">
         <v>676</v>
-      </c>
-      <c r="AD36" s="17" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
+        <v>701</v>
+      </c>
+      <c r="B37" s="15" t="s">
         <v>702</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="C37" s="15" t="s">
         <v>703</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="D37" s="15" t="s">
         <v>704</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="E37" s="15" t="s">
         <v>705</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="F37" s="15" t="s">
         <v>706</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="G37" s="15" t="s">
         <v>707</v>
       </c>
-      <c r="G37" s="15" t="s">
+      <c r="H37" s="15" t="s">
         <v>708</v>
       </c>
-      <c r="H37" s="15" t="s">
+      <c r="I37" s="15" t="s">
         <v>709</v>
       </c>
-      <c r="I37" s="15" t="s">
+      <c r="J37" s="15" t="s">
         <v>710</v>
       </c>
-      <c r="J37" s="15" t="s">
+      <c r="K37" s="15" t="s">
         <v>711</v>
       </c>
-      <c r="K37" s="15" t="s">
+      <c r="L37" s="15" t="s">
         <v>712</v>
       </c>
-      <c r="L37" s="15" t="s">
+      <c r="M37" s="16" t="s">
         <v>713</v>
       </c>
-      <c r="M37" s="16" t="s">
+      <c r="N37" s="16" t="s">
         <v>714</v>
       </c>
-      <c r="N37" s="16" t="s">
+      <c r="O37" s="16" t="s">
         <v>715</v>
       </c>
-      <c r="O37" s="16" t="s">
+      <c r="P37" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q37" s="16" t="s">
         <v>716</v>
       </c>
-      <c r="P37" s="16" t="s">
-        <v>714</v>
-      </c>
-      <c r="Q37" s="16" t="s">
+      <c r="R37" s="16" t="s">
         <v>717</v>
       </c>
-      <c r="R37" s="16" t="s">
+      <c r="S37" s="16" t="s">
         <v>718</v>
       </c>
-      <c r="S37" s="16" t="s">
+      <c r="T37" s="16" t="s">
         <v>719</v>
       </c>
-      <c r="T37" s="16" t="s">
+      <c r="U37" s="16" t="s">
         <v>720</v>
       </c>
-      <c r="U37" s="16" t="s">
+      <c r="V37" s="16" t="s">
         <v>721</v>
       </c>
-      <c r="V37" s="16" t="s">
+      <c r="W37" s="16" t="s">
         <v>722</v>
       </c>
-      <c r="W37" s="16" t="s">
+      <c r="X37" s="16" t="s">
         <v>723</v>
       </c>
-      <c r="X37" s="16" t="s">
+      <c r="Y37" s="16" t="s">
         <v>724</v>
       </c>
-      <c r="Y37" s="16" t="s">
+      <c r="Z37" s="16" t="s">
         <v>725</v>
       </c>
-      <c r="Z37" s="16" t="s">
+      <c r="AA37" s="16" t="s">
         <v>726</v>
       </c>
-      <c r="AA37" s="16" t="s">
+      <c r="AB37" s="16" t="s">
         <v>727</v>
       </c>
-      <c r="AB37" s="16" t="s">
-        <v>728</v>
-      </c>
       <c r="AC37" s="16" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD37" s="17" t="s">
         <v>703</v>
-      </c>
-      <c r="AD37" s="17" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="s">
+        <v>728</v>
+      </c>
+      <c r="B38" s="15" t="s">
         <v>729</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="C38" s="15" t="s">
         <v>730</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="D38" s="15" t="s">
         <v>731</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="E38" s="15" t="s">
         <v>732</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="F38" s="15" t="s">
         <v>733</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="G38" s="15" t="s">
         <v>734</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="H38" s="15" t="s">
         <v>735</v>
       </c>
-      <c r="H38" s="15" t="s">
+      <c r="I38" s="15" t="s">
         <v>736</v>
       </c>
-      <c r="I38" s="15" t="s">
+      <c r="J38" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="J38" s="15" t="s">
+      <c r="K38" s="15" t="s">
         <v>738</v>
       </c>
-      <c r="K38" s="15" t="s">
+      <c r="L38" s="15" t="s">
         <v>739</v>
       </c>
-      <c r="L38" s="15" t="s">
+      <c r="M38" s="16" t="s">
         <v>740</v>
       </c>
-      <c r="M38" s="16" t="s">
+      <c r="N38" s="16" t="s">
         <v>741</v>
       </c>
-      <c r="N38" s="16" t="s">
+      <c r="O38" s="16" t="s">
         <v>742</v>
       </c>
-      <c r="O38" s="16" t="s">
+      <c r="P38" s="16" t="s">
+        <v>740</v>
+      </c>
+      <c r="Q38" s="16" t="s">
         <v>743</v>
       </c>
-      <c r="P38" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="Q38" s="16" t="s">
+      <c r="R38" s="16" t="s">
         <v>744</v>
       </c>
-      <c r="R38" s="16" t="s">
+      <c r="S38" s="16" t="s">
         <v>745</v>
       </c>
-      <c r="S38" s="16" t="s">
+      <c r="T38" s="16" t="s">
         <v>746</v>
       </c>
-      <c r="T38" s="16" t="s">
+      <c r="U38" s="16" t="s">
         <v>747</v>
       </c>
-      <c r="U38" s="16" t="s">
+      <c r="V38" s="16" t="s">
         <v>748</v>
       </c>
-      <c r="V38" s="16" t="s">
+      <c r="W38" s="16" t="s">
         <v>749</v>
       </c>
-      <c r="W38" s="16" t="s">
+      <c r="X38" s="16" t="s">
         <v>750</v>
       </c>
-      <c r="X38" s="16" t="s">
+      <c r="Y38" s="16" t="s">
         <v>751</v>
       </c>
-      <c r="Y38" s="16" t="s">
+      <c r="Z38" s="16" t="s">
         <v>752</v>
       </c>
-      <c r="Z38" s="16" t="s">
+      <c r="AA38" s="16" t="s">
         <v>753</v>
       </c>
-      <c r="AA38" s="16" t="s">
+      <c r="AB38" s="16" t="s">
         <v>754</v>
       </c>
-      <c r="AB38" s="16" t="s">
-        <v>755</v>
-      </c>
       <c r="AC38" s="16" t="s">
+        <v>729</v>
+      </c>
+      <c r="AD38" s="17" t="s">
         <v>730</v>
-      </c>
-      <c r="AD38" s="17" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="31" t="s">
+        <v>755</v>
+      </c>
+      <c r="B39" s="15" t="s">
         <v>756</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="C39" s="15" t="s">
         <v>757</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="D39" s="15" t="s">
         <v>758</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="E39" s="15" t="s">
         <v>759</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="F39" s="15" t="s">
         <v>760</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="G39" s="15" t="s">
         <v>761</v>
       </c>
-      <c r="G39" s="15" t="s">
+      <c r="H39" s="15" t="s">
         <v>762</v>
       </c>
-      <c r="H39" s="15" t="s">
+      <c r="I39" s="15" t="s">
         <v>763</v>
       </c>
-      <c r="I39" s="15" t="s">
+      <c r="J39" s="15" t="s">
         <v>764</v>
       </c>
-      <c r="J39" s="15" t="s">
+      <c r="K39" s="15" t="s">
         <v>765</v>
       </c>
-      <c r="K39" s="15" t="s">
+      <c r="L39" s="15" t="s">
         <v>766</v>
       </c>
-      <c r="L39" s="15" t="s">
+      <c r="M39" s="16" t="s">
         <v>767</v>
       </c>
-      <c r="M39" s="16" t="s">
+      <c r="N39" s="16" t="s">
         <v>768</v>
       </c>
-      <c r="N39" s="16" t="s">
+      <c r="O39" s="16" t="s">
         <v>769</v>
       </c>
-      <c r="O39" s="16" t="s">
+      <c r="P39" s="16" t="s">
+        <v>767</v>
+      </c>
+      <c r="Q39" s="16" t="s">
         <v>770</v>
       </c>
-      <c r="P39" s="16" t="s">
-        <v>768</v>
-      </c>
-      <c r="Q39" s="16" t="s">
+      <c r="R39" s="16" t="s">
         <v>771</v>
       </c>
-      <c r="R39" s="16" t="s">
+      <c r="S39" s="16" t="s">
         <v>772</v>
       </c>
-      <c r="S39" s="16" t="s">
+      <c r="T39" s="16" t="s">
         <v>773</v>
       </c>
-      <c r="T39" s="16" t="s">
+      <c r="U39" s="16" t="s">
         <v>774</v>
       </c>
-      <c r="U39" s="16" t="s">
+      <c r="V39" s="16" t="s">
         <v>775</v>
       </c>
-      <c r="V39" s="16" t="s">
+      <c r="W39" s="16" t="s">
         <v>776</v>
       </c>
-      <c r="W39" s="16" t="s">
+      <c r="X39" s="16" t="s">
         <v>777</v>
       </c>
-      <c r="X39" s="16" t="s">
+      <c r="Y39" s="16" t="s">
         <v>778</v>
       </c>
-      <c r="Y39" s="16" t="s">
+      <c r="Z39" s="16" t="s">
         <v>779</v>
       </c>
-      <c r="Z39" s="16" t="s">
+      <c r="AA39" s="16" t="s">
         <v>780</v>
       </c>
-      <c r="AA39" s="16" t="s">
+      <c r="AB39" s="16" t="s">
         <v>781</v>
       </c>
-      <c r="AB39" s="16" t="s">
-        <v>782</v>
-      </c>
       <c r="AC39" s="16" t="s">
+        <v>756</v>
+      </c>
+      <c r="AD39" s="17" t="s">
         <v>757</v>
-      </c>
-      <c r="AD39" s="17" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6192,7 +6189,7 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6203,32 +6200,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6236,12 +6233,12 @@
     </row>
     <row r="9" customFormat="false" ht="80.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6249,7 +6246,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="35" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6257,22 +6254,22 @@
     </row>
     <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="37" t="s">
+        <v>791</v>
+      </c>
+      <c r="B14" s="38" t="s">
         <v>792</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>793</v>
       </c>
       <c r="C14" s="38"/>
       <c r="D14" s="38" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="38" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G14" s="38"/>
       <c r="H14" s="38" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="I14" s="38"/>
       <c r="J14" s="38" t="s">
@@ -6288,19 +6285,19 @@
       </c>
       <c r="O14" s="38"/>
       <c r="P14" s="38" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="Q14" s="38"/>
       <c r="R14" s="38" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="S14" s="38"/>
       <c r="T14" s="38" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="U14" s="38"/>
       <c r="V14" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="W14" s="38"/>
       <c r="X14" s="39" t="s">
@@ -6385,7 +6382,7 @@
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="42" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="42"/>
@@ -6414,7 +6411,7 @@
     </row>
     <row r="17" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="43" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -6443,7 +6440,7 @@
     </row>
     <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="43" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -6472,7 +6469,7 @@
     </row>
     <row r="19" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="43" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -6555,7 +6552,7 @@
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
@@ -6584,7 +6581,7 @@
     </row>
     <row r="23" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="43" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -6613,7 +6610,7 @@
     </row>
     <row r="24" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="43" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -6642,7 +6639,7 @@
     </row>
     <row r="25" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="43" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -6671,7 +6668,7 @@
     </row>
     <row r="26" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="43" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -6754,7 +6751,7 @@
     </row>
     <row r="29" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="46" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -6783,7 +6780,7 @@
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="42" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
@@ -6812,7 +6809,7 @@
     </row>
     <row r="31" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="43" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
@@ -6841,7 +6838,7 @@
     </row>
     <row r="32" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="43" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B32" s="44"/>
       <c r="C32" s="44"/>
@@ -6924,7 +6921,7 @@
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="42" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="42"/>
@@ -7034,7 +7031,7 @@
     </row>
     <row r="39" customFormat="false" ht="66.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="46" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B39" s="44"/>
       <c r="C39" s="44"/>
@@ -7063,7 +7060,7 @@
     </row>
     <row r="40" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="46" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B40" s="44"/>
       <c r="C40" s="44"/>
@@ -7092,7 +7089,7 @@
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="42" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="42"/>
@@ -7121,7 +7118,7 @@
     </row>
     <row r="42" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="43" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B42" s="44"/>
       <c r="C42" s="44"/>
@@ -7150,7 +7147,7 @@
     </row>
     <row r="43" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="43" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B43" s="44"/>
       <c r="C43" s="44"/>
@@ -7179,7 +7176,7 @@
     </row>
     <row r="44" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="43" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B44" s="44"/>
       <c r="C44" s="44"/>
@@ -7262,7 +7259,7 @@
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="42" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="42"/>
@@ -7345,7 +7342,7 @@
     </row>
     <row r="50" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="43" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B50" s="44"/>
       <c r="C50" s="44"/>
@@ -7374,7 +7371,7 @@
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="42" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="42"/>
@@ -7403,7 +7400,7 @@
     </row>
     <row r="52" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="47" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B52" s="44"/>
       <c r="C52" s="44"/>
@@ -7432,7 +7429,7 @@
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="47" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B53" s="44"/>
       <c r="C53" s="44"/>
@@ -7461,7 +7458,7 @@
     </row>
     <row r="54" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="47" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B54" s="44"/>
       <c r="C54" s="44"/>
@@ -7517,7 +7514,7 @@
     </row>
     <row r="56" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="48" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B56" s="44"/>
       <c r="C56" s="44"/>
@@ -7546,7 +7543,7 @@
     </row>
     <row r="57" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="49" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B57" s="50"/>
       <c r="C57" s="50"/>
@@ -7578,7 +7575,7 @@
     </row>
     <row r="59" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="53" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use FdnWho for stade_oms info as it FdcStadeOMS is not present on all databases
</commit_message>
<xml_diff>
--- a/resources/report_template.xlsx
+++ b/resources/report_template.xlsx
@@ -984,7 +984,7 @@
     <t>{key: 'ACTIVE_LIST', age_min: 50, gender: 1}</t>
   </si>
   <si>
-    <t>Nombre de personnes infectées par le VIH, qui répondent aux critères d’éligibilité à la prophylaxie au cotrimoxazole de la période de rapportage et ne sont pas sous TARV</t>
+    <t>Nombre de personnes infectées par le VIH, qui répondent aux critères d’éligibilité à la prophylaxie au cotrimoxazole au cours la période de rapportage et ne sont pas sous TARV</t>
   </si>
   <si>
     <t>{key: 'CTX_ELIGIBLE', gender: 0}</t>
@@ -3203,15 +3203,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>567000</xdr:colOff>
+      <xdr:colOff>594000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1045080</xdr:colOff>
+      <xdr:colOff>1071720</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3224,8 +3224,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="567000" y="610920"/>
-          <a:ext cx="478080" cy="354240"/>
+          <a:off x="594000" y="601920"/>
+          <a:ext cx="477720" cy="353880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>